<commit_message>
eu-gdpr: add establishment, authority; add other concepts
closes #93 Establishment and Lead SA
closes #92 A.19 Notification in title
closes #88 Cross-border transfer (in DPV Processing)
closes #87 Automated Scoring (in DPV Processing Context)
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="329">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="341">
   <si>
     <t>Term</t>
   </si>
@@ -159,6 +159,30 @@
     <t>Document that contains a publicly available list of entities that perform a certain activity within a certain location or jurisdiction</t>
   </si>
   <si>
+    <t>SubsidiaryLegalEntity</t>
+  </si>
+  <si>
+    <t>Subsidiary Legal Entity</t>
+  </si>
+  <si>
+    <t>A legal entity that operates as a subsidiary of another legal entity</t>
+  </si>
+  <si>
+    <t>dpv:Organisation</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Georg P Krog</t>
+  </si>
+  <si>
+    <t>ParentLegalEntity</t>
+  </si>
+  <si>
+    <t>Parent Legal Entity</t>
+  </si>
+  <si>
+    <t>A legal entity that has one or more subsidiary entities operating under it</t>
+  </si>
+  <si>
     <t>domain</t>
   </si>
   <si>
@@ -250,6 +274,24 @@
   </si>
   <si>
     <t>Indicates the entity is a representative for specified entity</t>
+  </si>
+  <si>
+    <t>hasSubsidiary</t>
+  </si>
+  <si>
+    <t>has subsidiary</t>
+  </si>
+  <si>
+    <t>Indicates this entity has the specified entity as its subsidiary</t>
+  </si>
+  <si>
+    <t>isSubsidiaryOf</t>
+  </si>
+  <si>
+    <t>is subsidiary of</t>
+  </si>
+  <si>
+    <t>Indicates this entity is the subsidiary of the specified entity</t>
   </si>
   <si>
     <t>Authority</t>
@@ -363,9 +405,6 @@
     <t>Indicates applicability of authority for a jurisdiction</t>
   </si>
   <si>
-    <t>Harshvardhan J. Pandit, Georg P Krog</t>
-  </si>
-  <si>
     <t>https://www.w3.org/community/dpvcg/wiki/MinutesOfMeeting_20220119</t>
   </si>
   <si>
@@ -699,9 +738,6 @@
   </si>
   <si>
     <t>A consortium established and comprising on industry organisations</t>
-  </si>
-  <si>
-    <t>dpv:Organisation</t>
   </si>
   <si>
     <t>(ADMS controlled vocabulary,http://purl.org/adms)</t>
@@ -2119,20 +2155,6 @@
       </c>
       <c r="P2" s="14"/>
       <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
-      <c r="Y2" s="14"/>
-      <c r="Z2" s="14"/>
-      <c r="AA2" s="14"/>
-      <c r="AB2" s="14"/>
-      <c r="AC2" s="14"/>
-      <c r="AD2" s="14"/>
-      <c r="AE2" s="14"/>
     </row>
     <row r="3">
       <c r="A3" s="12" t="s">
@@ -2170,20 +2192,6 @@
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
     </row>
     <row r="4">
       <c r="A4" s="12" t="s">
@@ -2221,20 +2229,6 @@
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
     </row>
     <row r="5">
       <c r="A5" s="19" t="s">
@@ -2378,10 +2372,74 @@
       <c r="AE7" s="31"/>
     </row>
     <row r="8">
-      <c r="B8" s="33"/>
+      <c r="A8" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="15">
+        <v>45396.0</v>
+      </c>
+      <c r="L8" s="14"/>
+      <c r="M8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N8" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
     </row>
     <row r="9">
-      <c r="B9" s="33"/>
+      <c r="A9" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15">
+        <v>45396.0</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
     </row>
     <row r="10">
       <c r="B10" s="33"/>
@@ -5178,7 +5236,7 @@
       <formula>$M2="deprecated"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1:D6 G1:AE6 E2:F6">
+  <conditionalFormatting sqref="A1:Q100">
     <cfRule type="expression" dxfId="2" priority="3">
       <formula>$M1="accepted"</formula>
     </cfRule>
@@ -5224,13 +5282,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -5245,7 +5303,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -5262,13 +5320,13 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>25</v>
@@ -5277,7 +5335,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G2" s="38"/>
       <c r="H2" s="39"/>
@@ -5291,7 +5349,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="O2" s="42" t="s">
         <v>37</v>
@@ -5312,13 +5370,13 @@
     </row>
     <row r="3">
       <c r="A3" s="36" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C3" s="36" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="D3" s="37" t="s">
         <v>25</v>
@@ -5327,7 +5385,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G3" s="38"/>
       <c r="H3" s="39"/>
@@ -5341,7 +5399,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="O3" s="42" t="s">
         <v>37</v>
@@ -5362,13 +5420,13 @@
     </row>
     <row r="4">
       <c r="A4" s="36" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="C4" s="36" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="D4" s="37" t="s">
         <v>25</v>
@@ -5377,7 +5435,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G4" s="38"/>
       <c r="H4" s="39"/>
@@ -5391,7 +5449,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="O4" s="42" t="s">
         <v>37</v>
@@ -5412,13 +5470,13 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
@@ -5427,12 +5485,12 @@
         <v>25</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="13" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="44">
@@ -5464,22 +5522,22 @@
     </row>
     <row r="6">
       <c r="A6" s="36" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="B6" s="36" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="C6" s="37" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="D6" s="37" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="37" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G6" s="37"/>
       <c r="H6" s="39"/>
@@ -5493,7 +5551,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="37" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="O6" s="42" t="s">
         <v>37</v>
@@ -5514,13 +5572,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>17</v>
@@ -5529,7 +5587,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -5546,7 +5604,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="46" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -5564,22 +5622,22 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="C8" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>76</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>68</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -5609,6 +5667,102 @@
       <c r="Z8" s="14"/>
       <c r="AA8" s="14"/>
       <c r="AB8" s="14"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="15">
+        <v>45396.0</v>
+      </c>
+      <c r="L9" s="14"/>
+      <c r="M9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="14"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
+      <c r="Y9" s="14"/>
+      <c r="Z9" s="14"/>
+      <c r="AA9" s="14"/>
+      <c r="AB9" s="14"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15">
+        <v>45396.0</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
+      <c r="R10" s="14"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
+      <c r="Y10" s="14"/>
+      <c r="Z10" s="14"/>
+      <c r="AA10" s="14"/>
+      <c r="AB10" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O7">
@@ -5721,16 +5875,16 @@
     </row>
     <row r="2">
       <c r="A2" s="47" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="B2" s="48" t="s">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C2" s="48" t="s">
-        <v>78</v>
+        <v>92</v>
       </c>
       <c r="D2" s="49" t="s">
-        <v>79</v>
+        <v>93</v>
       </c>
       <c r="E2" s="50" t="s">
         <v>26</v>
@@ -5748,7 +5902,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="48" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="O2" s="53" t="s">
         <v>37</v>
@@ -5769,16 +5923,16 @@
     </row>
     <row r="3">
       <c r="A3" s="47" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B3" s="54" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="D3" s="48" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E3" s="55" t="s">
         <v>26</v>
@@ -5796,7 +5950,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="48" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="O3" s="53" t="s">
         <v>37</v>
@@ -5817,16 +5971,16 @@
     </row>
     <row r="4">
       <c r="A4" s="48" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>86</v>
+        <v>100</v>
       </c>
       <c r="C4" s="55" t="s">
-        <v>87</v>
+        <v>101</v>
       </c>
       <c r="D4" s="48" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -5836,7 +5990,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="56"/>
       <c r="J4" s="57" t="s">
-        <v>88</v>
+        <v>102</v>
       </c>
       <c r="K4" s="52">
         <v>44594.0</v>
@@ -5867,16 +6021,16 @@
     </row>
     <row r="5">
       <c r="A5" s="54" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="B5" s="55" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>91</v>
+        <v>105</v>
       </c>
       <c r="D5" s="54" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -5886,7 +6040,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="57" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="K5" s="52">
         <v>44594.0</v>
@@ -5917,16 +6071,16 @@
     </row>
     <row r="6">
       <c r="A6" s="48" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="D6" s="48" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -5936,7 +6090,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="58" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="K6" s="52">
         <v>44594.0</v>
@@ -8812,13 +8966,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -8833,7 +8987,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -8850,19 +9004,19 @@
     </row>
     <row r="2">
       <c r="A2" s="36" t="s">
-        <v>97</v>
+        <v>111</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="D2" s="37" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="F2" s="43"/>
       <c r="G2" s="38"/>
@@ -8877,10 +9031,10 @@
         <v>19</v>
       </c>
       <c r="N2" s="37" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O2" s="42" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="P2" s="43"/>
       <c r="Q2" s="43"/>
@@ -8898,16 +9052,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>102</v>
+        <v>115</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>103</v>
+        <v>116</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>104</v>
+        <v>117</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -8925,10 +9079,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="O3" s="42" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -9052,13 +9206,13 @@
     </row>
     <row r="2">
       <c r="A2" s="59" t="s">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="B2" s="60" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C2" s="61" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="D2" s="59" t="s">
         <v>34</v>
@@ -9070,10 +9224,10 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="62" t="s">
-        <v>108</v>
+        <v>121</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="K2" s="25">
         <v>43560.0</v>
@@ -9085,7 +9239,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="59" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="O2" s="27" t="s">
         <v>27</v>
@@ -9106,16 +9260,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>111</v>
+        <v>124</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>113</v>
+        <v>126</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -9125,7 +9279,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="64" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="K3" s="15">
         <v>43620.0</v>
@@ -9138,7 +9292,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -9156,16 +9310,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>118</v>
+        <v>131</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>119</v>
+        <v>132</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>26</v>
@@ -9174,7 +9328,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="13" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="15">
@@ -9188,7 +9342,7 @@
         <v>20</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -9206,13 +9360,13 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>123</v>
+        <v>136</v>
       </c>
       <c r="C5" s="61" t="s">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="D5" s="59" t="s">
         <v>34</v>
@@ -9222,16 +9376,16 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>125</v>
+        <v>138</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>127</v>
+        <v>140</v>
       </c>
       <c r="J5" s="66" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
       <c r="K5" s="25">
         <v>43560.0</v>
@@ -9243,7 +9397,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="59" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="O5" s="27" t="s">
         <v>27</v>
@@ -9264,16 +9418,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>26</v>
@@ -9283,7 +9437,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="64" t="s">
-        <v>132</v>
+        <v>145</v>
       </c>
       <c r="K6" s="15">
         <v>43620.0</v>
@@ -9296,7 +9450,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>116</v>
+        <v>129</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -9314,13 +9468,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>134</v>
+        <v>147</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>135</v>
+        <v>148</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>34</v>
@@ -9332,10 +9486,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="13" t="s">
-        <v>136</v>
+        <v>149</v>
       </c>
       <c r="J7" s="68" t="s">
-        <v>137</v>
+        <v>150</v>
       </c>
       <c r="K7" s="15">
         <v>44447.0</v>
@@ -9345,10 +9499,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="37" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -9366,16 +9520,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>140</v>
+        <v>153</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>141</v>
+        <v>154</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>142</v>
+        <v>155</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>26</v>
@@ -9384,10 +9538,10 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="69" t="s">
-        <v>143</v>
+        <v>156</v>
       </c>
       <c r="J8" s="68" t="s">
-        <v>144</v>
+        <v>157</v>
       </c>
       <c r="K8" s="15">
         <v>44447.0</v>
@@ -9397,10 +9551,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="37" t="s">
-        <v>138</v>
+        <v>151</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>139</v>
+        <v>152</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -9418,16 +9572,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>145</v>
+        <v>158</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>146</v>
+        <v>159</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>147</v>
+        <v>160</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>26</v>
@@ -9436,7 +9590,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="13" t="s">
-        <v>149</v>
+        <v>162</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="15">
@@ -9447,7 +9601,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="37" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="O9" s="45" t="s">
         <v>21</v>
@@ -9468,16 +9622,16 @@
     </row>
     <row r="10">
       <c r="A10" s="70" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B10" s="70" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C10" s="71" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="D10" s="72" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E10" s="73" t="s">
         <v>26</v>
@@ -9487,7 +9641,7 @@
       <c r="H10" s="74"/>
       <c r="I10" s="74"/>
       <c r="J10" s="75" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="K10" s="76">
         <v>44139.0</v>
@@ -9499,7 +9653,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="71" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
       <c r="O10" s="78" t="s">
         <v>37</v>
@@ -9583,13 +9737,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -9604,7 +9758,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -9621,13 +9775,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>156</v>
+        <v>169</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>157</v>
+        <v>170</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>158</v>
+        <v>171</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -9637,7 +9791,7 @@
         <v>dpv:DataController</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -9653,7 +9807,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>27</v>
@@ -9674,22 +9828,22 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>161</v>
+        <v>174</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>162</v>
+        <v>175</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>163</v>
+        <v>176</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>164</v>
+        <v>177</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -9703,7 +9857,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="O3" s="86" t="s">
         <v>31</v>
@@ -9724,22 +9878,22 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>167</v>
+        <v>180</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -9753,7 +9907,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="O4" s="86" t="s">
         <v>31</v>
@@ -9774,28 +9928,28 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>170</v>
+        <v>183</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="K5" s="15">
         <v>43559.0</v>
@@ -9807,7 +9961,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="O5" s="45" t="s">
         <v>27</v>
@@ -9828,22 +9982,22 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>148</v>
+        <v>161</v>
       </c>
       <c r="F6" s="84" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -9857,7 +10011,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="O6" s="86" t="s">
         <v>31</v>
@@ -9878,22 +10032,22 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
       <c r="F7" s="84" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -9907,7 +10061,7 @@
         <v>19</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="O7" s="86" t="s">
         <v>31</v>
@@ -9928,22 +10082,22 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -9957,7 +10111,7 @@
         <v>19</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="O8" s="86" t="s">
         <v>31</v>
@@ -9978,22 +10132,22 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -10007,7 +10161,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="O9" s="86" t="s">
         <v>31</v>
@@ -10028,22 +10182,22 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>194</v>
+        <v>207</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -10057,10 +10211,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="O10" s="86" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10171,13 +10325,13 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>34</v>
@@ -10219,16 +10373,16 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="B3" s="88" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>200</v>
+        <v>213</v>
       </c>
       <c r="D3" s="84" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>26</v>
@@ -10238,7 +10392,7 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="21" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="K3" s="25">
         <v>44594.0</v>
@@ -10271,16 +10425,16 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>203</v>
+        <v>215</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>204</v>
+        <v>216</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>205</v>
+        <v>217</v>
       </c>
       <c r="D4" s="84" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -10321,16 +10475,16 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>206</v>
+        <v>218</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="D5" s="84" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -10340,7 +10494,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="21" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="K5" s="25">
         <v>44594.0</v>
@@ -10373,16 +10527,16 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>209</v>
+        <v>221</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>210</v>
+        <v>222</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>211</v>
+        <v>223</v>
       </c>
       <c r="D6" s="84" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -10423,16 +10577,16 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>212</v>
+        <v>224</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>214</v>
+        <v>226</v>
       </c>
       <c r="D7" s="84" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>26</v>
@@ -10442,7 +10596,7 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="21" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="K7" s="25">
         <v>44594.0</v>
@@ -10475,16 +10629,16 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>215</v>
+        <v>227</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>216</v>
+        <v>228</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="D8" s="84" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>26</v>
@@ -10494,7 +10648,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
@@ -10527,16 +10681,16 @@
     </row>
     <row r="9">
       <c r="A9" s="48" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="D9" s="90" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>26</v>
@@ -10546,7 +10700,7 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="57" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="K9" s="52">
         <v>44643.0</v>
@@ -10558,10 +10712,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="O9" s="91" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
@@ -10579,13 +10733,13 @@
     </row>
     <row r="10">
       <c r="A10" s="48" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>25</v>
@@ -10606,10 +10760,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
       <c r="O10" s="91" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10627,10 +10781,10 @@
     </row>
     <row r="11">
       <c r="A11" s="92" t="s">
-        <v>228</v>
+        <v>240</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>229</v>
+        <v>241</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="13" t="s">
@@ -10667,10 +10821,10 @@
     </row>
     <row r="12">
       <c r="A12" s="92" t="s">
-        <v>230</v>
+        <v>242</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>231</v>
+        <v>243</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="13" t="s">
@@ -10707,10 +10861,10 @@
     </row>
     <row r="13">
       <c r="A13" s="92" t="s">
-        <v>232</v>
+        <v>244</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="13" t="s">
@@ -10747,10 +10901,10 @@
     </row>
     <row r="14">
       <c r="A14" s="92" t="s">
-        <v>234</v>
+        <v>246</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>235</v>
+        <v>247</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="13" t="s">
@@ -10787,10 +10941,10 @@
     </row>
     <row r="15">
       <c r="A15" s="92" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="13" t="s">
@@ -10827,16 +10981,16 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>239</v>
+        <v>251</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>240</v>
+        <v>252</v>
       </c>
       <c r="D16" s="37" t="s">
-        <v>201</v>
+        <v>49</v>
       </c>
       <c r="E16" s="37" t="s">
         <v>26</v>
@@ -10919,13 +11073,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -10940,7 +11094,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="35" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -10957,13 +11111,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>241</v>
+        <v>253</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -10973,7 +11127,7 @@
         <v>dpv:DataSubject</v>
       </c>
       <c r="F2" s="59" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -10989,7 +11143,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>27</v>
@@ -11010,13 +11164,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>246</v>
+        <v>258</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -11052,13 +11206,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>247</v>
+        <v>259</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>249</v>
+        <v>261</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>25</v>
@@ -11067,7 +11221,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -11081,10 +11235,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>250</v>
+        <v>262</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>251</v>
+        <v>263</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11193,13 +11347,13 @@
     </row>
     <row r="2">
       <c r="A2" s="94" t="s">
-        <v>252</v>
+        <v>264</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>253</v>
+        <v>265</v>
       </c>
       <c r="C2" s="96" t="s">
-        <v>254</v>
+        <v>266</v>
       </c>
       <c r="D2" s="97" t="s">
         <v>34</v>
@@ -11211,10 +11365,10 @@
       <c r="G2" s="98"/>
       <c r="H2" s="98"/>
       <c r="I2" s="97" t="s">
-        <v>255</v>
+        <v>267</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>256</v>
+        <v>268</v>
       </c>
       <c r="K2" s="100">
         <v>43560.0</v>
@@ -11226,7 +11380,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="97" t="s">
-        <v>110</v>
+        <v>123</v>
       </c>
       <c r="O2" s="101" t="s">
         <v>27</v>
@@ -11251,23 +11405,23 @@
     </row>
     <row r="3">
       <c r="A3" s="59" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>257</v>
+        <v>269</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="102" t="s">
-        <v>260</v>
+        <v>272</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="25">
@@ -11283,7 +11437,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="102" t="s">
-        <v>122</v>
+        <v>135</v>
       </c>
       <c r="P3" s="28"/>
       <c r="Q3" s="28"/>
@@ -11305,17 +11459,17 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>261</v>
+        <v>273</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>262</v>
+        <v>274</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -11330,10 +11484,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11355,23 +11509,23 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>267</v>
+        <v>279</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="104" t="s">
-        <v>268</v>
+        <v>280</v>
       </c>
       <c r="J5" s="59"/>
       <c r="K5" s="25">
@@ -11382,7 +11536,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="59" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="O5" s="102" t="s">
         <v>37</v>
@@ -11407,17 +11561,17 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>269</v>
+        <v>281</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>270</v>
+        <v>282</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -11432,10 +11586,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -11457,17 +11611,17 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>273</v>
+        <v>285</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>274</v>
+        <v>286</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -11482,10 +11636,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -11507,17 +11661,17 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -11532,10 +11686,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -11557,17 +11711,17 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>278</v>
+        <v>290</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -11582,10 +11736,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -11607,17 +11761,17 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>279</v>
+        <v>291</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>280</v>
+        <v>292</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>281</v>
+        <v>293</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -11632,10 +11786,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -11657,17 +11811,17 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>282</v>
+        <v>294</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>283</v>
+        <v>295</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -11682,10 +11836,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
@@ -11707,17 +11861,17 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>284</v>
+        <v>296</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>285</v>
+        <v>297</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -11732,10 +11886,10 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -11757,23 +11911,23 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>286</v>
+        <v>298</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>287</v>
+        <v>299</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>288</v>
+        <v>300</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -11784,10 +11938,10 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -11809,17 +11963,17 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>289</v>
+        <v>301</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>290</v>
+        <v>302</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -11834,10 +11988,10 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -11859,17 +12013,17 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>291</v>
+        <v>303</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>292</v>
+        <v>304</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -11884,10 +12038,10 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O15" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -11909,17 +12063,17 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>293</v>
+        <v>305</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>294</v>
+        <v>306</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>295</v>
+        <v>307</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -11934,10 +12088,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O16" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -11959,17 +12113,17 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>296</v>
+        <v>308</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>297</v>
+        <v>309</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -11984,10 +12138,10 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -12009,17 +12163,17 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>298</v>
+        <v>310</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>299</v>
+        <v>311</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -12034,10 +12188,10 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O18" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
@@ -12059,17 +12213,17 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>300</v>
+        <v>312</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>301</v>
+        <v>313</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -12084,10 +12238,10 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O19" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
@@ -12109,23 +12263,23 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>302</v>
+        <v>314</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>303</v>
+        <v>315</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="15">
@@ -12136,10 +12290,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O20" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
@@ -12161,19 +12315,19 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>305</v>
+        <v>317</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>306</v>
+        <v>318</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>307</v>
+        <v>319</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -12188,10 +12342,10 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O21" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -12213,17 +12367,17 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>308</v>
+        <v>320</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>309</v>
+        <v>321</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -12238,10 +12392,10 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="O22" s="45" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -12263,19 +12417,19 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>310</v>
+        <v>322</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>311</v>
+        <v>323</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>312</v>
+        <v>324</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -12290,10 +12444,10 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="O23" s="45" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -12315,19 +12469,19 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>316</v>
+        <v>328</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>317</v>
+        <v>329</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>318</v>
+        <v>330</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -12342,10 +12496,10 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="O24" s="45" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -12367,19 +12521,19 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>319</v>
+        <v>331</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>320</v>
+        <v>332</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>321</v>
+        <v>333</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>313</v>
+        <v>325</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -12394,10 +12548,10 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="O25" s="45" t="s">
-        <v>315</v>
+        <v>327</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -12419,17 +12573,17 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>322</v>
+        <v>334</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>323</v>
+        <v>335</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>324</v>
+        <v>336</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -12444,10 +12598,10 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -12469,17 +12623,17 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>326</v>
+        <v>338</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>327</v>
+        <v>339</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>328</v>
+        <v>340</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="62" t="s">
-        <v>259</v>
+        <v>271</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -12494,10 +12648,10 @@
         <v>19</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>314</v>
+        <v>326</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>325</v>
+        <v>337</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>

</xml_diff>

<commit_message>
adds dpv:Service and Provider/Consumer roles
closes #124
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="853" uniqueCount="356">
   <si>
     <t>Term</t>
   </si>
@@ -604,6 +604,24 @@
     <t>Georg Krog, Paul Ryan</t>
   </si>
   <si>
+    <t>ServiceProvider</t>
+  </si>
+  <si>
+    <t>Service Provider</t>
+  </si>
+  <si>
+    <t>The entity that provides a service</t>
+  </si>
+  <si>
+    <t>ServiceConsumer</t>
+  </si>
+  <si>
+    <t>Service Consumer</t>
+  </si>
+  <si>
+    <t>The entity that consumes or receives the service</t>
+  </si>
+  <si>
     <t>hasDataController</t>
   </si>
   <si>
@@ -723,6 +741,33 @@
   </si>
   <si>
     <t>Paul Ryan, Rob Brennan</t>
+  </si>
+  <si>
+    <t>hasServiceProvider</t>
+  </si>
+  <si>
+    <t>has service provider</t>
+  </si>
+  <si>
+    <t>Indicates the entity that provides the associated service</t>
+  </si>
+  <si>
+    <t>dpv:Service</t>
+  </si>
+  <si>
+    <t>dpv:ServiceProvider</t>
+  </si>
+  <si>
+    <t>hasServiceConsumer</t>
+  </si>
+  <si>
+    <t>has service consumer</t>
+  </si>
+  <si>
+    <t>Indicates the entity that consumes or receives the associated service</t>
+  </si>
+  <si>
+    <t>dpv:ServiceConsumer</t>
   </si>
   <si>
     <t>Organisation</t>
@@ -9672,13 +9717,105 @@
       <c r="AA10" s="74"/>
       <c r="AB10" s="74"/>
     </row>
+    <row r="11">
+      <c r="A11" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15">
+        <v>45402.0</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15">
+        <v>45402.0</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AB10">
     <cfRule type="expression" dxfId="3" priority="1">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AB10">
+  <conditionalFormatting sqref="A2:AB100">
     <cfRule type="expression" dxfId="2" priority="2">
       <formula>$M2="accepted"</formula>
     </cfRule>
@@ -9775,13 +9912,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>169</v>
+        <v>175</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>170</v>
+        <v>176</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>171</v>
+        <v>177</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -9807,7 +9944,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>172</v>
+        <v>178</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>27</v>
@@ -9828,22 +9965,22 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>174</v>
+        <v>180</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>176</v>
+        <v>182</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>177</v>
+        <v>183</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -9857,7 +9994,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O3" s="86" t="s">
         <v>31</v>
@@ -9878,13 +10015,13 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>179</v>
+        <v>185</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>181</v>
+        <v>187</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>17</v>
@@ -9893,7 +10030,7 @@
         <v>133</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -9907,7 +10044,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O4" s="86" t="s">
         <v>31</v>
@@ -9928,13 +10065,13 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>183</v>
+        <v>189</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>184</v>
+        <v>190</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>185</v>
+        <v>191</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
@@ -9949,7 +10086,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>186</v>
+        <v>192</v>
       </c>
       <c r="K5" s="15">
         <v>43559.0</v>
@@ -9961,7 +10098,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="O5" s="45" t="s">
         <v>27</v>
@@ -9982,13 +10119,13 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>188</v>
+        <v>194</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>189</v>
+        <v>195</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>190</v>
+        <v>196</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
@@ -9997,7 +10134,7 @@
         <v>161</v>
       </c>
       <c r="F6" s="84" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -10011,7 +10148,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O6" s="86" t="s">
         <v>31</v>
@@ -10032,22 +10169,22 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>191</v>
+        <v>197</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>192</v>
+        <v>198</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>193</v>
+        <v>199</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>194</v>
+        <v>200</v>
       </c>
       <c r="F7" s="84" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -10061,7 +10198,7 @@
         <v>19</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O7" s="86" t="s">
         <v>31</v>
@@ -10082,19 +10219,19 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>77</v>
@@ -10111,7 +10248,7 @@
         <v>19</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O8" s="86" t="s">
         <v>31</v>
@@ -10132,22 +10269,22 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>202</v>
+        <v>208</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -10161,7 +10298,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>178</v>
+        <v>184</v>
       </c>
       <c r="O9" s="86" t="s">
         <v>31</v>
@@ -10182,22 +10319,22 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>207</v>
+        <v>213</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -10211,7 +10348,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>208</v>
+        <v>214</v>
       </c>
       <c r="O10" s="86" t="s">
         <v>81</v>
@@ -10229,6 +10366,102 @@
       <c r="Z10" s="23"/>
       <c r="AA10" s="23"/>
       <c r="AB10" s="23"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="13" t="s">
+        <v>215</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15">
+        <v>45402.0</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>218</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15">
+        <v>45402.0</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AB13">
@@ -10325,13 +10558,13 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>34</v>
@@ -10373,13 +10606,13 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="B3" s="88" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>213</v>
+        <v>228</v>
       </c>
       <c r="D3" s="84" t="s">
         <v>49</v>
@@ -10392,7 +10625,7 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="21" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="K3" s="25">
         <v>44594.0</v>
@@ -10425,13 +10658,13 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="B4" s="62" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D4" s="84" t="s">
         <v>49</v>
@@ -10475,13 +10708,13 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>218</v>
+        <v>233</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>219</v>
+        <v>234</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>220</v>
+        <v>235</v>
       </c>
       <c r="D5" s="84" t="s">
         <v>49</v>
@@ -10494,7 +10727,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="21" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="K5" s="25">
         <v>44594.0</v>
@@ -10527,13 +10760,13 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="D6" s="84" t="s">
         <v>49</v>
@@ -10577,13 +10810,13 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="D7" s="84" t="s">
         <v>49</v>
@@ -10596,7 +10829,7 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="21" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="K7" s="25">
         <v>44594.0</v>
@@ -10629,13 +10862,13 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>229</v>
+        <v>244</v>
       </c>
       <c r="D8" s="84" t="s">
         <v>49</v>
@@ -10648,7 +10881,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
@@ -10681,13 +10914,13 @@
     </row>
     <row r="9">
       <c r="A9" s="48" t="s">
-        <v>230</v>
+        <v>245</v>
       </c>
       <c r="B9" s="48" t="s">
-        <v>231</v>
+        <v>246</v>
       </c>
       <c r="C9" s="48" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="D9" s="90" t="s">
         <v>49</v>
@@ -10700,7 +10933,7 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="57" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="K9" s="52">
         <v>44643.0</v>
@@ -10712,10 +10945,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="48" t="s">
-        <v>234</v>
+        <v>249</v>
       </c>
       <c r="O9" s="91" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="P9" s="28"/>
       <c r="Q9" s="28"/>
@@ -10733,13 +10966,13 @@
     </row>
     <row r="10">
       <c r="A10" s="48" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>25</v>
@@ -10760,10 +10993,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="48" t="s">
-        <v>239</v>
+        <v>254</v>
       </c>
       <c r="O10" s="91" t="s">
-        <v>235</v>
+        <v>250</v>
       </c>
       <c r="P10" s="28"/>
       <c r="Q10" s="28"/>
@@ -10781,10 +11014,10 @@
     </row>
     <row r="11">
       <c r="A11" s="92" t="s">
-        <v>240</v>
+        <v>255</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>241</v>
+        <v>256</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="13" t="s">
@@ -10821,10 +11054,10 @@
     </row>
     <row r="12">
       <c r="A12" s="92" t="s">
-        <v>242</v>
+        <v>257</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="13" t="s">
@@ -10861,10 +11094,10 @@
     </row>
     <row r="13">
       <c r="A13" s="92" t="s">
-        <v>244</v>
+        <v>259</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>245</v>
+        <v>260</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="13" t="s">
@@ -10901,10 +11134,10 @@
     </row>
     <row r="14">
       <c r="A14" s="92" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>247</v>
+        <v>262</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="13" t="s">
@@ -10941,10 +11174,10 @@
     </row>
     <row r="15">
       <c r="A15" s="92" t="s">
-        <v>248</v>
+        <v>263</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>249</v>
+        <v>264</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="13" t="s">
@@ -10981,13 +11214,13 @@
     </row>
     <row r="16">
       <c r="A16" s="36" t="s">
-        <v>250</v>
+        <v>265</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>251</v>
+        <v>266</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>252</v>
+        <v>267</v>
       </c>
       <c r="D16" s="37" t="s">
         <v>49</v>
@@ -11111,13 +11344,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>253</v>
+        <v>268</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>254</v>
+        <v>269</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>255</v>
+        <v>270</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -11143,7 +11376,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>187</v>
+        <v>193</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>27</v>
@@ -11164,13 +11397,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>256</v>
+        <v>271</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>17</v>
@@ -11206,13 +11439,13 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>261</v>
+        <v>276</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>25</v>
@@ -11235,10 +11468,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="13" t="s">
-        <v>262</v>
+        <v>277</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>263</v>
+        <v>278</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11347,13 +11580,13 @@
     </row>
     <row r="2">
       <c r="A2" s="94" t="s">
-        <v>264</v>
+        <v>279</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>265</v>
+        <v>280</v>
       </c>
       <c r="C2" s="96" t="s">
-        <v>266</v>
+        <v>281</v>
       </c>
       <c r="D2" s="97" t="s">
         <v>34</v>
@@ -11365,10 +11598,10 @@
       <c r="G2" s="98"/>
       <c r="H2" s="98"/>
       <c r="I2" s="97" t="s">
-        <v>267</v>
+        <v>282</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>268</v>
+        <v>283</v>
       </c>
       <c r="K2" s="100">
         <v>43560.0</v>
@@ -11405,23 +11638,23 @@
     </row>
     <row r="3">
       <c r="A3" s="59" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="B3" s="60" t="s">
-        <v>269</v>
+        <v>284</v>
       </c>
       <c r="C3" s="59" t="s">
-        <v>270</v>
+        <v>285</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="102" t="s">
-        <v>272</v>
+        <v>287</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="25">
@@ -11459,17 +11692,17 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>274</v>
+        <v>289</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -11484,10 +11717,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="37" t="s">
-        <v>275</v>
+        <v>290</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>276</v>
+        <v>291</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11509,23 +11742,23 @@
     </row>
     <row r="5">
       <c r="A5" s="59" t="s">
-        <v>277</v>
+        <v>292</v>
       </c>
       <c r="B5" s="60" t="s">
-        <v>278</v>
+        <v>293</v>
       </c>
       <c r="C5" s="59" t="s">
-        <v>279</v>
+        <v>294</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="104" t="s">
-        <v>280</v>
+        <v>295</v>
       </c>
       <c r="J5" s="59"/>
       <c r="K5" s="25">
@@ -11561,17 +11794,17 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>281</v>
+        <v>296</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>282</v>
+        <v>297</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -11586,10 +11819,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -11611,17 +11844,17 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>285</v>
+        <v>300</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>286</v>
+        <v>301</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -11636,10 +11869,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O7" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -11661,17 +11894,17 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>287</v>
+        <v>302</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -11686,10 +11919,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O8" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -11711,17 +11944,17 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>289</v>
+        <v>304</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>289</v>
+        <v>304</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>290</v>
+        <v>305</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -11736,10 +11969,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O9" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -11761,17 +11994,17 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>291</v>
+        <v>306</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>292</v>
+        <v>307</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>293</v>
+        <v>308</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -11786,10 +12019,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O10" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -11811,17 +12044,17 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>294</v>
+        <v>309</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>295</v>
+        <v>310</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -11836,10 +12069,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O11" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
@@ -11861,17 +12094,17 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -11886,10 +12119,10 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O12" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -11911,23 +12144,23 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>298</v>
+        <v>313</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>299</v>
+        <v>314</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -11938,10 +12171,10 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O13" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -11963,17 +12196,17 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -11988,10 +12221,10 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O14" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -12013,17 +12246,17 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>303</v>
+        <v>318</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>304</v>
+        <v>319</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -12038,10 +12271,10 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O15" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -12063,17 +12296,17 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>305</v>
+        <v>320</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>306</v>
+        <v>321</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>307</v>
+        <v>322</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -12088,10 +12321,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O16" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -12113,17 +12346,17 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>309</v>
+        <v>324</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -12138,10 +12371,10 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O17" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -12163,17 +12396,17 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>310</v>
+        <v>325</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>311</v>
+        <v>326</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -12188,10 +12421,10 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O18" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
@@ -12213,17 +12446,17 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>312</v>
+        <v>327</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>313</v>
+        <v>328</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -12238,10 +12471,10 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O19" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
@@ -12263,23 +12496,23 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>314</v>
+        <v>329</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>315</v>
+        <v>330</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13" t="s">
-        <v>316</v>
+        <v>331</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="15">
@@ -12290,10 +12523,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O20" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
@@ -12315,19 +12548,19 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>317</v>
+        <v>332</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>318</v>
+        <v>333</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>319</v>
+        <v>334</v>
       </c>
       <c r="E21" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -12342,10 +12575,10 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O21" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -12367,17 +12600,17 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>320</v>
+        <v>335</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>321</v>
+        <v>336</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -12392,10 +12625,10 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>283</v>
+        <v>298</v>
       </c>
       <c r="O22" s="45" t="s">
-        <v>284</v>
+        <v>299</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -12417,19 +12650,19 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>322</v>
+        <v>337</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>323</v>
+        <v>338</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>324</v>
+        <v>339</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="E23" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -12444,10 +12677,10 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="O23" s="45" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -12469,19 +12702,19 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>328</v>
+        <v>343</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>329</v>
+        <v>344</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="E24" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -12496,10 +12729,10 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="O24" s="45" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -12521,19 +12754,19 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>333</v>
+        <v>348</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>325</v>
+        <v>340</v>
       </c>
       <c r="E25" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -12548,10 +12781,10 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="O25" s="45" t="s">
-        <v>327</v>
+        <v>342</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -12573,17 +12806,17 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>336</v>
+        <v>351</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -12598,10 +12831,10 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="O26" s="45" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -12623,17 +12856,17 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>338</v>
+        <v>353</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>339</v>
+        <v>354</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>340</v>
+        <v>355</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="62" t="s">
-        <v>271</v>
+        <v>286</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -12648,10 +12881,10 @@
         <v>19</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>326</v>
+        <v>341</v>
       </c>
       <c r="O27" s="45" t="s">
-        <v>337</v>
+        <v>352</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>

</xml_diff>

<commit_message>
documentation dpv/entities module; new example
- adds documentation for entities module in dpv (separate page)
- adds examples for entities
- adds property for organisational unit (was missing)
- fixes misc. issues in entities page
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="921" uniqueCount="381">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="937" uniqueCount="388">
   <si>
     <t>Term</t>
   </si>
@@ -293,6 +293,27 @@
   </si>
   <si>
     <t>Indicates this entity is the subsidiary of the specified entity</t>
+  </si>
+  <si>
+    <t>hasOrganisationalUnit</t>
+  </si>
+  <si>
+    <t>has organisational unit</t>
+  </si>
+  <si>
+    <t>Indicates the specified entity is a unit of the organisation</t>
+  </si>
+  <si>
+    <t>dpv:OrganisationalUnit</t>
+  </si>
+  <si>
+    <t>isOrganistionalUnitOf</t>
+  </si>
+  <si>
+    <t>is organisational unit of</t>
+  </si>
+  <si>
+    <t>Indicates this entity is an organisational unit of the specified entity</t>
   </si>
   <si>
     <t>Authority</t>
@@ -5515,13 +5536,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="C2" s="80" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -5547,7 +5568,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>27</v>
@@ -5568,13 +5589,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>25</v>
@@ -5597,10 +5618,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="O3" s="46" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -6143,6 +6164,102 @@
       <c r="Z10" s="14"/>
       <c r="AA10" s="14"/>
       <c r="AB10" s="14"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15">
+        <v>45453.0</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
+      <c r="R11" s="14"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
+      <c r="Y11" s="14"/>
+      <c r="Z11" s="14"/>
+      <c r="AA11" s="14"/>
+      <c r="AB11" s="14"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="F12" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="15">
+        <v>45453.0</v>
+      </c>
+      <c r="L12" s="14"/>
+      <c r="M12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="14"/>
+      <c r="P12" s="14"/>
+      <c r="Q12" s="14"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
+      <c r="Y12" s="14"/>
+      <c r="Z12" s="14"/>
+      <c r="AA12" s="14"/>
+      <c r="AB12" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="O7">
@@ -6255,16 +6372,16 @@
     </row>
     <row r="2">
       <c r="A2" s="48" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="C2" s="49" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="D2" s="50" t="s">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="E2" s="51" t="s">
         <v>26</v>
@@ -6282,7 +6399,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="54" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="O2" s="55" t="s">
         <v>37</v>
@@ -6303,16 +6420,16 @@
     </row>
     <row r="3">
       <c r="A3" s="48" t="s">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B3" s="56" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C3" s="49" t="s">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="D3" s="49" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E3" s="54" t="s">
         <v>26</v>
@@ -6330,7 +6447,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="54" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="O3" s="55" t="s">
         <v>37</v>
@@ -6351,16 +6468,16 @@
     </row>
     <row r="4">
       <c r="A4" s="49" t="s">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B4" s="54" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="C4" s="54" t="s">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="D4" s="49" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -6370,7 +6487,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="57"/>
       <c r="J4" s="58" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="K4" s="53">
         <v>44594.0</v>
@@ -6401,16 +6518,16 @@
     </row>
     <row r="5">
       <c r="A5" s="56" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B5" s="54" t="s">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="C5" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D5" s="56" t="s">
         <v>105</v>
-      </c>
-      <c r="D5" s="56" t="s">
-        <v>98</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -6420,7 +6537,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="58" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="K5" s="53">
         <v>44594.0</v>
@@ -6451,16 +6568,16 @@
     </row>
     <row r="6">
       <c r="A6" s="49" t="s">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B6" s="54" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="C6" s="54" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="D6" s="49" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -6470,7 +6587,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="59" t="s">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="K6" s="53">
         <v>44594.0</v>
@@ -9384,19 +9501,19 @@
     </row>
     <row r="2">
       <c r="A2" s="37" t="s">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B2" s="38" t="s">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="38" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="F2" s="44"/>
       <c r="G2" s="39"/>
@@ -9414,7 +9531,7 @@
         <v>50</v>
       </c>
       <c r="O2" s="43" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="P2" s="44"/>
       <c r="Q2" s="44"/>
@@ -9432,16 +9549,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -9462,7 +9579,7 @@
         <v>50</v>
       </c>
       <c r="O3" s="43" t="s">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -9586,13 +9703,13 @@
     </row>
     <row r="2">
       <c r="A2" s="60" t="s">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B2" s="61" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="C2" s="62" t="s">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="D2" s="60" t="s">
         <v>34</v>
@@ -9604,10 +9721,10 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="27" t="s">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="J2" s="63" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="K2" s="25">
         <v>43560.0</v>
@@ -9619,7 +9736,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="60" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="O2" s="28" t="s">
         <v>27</v>
@@ -9640,16 +9757,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -9659,7 +9776,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="64" t="s">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="K3" s="15">
         <v>43620.0</v>
@@ -9672,7 +9789,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="46" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -9690,16 +9807,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>26</v>
@@ -9708,7 +9825,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="13" t="s">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="15">
@@ -9722,7 +9839,7 @@
         <v>20</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -9740,13 +9857,13 @@
     </row>
     <row r="5">
       <c r="A5" s="60" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="D5" s="60" t="s">
         <v>34</v>
@@ -9756,16 +9873,16 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="I5" s="65" t="s">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="J5" s="66" t="s">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="K5" s="25">
         <v>43560.0</v>
@@ -9777,7 +9894,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="60" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>27</v>
@@ -9798,16 +9915,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E6" s="13" t="s">
         <v>26</v>
@@ -9816,10 +9933,10 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="13" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="J6" s="64" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="K6" s="15">
         <v>43620.0</v>
@@ -9834,7 +9951,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="46" t="s">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -9852,13 +9969,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>34</v>
@@ -9870,10 +9987,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="13" t="s">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="J7" s="67" t="s">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="K7" s="15">
         <v>44447.0</v>
@@ -9883,10 +10000,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="38" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="O7" s="46" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -9904,16 +10021,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>26</v>
@@ -9922,10 +10039,10 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="68" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="J8" s="67" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="K8" s="15">
         <v>44447.0</v>
@@ -9935,10 +10052,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="38" t="s">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -9956,16 +10073,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>26</v>
@@ -9974,7 +10091,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="13" t="s">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="15">
@@ -9985,7 +10102,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="38" t="s">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="O9" s="46" t="s">
         <v>21</v>
@@ -10006,13 +10123,13 @@
     </row>
     <row r="10">
       <c r="A10" s="69" t="s">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B10" s="69" t="s">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="C10" s="70" t="s">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="D10" s="71" t="s">
         <v>76</v>
@@ -10025,7 +10142,7 @@
       <c r="H10" s="73"/>
       <c r="I10" s="73"/>
       <c r="J10" s="74" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="K10" s="75">
         <v>44139.0</v>
@@ -10037,7 +10154,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="77" t="s">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="O10" s="78" t="s">
         <v>37</v>
@@ -10058,13 +10175,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>34</v>
@@ -10104,13 +10221,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>34</v>
@@ -10251,13 +10368,13 @@
     </row>
     <row r="2">
       <c r="A2" s="80" t="s">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="C2" s="81" t="s">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="D2" s="80" t="s">
         <v>17</v>
@@ -10283,7 +10400,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="80" t="s">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="O2" s="83" t="s">
         <v>27</v>
@@ -10304,22 +10421,22 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="F3" s="84" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -10333,7 +10450,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="O3" s="86" t="s">
         <v>31</v>
@@ -10354,22 +10471,22 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="F4" s="84" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -10383,7 +10500,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="O4" s="86" t="s">
         <v>31</v>
@@ -10404,19 +10521,19 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C5" s="87" t="s">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="F5" s="13" t="s">
         <v>77</v>
@@ -10425,7 +10542,7 @@
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="K5" s="15">
         <v>43559.0</v>
@@ -10437,7 +10554,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="O5" s="46" t="s">
         <v>27</v>
@@ -10458,22 +10575,22 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="F6" s="84" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -10487,7 +10604,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="O6" s="86" t="s">
         <v>31</v>
@@ -10508,22 +10625,22 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>198</v>
+        <v>205</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>199</v>
+        <v>206</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>200</v>
+        <v>207</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>201</v>
+        <v>208</v>
       </c>
       <c r="F7" s="84" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -10537,7 +10654,7 @@
         <v>19</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="O7" s="86" t="s">
         <v>31</v>
@@ -10558,19 +10675,19 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>202</v>
+        <v>209</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>204</v>
+        <v>211</v>
       </c>
       <c r="D8" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="21" t="s">
-        <v>205</v>
+        <v>212</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>77</v>
@@ -10587,7 +10704,7 @@
         <v>19</v>
       </c>
       <c r="N8" s="21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="O8" s="86" t="s">
         <v>31</v>
@@ -10608,22 +10725,22 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>206</v>
+        <v>213</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>207</v>
+        <v>214</v>
       </c>
       <c r="C9" s="21" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>209</v>
+        <v>216</v>
       </c>
       <c r="F9" s="84" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -10637,7 +10754,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="O9" s="86" t="s">
         <v>31</v>
@@ -10658,22 +10775,22 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>210</v>
+        <v>217</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>211</v>
+        <v>218</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="F10" s="84" t="s">
-        <v>214</v>
+        <v>221</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -10687,7 +10804,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>215</v>
+        <v>222</v>
       </c>
       <c r="O10" s="86" t="s">
         <v>81</v>
@@ -10708,19 +10825,19 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>216</v>
+        <v>223</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>217</v>
+        <v>224</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>218</v>
+        <v>225</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>220</v>
+        <v>227</v>
       </c>
       <c r="F11" s="13" t="s">
         <v>77</v>
@@ -10756,19 +10873,19 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>222</v>
+        <v>229</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>219</v>
+        <v>226</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="F12" s="13" t="s">
         <v>77</v>
@@ -10897,13 +11014,13 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="B2" s="80" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>34</v>
@@ -10945,13 +11062,13 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>227</v>
+        <v>234</v>
       </c>
       <c r="B3" s="88" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="D3" s="84" t="s">
         <v>49</v>
@@ -10964,7 +11081,7 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="21" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="K3" s="25">
         <v>44594.0</v>
@@ -10997,13 +11114,13 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>231</v>
+        <v>238</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>232</v>
+        <v>239</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>233</v>
+        <v>240</v>
       </c>
       <c r="D4" s="84" t="s">
         <v>49</v>
@@ -11047,13 +11164,13 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>234</v>
+        <v>241</v>
       </c>
       <c r="B5" s="88" t="s">
-        <v>235</v>
+        <v>242</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>236</v>
+        <v>243</v>
       </c>
       <c r="D5" s="84" t="s">
         <v>49</v>
@@ -11066,7 +11183,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="21" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="K5" s="25">
         <v>44594.0</v>
@@ -11099,13 +11216,13 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>237</v>
+        <v>244</v>
       </c>
       <c r="B6" s="88" t="s">
-        <v>238</v>
+        <v>245</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>239</v>
+        <v>246</v>
       </c>
       <c r="D6" s="84" t="s">
         <v>49</v>
@@ -11149,13 +11266,13 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>240</v>
+        <v>247</v>
       </c>
       <c r="B7" s="88" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>242</v>
+        <v>249</v>
       </c>
       <c r="D7" s="84" t="s">
         <v>49</v>
@@ -11168,7 +11285,7 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="21" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="K7" s="25">
         <v>44594.0</v>
@@ -11201,13 +11318,13 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>243</v>
+        <v>250</v>
       </c>
       <c r="B8" s="88" t="s">
-        <v>244</v>
+        <v>251</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>245</v>
+        <v>252</v>
       </c>
       <c r="D8" s="84" t="s">
         <v>49</v>
@@ -11220,7 +11337,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>230</v>
+        <v>237</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
@@ -11253,13 +11370,13 @@
     </row>
     <row r="9">
       <c r="A9" s="49" t="s">
-        <v>246</v>
+        <v>253</v>
       </c>
       <c r="B9" s="49" t="s">
-        <v>247</v>
+        <v>254</v>
       </c>
       <c r="C9" s="49" t="s">
-        <v>248</v>
+        <v>255</v>
       </c>
       <c r="D9" s="90" t="s">
         <v>49</v>
@@ -11272,7 +11389,7 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="58" t="s">
-        <v>249</v>
+        <v>256</v>
       </c>
       <c r="K9" s="53">
         <v>44643.0</v>
@@ -11284,10 +11401,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="49" t="s">
-        <v>250</v>
+        <v>257</v>
       </c>
       <c r="O9" s="91" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -11305,13 +11422,13 @@
     </row>
     <row r="10">
       <c r="A10" s="49" t="s">
-        <v>252</v>
+        <v>259</v>
       </c>
       <c r="B10" s="49" t="s">
-        <v>253</v>
+        <v>260</v>
       </c>
       <c r="C10" s="90" t="s">
-        <v>254</v>
+        <v>261</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>25</v>
@@ -11332,10 +11449,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="49" t="s">
-        <v>255</v>
+        <v>262</v>
       </c>
       <c r="O10" s="91" t="s">
-        <v>251</v>
+        <v>258</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -11353,10 +11470,10 @@
     </row>
     <row r="11">
       <c r="A11" s="92" t="s">
-        <v>256</v>
+        <v>263</v>
       </c>
       <c r="B11" s="92" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="C11" s="14"/>
       <c r="D11" s="13" t="s">
@@ -11393,10 +11510,10 @@
     </row>
     <row r="12">
       <c r="A12" s="92" t="s">
-        <v>258</v>
+        <v>265</v>
       </c>
       <c r="B12" s="92" t="s">
-        <v>259</v>
+        <v>266</v>
       </c>
       <c r="C12" s="14"/>
       <c r="D12" s="13" t="s">
@@ -11433,10 +11550,10 @@
     </row>
     <row r="13">
       <c r="A13" s="92" t="s">
-        <v>260</v>
+        <v>267</v>
       </c>
       <c r="B13" s="92" t="s">
-        <v>261</v>
+        <v>268</v>
       </c>
       <c r="C13" s="14"/>
       <c r="D13" s="13" t="s">
@@ -11473,10 +11590,10 @@
     </row>
     <row r="14">
       <c r="A14" s="92" t="s">
-        <v>262</v>
+        <v>269</v>
       </c>
       <c r="B14" s="92" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="C14" s="14"/>
       <c r="D14" s="13" t="s">
@@ -11513,10 +11630,10 @@
     </row>
     <row r="15">
       <c r="A15" s="92" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="B15" s="92" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="C15" s="14"/>
       <c r="D15" s="13" t="s">
@@ -11553,13 +11670,13 @@
     </row>
     <row r="16">
       <c r="A16" s="37" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>267</v>
+        <v>274</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="D16" s="38" t="s">
         <v>49</v>
@@ -11687,13 +11804,13 @@
     </row>
     <row r="2">
       <c r="A2" s="94" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="B2" s="95" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="C2" s="96" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D2" s="97" t="s">
         <v>34</v>
@@ -11705,10 +11822,10 @@
       <c r="G2" s="98"/>
       <c r="H2" s="98"/>
       <c r="I2" s="97" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="J2" s="99" t="s">
-        <v>273</v>
+        <v>280</v>
       </c>
       <c r="K2" s="100">
         <v>43560.0</v>
@@ -11720,7 +11837,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="97" t="s">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="O2" s="101" t="s">
         <v>27</v>
@@ -11745,23 +11862,23 @@
     </row>
     <row r="3">
       <c r="A3" s="60" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="B3" s="61" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C3" s="60" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="D3" s="14"/>
       <c r="E3" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
       <c r="I3" s="102" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="J3" s="23"/>
       <c r="K3" s="25">
@@ -11777,7 +11894,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="102" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
@@ -11799,17 +11916,17 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="D4" s="14"/>
       <c r="E4" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
@@ -11824,10 +11941,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="38" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O4" s="46" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -11849,23 +11966,23 @@
     </row>
     <row r="5">
       <c r="A5" s="60" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="B5" s="61" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="C5" s="60" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="D5" s="14"/>
       <c r="E5" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="104" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="J5" s="60"/>
       <c r="K5" s="25">
@@ -11876,7 +11993,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="27" t="s">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="O5" s="102" t="s">
         <v>37</v>
@@ -11901,17 +12018,17 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
@@ -11926,10 +12043,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O6" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -11951,17 +12068,17 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
@@ -11976,10 +12093,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O7" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -12001,17 +12118,17 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
@@ -12026,10 +12143,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O8" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -12051,17 +12168,17 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
@@ -12076,10 +12193,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O9" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
@@ -12101,17 +12218,17 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
@@ -12126,10 +12243,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O10" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P10" s="14"/>
       <c r="Q10" s="14"/>
@@ -12151,17 +12268,17 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
@@ -12176,10 +12293,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O11" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P11" s="14"/>
       <c r="Q11" s="14"/>
@@ -12201,17 +12318,17 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
@@ -12226,10 +12343,10 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O12" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
@@ -12251,23 +12368,23 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
       <c r="I13" s="13" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="J13" s="14"/>
       <c r="K13" s="15">
@@ -12278,10 +12395,10 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O13" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P13" s="14"/>
       <c r="Q13" s="14"/>
@@ -12303,17 +12420,17 @@
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
@@ -12328,10 +12445,10 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O14" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P14" s="14"/>
       <c r="Q14" s="14"/>
@@ -12353,17 +12470,17 @@
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -12378,10 +12495,10 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O15" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P15" s="14"/>
       <c r="Q15" s="14"/>
@@ -12403,17 +12520,17 @@
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -12428,10 +12545,10 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O16" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P16" s="14"/>
       <c r="Q16" s="14"/>
@@ -12453,17 +12570,17 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -12478,10 +12595,10 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O17" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P17" s="14"/>
       <c r="Q17" s="14"/>
@@ -12503,17 +12620,17 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="D18" s="14"/>
       <c r="E18" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="14"/>
@@ -12528,10 +12645,10 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O18" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P18" s="14"/>
       <c r="Q18" s="14"/>
@@ -12553,17 +12670,17 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="D19" s="14"/>
       <c r="E19" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -12578,10 +12695,10 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O19" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P19" s="14"/>
       <c r="Q19" s="14"/>
@@ -12603,23 +12720,23 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="D20" s="14"/>
       <c r="E20" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
       <c r="H20" s="14"/>
       <c r="I20" s="13" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="J20" s="14"/>
       <c r="K20" s="15">
@@ -12630,10 +12747,10 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O20" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P20" s="14"/>
       <c r="Q20" s="14"/>
@@ -12655,19 +12772,19 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
@@ -12682,10 +12799,10 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O21" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P21" s="14"/>
       <c r="Q21" s="14"/>
@@ -12707,17 +12824,17 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -12732,10 +12849,10 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="O22" s="46" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
@@ -12757,19 +12874,19 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
@@ -12784,10 +12901,10 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O23" s="46" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
@@ -12809,19 +12926,19 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -12836,10 +12953,10 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O24" s="46" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
@@ -12861,19 +12978,19 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="C25" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D25" s="13" t="s">
         <v>337</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>330</v>
-      </c>
       <c r="E25" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="14"/>
@@ -12888,10 +13005,10 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O25" s="46" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="P25" s="14"/>
       <c r="Q25" s="14"/>
@@ -12913,17 +13030,17 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="D26" s="14"/>
       <c r="E26" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -12938,10 +13055,10 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O26" s="46" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
@@ -12963,17 +13080,17 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="27" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F27" s="14"/>
       <c r="G27" s="14"/>
@@ -12988,10 +13105,10 @@
         <v>19</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="O27" s="46" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="P27" s="14"/>
       <c r="Q27" s="14"/>
@@ -13137,13 +13254,13 @@
     </row>
     <row r="2">
       <c r="A2" s="33" t="s">
-        <v>269</v>
+        <v>276</v>
       </c>
       <c r="B2" s="110" t="s">
-        <v>270</v>
+        <v>277</v>
       </c>
       <c r="C2" s="111" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
       <c r="D2" s="112" t="s">
         <v>34</v>
@@ -13155,7 +13272,7 @@
       <c r="G2" s="32"/>
       <c r="H2" s="32"/>
       <c r="I2" s="112" t="s">
-        <v>272</v>
+        <v>279</v>
       </c>
       <c r="J2" s="113"/>
       <c r="K2" s="114"/>
@@ -13185,22 +13302,22 @@
     </row>
     <row r="3">
       <c r="A3" s="116" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="B3" s="117" t="s">
-        <v>274</v>
+        <v>281</v>
       </c>
       <c r="C3" s="116" t="s">
-        <v>275</v>
+        <v>282</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="F3" s="34"/>
       <c r="G3" s="34"/>
       <c r="H3" s="34"/>
       <c r="I3" s="118" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="J3" s="34"/>
       <c r="K3" s="119"/>
@@ -13208,7 +13325,7 @@
       <c r="M3" s="10"/>
       <c r="N3" s="116"/>
       <c r="O3" s="118" t="s">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="P3" s="121"/>
       <c r="Q3" s="121"/>
@@ -13235,13 +13352,13 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="10"/>
@@ -13252,7 +13369,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -13281,13 +13398,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="10"/>
@@ -13298,7 +13415,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -13327,13 +13444,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="10"/>
@@ -13344,7 +13461,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -13373,13 +13490,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="10"/>
@@ -13390,7 +13507,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
@@ -13419,13 +13536,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="10"/>
@@ -13436,7 +13553,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -13465,13 +13582,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="10"/>
@@ -13482,7 +13599,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
@@ -13511,13 +13628,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="10"/>
@@ -13528,7 +13645,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -13557,13 +13674,13 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="10"/>
@@ -13574,7 +13691,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
@@ -13603,13 +13720,13 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="B14" s="122" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="10"/>
@@ -13620,7 +13737,7 @@
       <c r="H14" s="34"/>
       <c r="I14" s="123"/>
       <c r="J14" s="13" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="K14" s="119"/>
       <c r="L14" s="124"/>

</xml_diff>

<commit_message>
Adds dpv:HumanSubject as parent of dpv:DataSubject
- adds `dpv:HumanSubject` and `dpv:hasHumanSubject`
- changed parent of `dpv:DataSubject` to `dpv:HumanSubject` with the
  same change in correponding properties
- moved data subject taxonomy with `dpv:HumanSubject` as the top concept
- added note to `tech:Subject` to use `dpv:HumanSubject` when the
  subject is a human
- includes RDF and HTML outputs
- closes #205
- This change is a result of discussions of integrating AIRO/VAIR which
  included the concept `AISubject` and the desire to reuse the existing
  data subjects taxonomy
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1033" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="443">
   <si>
     <t>Term</t>
   </si>
@@ -1085,6 +1085,12 @@
     <t>HarbourPolice</t>
   </si>
   <si>
+    <t>HumanSubject</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Delaram Golpayegani</t>
+  </si>
+  <si>
     <t>DataSubject</t>
   </si>
   <si>
@@ -1094,222 +1100,228 @@
     <t>The individual (or category of individuals) whose personal data is being processed</t>
   </si>
   <si>
+    <t>dpv:HumanSubject</t>
+  </si>
+  <si>
     <t>The term 'data subject' is specific to the GDPR, but is functionally equivalent to the term 'individual associated with data' and the ISO/IEC term 'PII Principle'</t>
   </si>
   <si>
     <t>(GDPR Art.4-1g,https://eur-lex.europa.eu/eli/reg/2016/679/art_4/par_1/oj)</t>
   </si>
   <si>
+    <t>modified</t>
+  </si>
+  <si>
     <t>Child</t>
   </si>
   <si>
     <t>A 'child' is a natural legal person who is below a certain legal age depending on the legal jurisdiction.</t>
   </si>
   <si>
+    <t>The legality of age defining a child varies by jurisdiction. In addition, 'child' is distinct from a 'minor'. For example, the legal age for consumption of alcohol can be 21, which makes a person of age 20 a 'minor' in this context. In other cases, 'minor' and 'child' are used interchangeably to refer to a person below some legally defined age.</t>
+  </si>
+  <si>
+    <t>Adult</t>
+  </si>
+  <si>
+    <t>A natural person that is not a child i.e. has attained some legally specified age of adulthood</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/2022/03/30-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>VulnerableDataSubject</t>
+  </si>
+  <si>
+    <t>Vulnerable Data Subject</t>
+  </si>
+  <si>
+    <t>Data Subjects which should be considered 'vulnerable' and therefore would require additional measures and safeguards</t>
+  </si>
+  <si>
+    <t>This concept denotes a Data Subject or a group are vulnerable, but not what vulnerability they possess or its context. This information can be provided additionally as comments, or as separate concepts and relations. Proposals for this are welcome.</t>
+  </si>
+  <si>
+    <t>Patient</t>
+  </si>
+  <si>
+    <t>Data subjects that receive medical attention, treatment, care, advice, or other health related services</t>
+  </si>
+  <si>
+    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Paul Ryan, Beatriz Esteves</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/2022/04/06-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Data subjects that are employees</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Data subjects that are students</t>
+  </si>
+  <si>
+    <t>Citizen</t>
+  </si>
+  <si>
+    <t>Data subjects that are citizens (for a jurisdiction)</t>
+  </si>
+  <si>
+    <t>NonCitizen</t>
+  </si>
+  <si>
+    <t>Non-Citizen</t>
+  </si>
+  <si>
+    <t>Data subjects that are not citizens (for a jurisdiction)</t>
+  </si>
+  <si>
+    <t>Immigrant</t>
+  </si>
+  <si>
+    <t>Data subjects that are immigrants (for a jurisdiction)</t>
+  </si>
+  <si>
+    <t>Tourist</t>
+  </si>
+  <si>
+    <t>Data subjects that are tourists i.e. not citizens and not immigrants</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Data subjects that purchase goods or services</t>
+  </si>
+  <si>
+    <t>note: for B2B relations where customers are organisations, this concept only applies for data subjects</t>
+  </si>
+  <si>
+    <t>Consumer</t>
+  </si>
+  <si>
+    <t>Data subjects that consume goods or services for direct use</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Data subjects that use service(s)</t>
+  </si>
+  <si>
+    <t>JobApplicant</t>
+  </si>
+  <si>
+    <t>Job Applicant</t>
+  </si>
+  <si>
+    <t>Data subjects that apply for jobs or employments</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>Data subjects that are temporary visitors</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>Data subjects that are members of a group, organisation, or other collectives</t>
+  </si>
+  <si>
+    <t>Applicant</t>
+  </si>
+  <si>
+    <t>Data subjects that are applicants in some context</t>
+  </si>
+  <si>
+    <t>Subscriber</t>
+  </si>
+  <si>
+    <t>Data subjects that subscribe to service(s)</t>
+  </si>
+  <si>
+    <t>note: subscriber can be customer or consumer</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Data subjects that are clients or recipients of services</t>
+  </si>
+  <si>
+    <t>dpv:Customer</t>
+  </si>
+  <si>
+    <t>Participant</t>
+  </si>
+  <si>
+    <t>Data subjects that participate in some context such as volunteers in a function</t>
+  </si>
+  <si>
+    <t>MentallyVulnerableDataSubject</t>
+  </si>
+  <si>
+    <t>Mentally Vulnerable Data Subject</t>
+  </si>
+  <si>
+    <t>Data subjects that are considered mentally vulnerable</t>
+  </si>
+  <si>
+    <t>dpv:VulnerableDataSubject</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/2022/06/15-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>AsylumSeeker</t>
+  </si>
+  <si>
+    <t>Asylum Seeker</t>
+  </si>
+  <si>
+    <t>Data subjects that are asylum seekers</t>
+  </si>
+  <si>
+    <t>ElderlyDataSubject</t>
+  </si>
+  <si>
+    <t>Elderly Data Subject</t>
+  </si>
+  <si>
+    <t>Data subjects that are considered elderly (i.e. based on age)</t>
+  </si>
+  <si>
+    <t>ParentOfDataSubject</t>
+  </si>
+  <si>
+    <t>Parent(s) of Data Subject</t>
+  </si>
+  <si>
+    <t>Parent(s) of data subjects such as children</t>
+  </si>
+  <si>
+    <t>https://lists.w3.org/Archives/Public/public-dpvcg/2022Jul/0003.html</t>
+  </si>
+  <si>
+    <t>GuardianOfDataSubject</t>
+  </si>
+  <si>
+    <t>Guardian(s) of Data Subject</t>
+  </si>
+  <si>
+    <t>Guardian(s) of data subjects such as children</t>
+  </si>
+  <si>
     <t>dpv:DataSubject</t>
   </si>
   <si>
-    <t>The legality of age defining a child varies by jurisdiction. In addition, 'child' is distinct from a 'minor'. For example, the legal age for consumption of alcohol can be 21, which makes a person of age 20 a 'minor' in this context. In other cases, 'minor' and 'child' are used interchangeably to refer to a person below some legally defined age.</t>
-  </si>
-  <si>
-    <t>Adult</t>
-  </si>
-  <si>
-    <t>A natural person that is not a child i.e. has attained some legally specified age of adulthood</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/2022/03/30-dpvcg-minutes.html</t>
-  </si>
-  <si>
-    <t>VulnerableDataSubject</t>
-  </si>
-  <si>
-    <t>Vulnerable Data Subject</t>
-  </si>
-  <si>
-    <t>Data Subjects which should be considered 'vulnerable' and therefore would require additional measures and safeguards</t>
-  </si>
-  <si>
-    <t>This concept denotes a Data Subject or a group are vulnerable, but not what vulnerability they possess or its context. This information can be provided additionally as comments, or as separate concepts and relations. Proposals for this are welcome.</t>
-  </si>
-  <si>
-    <t>Patient</t>
-  </si>
-  <si>
-    <t>Data subjects that receive medical attention, treatment, care, advice, or other health related services</t>
-  </si>
-  <si>
-    <t>Harshvardhan J. Pandit, Georg P. Krog, Julian Flake, Paul Ryan, Beatriz Esteves</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/2022/04/06-dpvcg-minutes.html</t>
-  </si>
-  <si>
-    <t>Employee</t>
-  </si>
-  <si>
-    <t>Data subjects that are employees</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Data subjects that are students</t>
-  </si>
-  <si>
-    <t>Citizen</t>
-  </si>
-  <si>
-    <t>Data subjects that are citizens (for a jurisdiction)</t>
-  </si>
-  <si>
-    <t>NonCitizen</t>
-  </si>
-  <si>
-    <t>Non-Citizen</t>
-  </si>
-  <si>
-    <t>Data subjects that are not citizens (for a jurisdiction)</t>
-  </si>
-  <si>
-    <t>Immigrant</t>
-  </si>
-  <si>
-    <t>Data subjects that are immigrants (for a jurisdiction)</t>
-  </si>
-  <si>
-    <t>Tourist</t>
-  </si>
-  <si>
-    <t>Data subjects that are tourists i.e. not citizens and not immigrants</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Data subjects that purchase goods or services</t>
-  </si>
-  <si>
-    <t>note: for B2B relations where customers are organisations, this concept only applies for data subjects</t>
-  </si>
-  <si>
-    <t>Consumer</t>
-  </si>
-  <si>
-    <t>Data subjects that consume goods or services for direct use</t>
-  </si>
-  <si>
-    <t>User</t>
-  </si>
-  <si>
-    <t>Data subjects that use service(s)</t>
-  </si>
-  <si>
-    <t>JobApplicant</t>
-  </si>
-  <si>
-    <t>Job Applicant</t>
-  </si>
-  <si>
-    <t>Data subjects that apply for jobs or employments</t>
-  </si>
-  <si>
-    <t>Visitor</t>
-  </si>
-  <si>
-    <t>Data subjects that are temporary visitors</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>Data subjects that are members of a group, organisation, or other collectives</t>
-  </si>
-  <si>
-    <t>Applicant</t>
-  </si>
-  <si>
-    <t>Data subjects that are applicants in some context</t>
-  </si>
-  <si>
-    <t>Subscriber</t>
-  </si>
-  <si>
-    <t>Data subjects that subscribe to service(s)</t>
-  </si>
-  <si>
-    <t>note: subscriber can be customer or consumer</t>
-  </si>
-  <si>
-    <t>Client</t>
-  </si>
-  <si>
-    <t>Data subjects that are clients or recipients of services</t>
-  </si>
-  <si>
-    <t>dpv:Customer</t>
-  </si>
-  <si>
-    <t>Participant</t>
-  </si>
-  <si>
-    <t>Data subjects that participate in some context such as volunteers in a function</t>
-  </si>
-  <si>
-    <t>MentallyVulnerableDataSubject</t>
-  </si>
-  <si>
-    <t>Mentally Vulnerable Data Subject</t>
-  </si>
-  <si>
-    <t>Data subjects that are considered mentally vulnerable</t>
-  </si>
-  <si>
-    <t>dpv:VulnerableDataSubject</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/2022/06/15-dpvcg-minutes.html</t>
-  </si>
-  <si>
-    <t>AsylumSeeker</t>
-  </si>
-  <si>
-    <t>Asylum Seeker</t>
-  </si>
-  <si>
-    <t>Data subjects that are asylum seekers</t>
-  </si>
-  <si>
-    <t>ElderlyDataSubject</t>
-  </si>
-  <si>
-    <t>Elderly Data Subject</t>
-  </si>
-  <si>
-    <t>Data subjects that are considered elderly (i.e. based on age)</t>
-  </si>
-  <si>
-    <t>ParentOfDataSubject</t>
-  </si>
-  <si>
-    <t>Parent(s) of Data Subject</t>
-  </si>
-  <si>
-    <t>Parent(s) of data subjects such as children</t>
-  </si>
-  <si>
-    <t>https://lists.w3.org/Archives/Public/public-dpvcg/2022Jul/0003.html</t>
-  </si>
-  <si>
-    <t>GuardianOfDataSubject</t>
-  </si>
-  <si>
-    <t>Guardian(s) of Data Subject</t>
-  </si>
-  <si>
-    <t>Guardian(s) of data subjects such as children</t>
-  </si>
-  <si>
     <t>ChildAbove13</t>
   </si>
   <si>
@@ -1403,6 +1415,9 @@
     <t>Indicates association with Data Subject</t>
   </si>
   <si>
+    <t>dpv:hasHumanSubject</t>
+  </si>
+  <si>
     <t>hasRelationWithDataSubject</t>
   </si>
   <si>
@@ -1416,6 +1431,15 @@
   </si>
   <si>
     <t>https://www.w3.org/2022/06/22-dpvcg-minutes.html</t>
+  </si>
+  <si>
+    <t>hasHumanSubject</t>
+  </si>
+  <si>
+    <t>has human subject</t>
+  </si>
+  <si>
+    <t>Indicates association with Human Subject</t>
   </si>
 </sst>
 </file>
@@ -1703,7 +1727,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="127">
+  <cellXfs count="129">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1987,6 +2011,15 @@
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1994,9 +2027,6 @@
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
@@ -2012,9 +2042,6 @@
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
@@ -2078,6 +2105,9 @@
     </xf>
     <xf borderId="0" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5689,13 +5719,13 @@
     </row>
     <row r="2">
       <c r="A2" s="82" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>17</v>
@@ -5704,8 +5734,8 @@
         <f>CONCATENATE("dpv:",RIGHT(A2,LEN(A2) - 3))</f>
         <v>dpv:DataSubject</v>
       </c>
-      <c r="F2" s="62" t="s">
-        <v>77</v>
+      <c r="F2" s="27" t="s">
+        <v>434</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -5714,11 +5744,11 @@
       <c r="K2" s="84">
         <v>43559.0</v>
       </c>
-      <c r="L2" s="84">
-        <v>44139.0</v>
-      </c>
-      <c r="M2" s="82" t="s">
-        <v>19</v>
+      <c r="L2" s="128">
+        <v>45643.0</v>
+      </c>
+      <c r="M2" s="90" t="s">
+        <v>332</v>
       </c>
       <c r="N2" s="82" t="s">
         <v>201</v>
@@ -5742,13 +5772,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>430</v>
+        <v>435</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>431</v>
+        <v>436</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>432</v>
+        <v>437</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>25</v>
@@ -5771,10 +5801,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>433</v>
+        <v>438</v>
       </c>
       <c r="O3" s="48" t="s">
-        <v>434</v>
+        <v>439</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -5789,6 +5819,54 @@
       <c r="Z3" s="14"/>
       <c r="AA3" s="14"/>
       <c r="AB3" s="14"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="13" t="s">
+        <v>440</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>441</v>
+      </c>
+      <c r="C4" s="90" t="s">
+        <v>442</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="15">
+        <v>45643.0</v>
+      </c>
+      <c r="L4" s="14"/>
+      <c r="M4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O4" s="14"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="14"/>
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="14"/>
+      <c r="Y4" s="14"/>
+      <c r="Z4" s="14"/>
+      <c r="AA4" s="14"/>
+      <c r="AB4" s="14"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2:AB36">
@@ -12523,200 +12601,146 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="27" t="s">
         <v>324</v>
       </c>
-      <c r="B2" s="97" t="s">
+      <c r="B2" s="63"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="96" t="s">
+        <v>34</v>
+      </c>
+      <c r="E2" s="96" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="97"/>
+      <c r="J2" s="23"/>
+      <c r="K2" s="25"/>
+      <c r="L2" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="27" t="s">
         <v>325</v>
       </c>
-      <c r="C2" s="98" t="s">
+      <c r="O2" s="97"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="99" t="s">
         <v>326</v>
       </c>
-      <c r="D2" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="99" t="s">
+      <c r="B3" s="100" t="s">
+        <v>327</v>
+      </c>
+      <c r="C3" s="101" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>329</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="F2" s="100"/>
-      <c r="G2" s="100"/>
-      <c r="H2" s="100"/>
-      <c r="I2" s="99" t="s">
-        <v>327</v>
-      </c>
-      <c r="J2" s="101" t="s">
-        <v>328</v>
-      </c>
-      <c r="K2" s="102">
+      <c r="F3" s="102"/>
+      <c r="G3" s="102"/>
+      <c r="H3" s="102"/>
+      <c r="I3" s="96" t="s">
+        <v>330</v>
+      </c>
+      <c r="J3" s="103" t="s">
+        <v>331</v>
+      </c>
+      <c r="K3" s="104">
         <v>43560.0</v>
       </c>
-      <c r="L2" s="102">
-        <v>44139.0</v>
-      </c>
-      <c r="M2" s="99" t="s">
-        <v>19</v>
-      </c>
-      <c r="N2" s="99" t="s">
+      <c r="L3" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M3" s="99" t="s">
+        <v>332</v>
+      </c>
+      <c r="N3" s="96" t="s">
         <v>130</v>
       </c>
-      <c r="O2" s="103" t="s">
+      <c r="O3" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="100"/>
-      <c r="Q2" s="100"/>
-      <c r="R2" s="100"/>
-      <c r="S2" s="100"/>
-      <c r="T2" s="100"/>
-      <c r="U2" s="100"/>
-      <c r="V2" s="100"/>
-      <c r="W2" s="100"/>
-      <c r="X2" s="100"/>
-      <c r="Y2" s="100"/>
-      <c r="Z2" s="100"/>
-      <c r="AA2" s="100"/>
-      <c r="AB2" s="100"/>
-      <c r="AC2" s="100"/>
-      <c r="AD2" s="100"/>
-      <c r="AE2" s="100"/>
-      <c r="AF2" s="100"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="62" t="s">
-        <v>329</v>
-      </c>
-      <c r="B3" s="63" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="62" t="s">
-        <v>330</v>
-      </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="23"/>
-      <c r="I3" s="104" t="s">
-        <v>332</v>
-      </c>
-      <c r="J3" s="23"/>
-      <c r="K3" s="25">
-        <v>44160.0</v>
-      </c>
-      <c r="L3" s="105">
-        <v>44734.0</v>
-      </c>
-      <c r="M3" s="27" t="s">
-        <v>19</v>
-      </c>
-      <c r="N3" s="62" t="s">
-        <v>20</v>
-      </c>
-      <c r="O3" s="104" t="s">
-        <v>142</v>
-      </c>
-      <c r="P3" s="29"/>
-      <c r="Q3" s="29"/>
-      <c r="R3" s="23"/>
-      <c r="S3" s="23"/>
-      <c r="T3" s="23"/>
-      <c r="U3" s="23"/>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23"/>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="23"/>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23"/>
-      <c r="AB3" s="23"/>
-      <c r="AC3" s="23"/>
-      <c r="AD3" s="23"/>
-      <c r="AE3" s="23"/>
-      <c r="AF3" s="23"/>
+      <c r="P3" s="102"/>
+      <c r="Q3" s="102"/>
+      <c r="R3" s="102"/>
+      <c r="S3" s="102"/>
+      <c r="T3" s="102"/>
+      <c r="U3" s="102"/>
+      <c r="V3" s="102"/>
+      <c r="W3" s="102"/>
+      <c r="X3" s="102"/>
+      <c r="Y3" s="102"/>
+      <c r="Z3" s="102"/>
+      <c r="AA3" s="102"/>
+      <c r="AB3" s="102"/>
+      <c r="AC3" s="102"/>
+      <c r="AD3" s="102"/>
+      <c r="AE3" s="102"/>
+      <c r="AF3" s="102"/>
     </row>
     <row r="4">
-      <c r="A4" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="B4" s="13" t="s">
-        <v>333</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>334</v>
-      </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="14"/>
-      <c r="J4" s="14"/>
-      <c r="K4" s="15">
-        <v>44650.0</v>
-      </c>
-      <c r="L4" s="14"/>
-      <c r="M4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="N4" s="40" t="s">
-        <v>266</v>
-      </c>
-      <c r="O4" s="48" t="s">
-        <v>335</v>
-      </c>
-      <c r="P4" s="14"/>
-      <c r="Q4" s="14"/>
-      <c r="R4" s="14"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
-      <c r="U4" s="14"/>
-      <c r="V4" s="14"/>
-      <c r="W4" s="14"/>
-      <c r="X4" s="14"/>
-      <c r="Y4" s="14"/>
-      <c r="Z4" s="14"/>
-      <c r="AA4" s="14"/>
-      <c r="AB4" s="14"/>
-      <c r="AC4" s="14"/>
-      <c r="AD4" s="14"/>
-      <c r="AE4" s="14"/>
-      <c r="AF4" s="14"/>
+      <c r="L4" s="98"/>
     </row>
     <row r="5">
       <c r="A5" s="62" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>338</v>
-      </c>
-      <c r="D5" s="14"/>
+        <v>334</v>
+      </c>
       <c r="E5" s="27" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="106" t="s">
-        <v>339</v>
-      </c>
-      <c r="J5" s="62"/>
+        <v>335</v>
+      </c>
+      <c r="J5" s="23"/>
       <c r="K5" s="25">
-        <v>44139.0</v>
-      </c>
-      <c r="L5" s="26"/>
-      <c r="M5" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="N5" s="27" t="s">
-        <v>101</v>
-      </c>
-      <c r="O5" s="104" t="s">
-        <v>37</v>
+        <v>44160.0</v>
+      </c>
+      <c r="L5" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M5" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="N5" s="62" t="s">
+        <v>20</v>
+      </c>
+      <c r="O5" s="106" t="s">
+        <v>142</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -12738,1168 +12762,794 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>336</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="K6" s="15">
+        <v>44650.0</v>
+      </c>
+      <c r="L6" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M6" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="N6" s="40" t="s">
+        <v>266</v>
+      </c>
+      <c r="O6" s="48" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="62" t="s">
+        <v>339</v>
+      </c>
+      <c r="B7" s="63" t="s">
         <v>340</v>
       </c>
-      <c r="B6" s="13" t="s">
-        <v>340</v>
-      </c>
-      <c r="C6" s="13" t="s">
+      <c r="C7" s="62" t="s">
         <v>341</v>
       </c>
-      <c r="D6" s="14"/>
-      <c r="E6" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="15">
-        <v>44657.0</v>
-      </c>
-      <c r="L6" s="14"/>
-      <c r="M6" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="N6" s="13" t="s">
+      <c r="E7" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="107" t="s">
         <v>342</v>
       </c>
-      <c r="O6" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P6" s="14"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="14"/>
-      <c r="S6" s="14"/>
-      <c r="T6" s="14"/>
-      <c r="U6" s="14"/>
-      <c r="V6" s="14"/>
-      <c r="W6" s="14"/>
-      <c r="X6" s="14"/>
-      <c r="Y6" s="14"/>
-      <c r="Z6" s="14"/>
-      <c r="AA6" s="14"/>
-      <c r="AB6" s="14"/>
-      <c r="AC6" s="14"/>
-      <c r="AD6" s="14"/>
-      <c r="AE6" s="14"/>
-      <c r="AF6" s="14"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="B7" s="13" t="s">
-        <v>344</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="D7" s="14"/>
-      <c r="E7" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
-      <c r="K7" s="15">
-        <v>44657.0</v>
-      </c>
-      <c r="L7" s="14"/>
-      <c r="M7" s="62" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="O7" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="14"/>
-      <c r="T7" s="14"/>
-      <c r="U7" s="14"/>
-      <c r="V7" s="14"/>
-      <c r="W7" s="14"/>
-      <c r="X7" s="14"/>
-      <c r="Y7" s="14"/>
-      <c r="Z7" s="14"/>
-      <c r="AA7" s="14"/>
-      <c r="AB7" s="14"/>
-      <c r="AC7" s="14"/>
-      <c r="AD7" s="14"/>
-      <c r="AE7" s="14"/>
-      <c r="AF7" s="14"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="25">
+        <v>44139.0</v>
+      </c>
+      <c r="L7" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M7" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="N7" s="27" t="s">
+        <v>101</v>
+      </c>
+      <c r="O7" s="106" t="s">
+        <v>37</v>
+      </c>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="29"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>347</v>
-      </c>
-      <c r="D8" s="14"/>
+        <v>344</v>
+      </c>
       <c r="E8" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K8" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L8" s="14"/>
-      <c r="M8" s="62" t="s">
-        <v>19</v>
+      <c r="L8" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M8" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O8" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="14"/>
-      <c r="T8" s="14"/>
-      <c r="U8" s="14"/>
-      <c r="V8" s="14"/>
-      <c r="W8" s="14"/>
-      <c r="X8" s="14"/>
-      <c r="Y8" s="14"/>
-      <c r="Z8" s="14"/>
-      <c r="AA8" s="14"/>
-      <c r="AB8" s="14"/>
-      <c r="AC8" s="14"/>
-      <c r="AD8" s="14"/>
-      <c r="AE8" s="14"/>
-      <c r="AF8" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>347</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="B9" s="13" t="s">
-        <v>348</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>349</v>
-      </c>
-      <c r="D9" s="14"/>
       <c r="E9" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K9" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L9" s="14"/>
-      <c r="M9" s="62" t="s">
-        <v>19</v>
+      <c r="L9" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M9" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O9" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
-      <c r="U9" s="14"/>
-      <c r="V9" s="14"/>
-      <c r="W9" s="14"/>
-      <c r="X9" s="14"/>
-      <c r="Y9" s="14"/>
-      <c r="Z9" s="14"/>
-      <c r="AA9" s="14"/>
-      <c r="AB9" s="14"/>
-      <c r="AC9" s="14"/>
-      <c r="AD9" s="14"/>
-      <c r="AE9" s="14"/>
-      <c r="AF9" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>349</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="C10" s="13" t="s">
-        <v>352</v>
-      </c>
-      <c r="D10" s="14"/>
       <c r="E10" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="14"/>
-      <c r="I10" s="14"/>
-      <c r="J10" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K10" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L10" s="14"/>
-      <c r="M10" s="62" t="s">
-        <v>19</v>
+      <c r="L10" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M10" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O10" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P10" s="14"/>
-      <c r="Q10" s="14"/>
-      <c r="R10" s="14"/>
-      <c r="S10" s="14"/>
-      <c r="T10" s="14"/>
-      <c r="U10" s="14"/>
-      <c r="V10" s="14"/>
-      <c r="W10" s="14"/>
-      <c r="X10" s="14"/>
-      <c r="Y10" s="14"/>
-      <c r="Z10" s="14"/>
-      <c r="AA10" s="14"/>
-      <c r="AB10" s="14"/>
-      <c r="AC10" s="14"/>
-      <c r="AD10" s="14"/>
-      <c r="AE10" s="14"/>
-      <c r="AF10" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>354</v>
-      </c>
-      <c r="D11" s="14"/>
+        <v>352</v>
+      </c>
       <c r="E11" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K11" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L11" s="14"/>
-      <c r="M11" s="62" t="s">
-        <v>19</v>
+      <c r="L11" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M11" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O11" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P11" s="14"/>
-      <c r="Q11" s="14"/>
-      <c r="R11" s="14"/>
-      <c r="S11" s="14"/>
-      <c r="T11" s="14"/>
-      <c r="U11" s="14"/>
-      <c r="V11" s="14"/>
-      <c r="W11" s="14"/>
-      <c r="X11" s="14"/>
-      <c r="Y11" s="14"/>
-      <c r="Z11" s="14"/>
-      <c r="AA11" s="14"/>
-      <c r="AB11" s="14"/>
-      <c r="AC11" s="14"/>
-      <c r="AD11" s="14"/>
-      <c r="AE11" s="14"/>
-      <c r="AF11" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
+        <v>353</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C12" s="13" t="s">
         <v>355</v>
       </c>
-      <c r="B12" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="C12" s="13" t="s">
-        <v>356</v>
-      </c>
-      <c r="D12" s="14"/>
       <c r="E12" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="14"/>
-      <c r="I12" s="14"/>
-      <c r="J12" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K12" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L12" s="14"/>
-      <c r="M12" s="62" t="s">
-        <v>19</v>
+      <c r="L12" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M12" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P12" s="14"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14"/>
-      <c r="S12" s="14"/>
-      <c r="T12" s="14"/>
-      <c r="U12" s="14"/>
-      <c r="V12" s="14"/>
-      <c r="W12" s="14"/>
-      <c r="X12" s="14"/>
-      <c r="Y12" s="14"/>
-      <c r="Z12" s="14"/>
-      <c r="AA12" s="14"/>
-      <c r="AB12" s="14"/>
-      <c r="AC12" s="14"/>
-      <c r="AD12" s="14"/>
-      <c r="AE12" s="14"/>
-      <c r="AF12" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>356</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>357</v>
       </c>
-      <c r="B13" s="13" t="s">
-        <v>357</v>
-      </c>
-      <c r="C13" s="13" t="s">
-        <v>358</v>
-      </c>
-      <c r="D13" s="14"/>
       <c r="E13" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="14"/>
-      <c r="I13" s="13" t="s">
-        <v>359</v>
-      </c>
-      <c r="J13" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K13" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L13" s="14"/>
-      <c r="M13" s="62" t="s">
-        <v>19</v>
+      <c r="L13" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M13" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O13" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P13" s="14"/>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14"/>
-      <c r="S13" s="14"/>
-      <c r="T13" s="14"/>
-      <c r="U13" s="14"/>
-      <c r="V13" s="14"/>
-      <c r="W13" s="14"/>
-      <c r="X13" s="14"/>
-      <c r="Y13" s="14"/>
-      <c r="Z13" s="14"/>
-      <c r="AA13" s="14"/>
-      <c r="AB13" s="14"/>
-      <c r="AC13" s="14"/>
-      <c r="AD13" s="14"/>
-      <c r="AE13" s="14"/>
-      <c r="AF13" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>361</v>
-      </c>
-      <c r="D14" s="14"/>
+        <v>359</v>
+      </c>
       <c r="E14" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="14"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K14" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L14" s="14"/>
-      <c r="M14" s="62" t="s">
-        <v>19</v>
+      <c r="L14" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M14" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O14" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
-      <c r="X14" s="14"/>
-      <c r="Y14" s="14"/>
-      <c r="Z14" s="14"/>
-      <c r="AA14" s="14"/>
-      <c r="AB14" s="14"/>
-      <c r="AC14" s="14"/>
-      <c r="AD14" s="14"/>
-      <c r="AE14" s="14"/>
-      <c r="AF14" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>361</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="I15" s="13" t="s">
         <v>362</v>
       </c>
-      <c r="B15" s="13" t="s">
-        <v>362</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>363</v>
-      </c>
-      <c r="D15" s="14"/>
-      <c r="E15" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="14"/>
-      <c r="I15" s="14"/>
-      <c r="J15" s="14"/>
       <c r="K15" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L15" s="14"/>
-      <c r="M15" s="62" t="s">
-        <v>19</v>
+      <c r="L15" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M15" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O15" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P15" s="14"/>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
-      <c r="T15" s="14"/>
-      <c r="U15" s="14"/>
-      <c r="V15" s="14"/>
-      <c r="W15" s="14"/>
-      <c r="X15" s="14"/>
-      <c r="Y15" s="14"/>
-      <c r="Z15" s="14"/>
-      <c r="AA15" s="14"/>
-      <c r="AB15" s="14"/>
-      <c r="AC15" s="14"/>
-      <c r="AD15" s="14"/>
-      <c r="AE15" s="14"/>
-      <c r="AF15" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>363</v>
+      </c>
+      <c r="C16" s="13" t="s">
         <v>364</v>
       </c>
-      <c r="B16" s="13" t="s">
-        <v>365</v>
-      </c>
-      <c r="C16" s="13" t="s">
-        <v>366</v>
-      </c>
-      <c r="D16" s="14"/>
       <c r="E16" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="14"/>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K16" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L16" s="14"/>
-      <c r="M16" s="62" t="s">
-        <v>19</v>
+      <c r="L16" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M16" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O16" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P16" s="14"/>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14"/>
-      <c r="S16" s="14"/>
-      <c r="T16" s="14"/>
-      <c r="U16" s="14"/>
-      <c r="V16" s="14"/>
-      <c r="W16" s="14"/>
-      <c r="X16" s="14"/>
-      <c r="Y16" s="14"/>
-      <c r="Z16" s="14"/>
-      <c r="AA16" s="14"/>
-      <c r="AB16" s="14"/>
-      <c r="AC16" s="14"/>
-      <c r="AD16" s="14"/>
-      <c r="AE16" s="14"/>
-      <c r="AF16" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>368</v>
-      </c>
-      <c r="D17" s="14"/>
+        <v>366</v>
+      </c>
       <c r="E17" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K17" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L17" s="14"/>
-      <c r="M17" s="62" t="s">
-        <v>19</v>
+      <c r="L17" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M17" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O17" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P17" s="14"/>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14"/>
-      <c r="S17" s="14"/>
-      <c r="T17" s="14"/>
-      <c r="U17" s="14"/>
-      <c r="V17" s="14"/>
-      <c r="W17" s="14"/>
-      <c r="X17" s="14"/>
-      <c r="Y17" s="14"/>
-      <c r="Z17" s="14"/>
-      <c r="AA17" s="14"/>
-      <c r="AB17" s="14"/>
-      <c r="AC17" s="14"/>
-      <c r="AD17" s="14"/>
-      <c r="AE17" s="14"/>
-      <c r="AF17" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
+        <v>367</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>368</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>369</v>
       </c>
-      <c r="B18" s="13" t="s">
-        <v>369</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>370</v>
-      </c>
-      <c r="D18" s="14"/>
       <c r="E18" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="14"/>
-      <c r="I18" s="14"/>
-      <c r="J18" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K18" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L18" s="14"/>
-      <c r="M18" s="62" t="s">
-        <v>19</v>
+      <c r="L18" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M18" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O18" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P18" s="14"/>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14"/>
-      <c r="S18" s="14"/>
-      <c r="T18" s="14"/>
-      <c r="U18" s="14"/>
-      <c r="V18" s="14"/>
-      <c r="W18" s="14"/>
-      <c r="X18" s="14"/>
-      <c r="Y18" s="14"/>
-      <c r="Z18" s="14"/>
-      <c r="AA18" s="14"/>
-      <c r="AB18" s="14"/>
-      <c r="AC18" s="14"/>
-      <c r="AD18" s="14"/>
-      <c r="AE18" s="14"/>
-      <c r="AF18" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>370</v>
+      </c>
+      <c r="C19" s="13" t="s">
         <v>371</v>
       </c>
-      <c r="B19" s="13" t="s">
-        <v>371</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="D19" s="14"/>
       <c r="E19" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="14"/>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K19" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L19" s="14"/>
-      <c r="M19" s="62" t="s">
-        <v>19</v>
+      <c r="L19" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M19" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O19" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P19" s="14"/>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14"/>
-      <c r="S19" s="14"/>
-      <c r="T19" s="14"/>
-      <c r="U19" s="14"/>
-      <c r="V19" s="14"/>
-      <c r="W19" s="14"/>
-      <c r="X19" s="14"/>
-      <c r="Y19" s="14"/>
-      <c r="Z19" s="14"/>
-      <c r="AA19" s="14"/>
-      <c r="AB19" s="14"/>
-      <c r="AC19" s="14"/>
-      <c r="AD19" s="14"/>
-      <c r="AE19" s="14"/>
-      <c r="AF19" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="B20" s="13" t="s">
+        <v>372</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>373</v>
       </c>
-      <c r="B20" s="13" t="s">
-        <v>373</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>374</v>
-      </c>
-      <c r="D20" s="14"/>
       <c r="E20" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="13" t="s">
-        <v>375</v>
-      </c>
-      <c r="J20" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K20" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L20" s="14"/>
-      <c r="M20" s="62" t="s">
-        <v>19</v>
+      <c r="L20" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M20" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O20" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P20" s="14"/>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14"/>
-      <c r="S20" s="14"/>
-      <c r="T20" s="14"/>
-      <c r="U20" s="14"/>
-      <c r="V20" s="14"/>
-      <c r="W20" s="14"/>
-      <c r="X20" s="14"/>
-      <c r="Y20" s="14"/>
-      <c r="Z20" s="14"/>
-      <c r="AA20" s="14"/>
-      <c r="AB20" s="14"/>
-      <c r="AC20" s="14"/>
-      <c r="AD20" s="14"/>
-      <c r="AE20" s="14"/>
-      <c r="AF20" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>377</v>
-      </c>
-      <c r="D21" s="13" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="14"/>
-      <c r="I21" s="14"/>
-      <c r="J21" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K21" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L21" s="14"/>
-      <c r="M21" s="62" t="s">
-        <v>19</v>
+      <c r="L21" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M21" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O21" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P21" s="14"/>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14"/>
-      <c r="S21" s="14"/>
-      <c r="T21" s="14"/>
-      <c r="U21" s="14"/>
-      <c r="V21" s="14"/>
-      <c r="W21" s="14"/>
-      <c r="X21" s="14"/>
-      <c r="Y21" s="14"/>
-      <c r="Z21" s="14"/>
-      <c r="AA21" s="14"/>
-      <c r="AB21" s="14"/>
-      <c r="AC21" s="14"/>
-      <c r="AD21" s="14"/>
-      <c r="AE21" s="14"/>
-      <c r="AF21" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>380</v>
-      </c>
-      <c r="D22" s="14"/>
+        <v>377</v>
+      </c>
       <c r="E22" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
+        <v>329</v>
+      </c>
+      <c r="I22" s="13" t="s">
+        <v>378</v>
+      </c>
       <c r="K22" s="15">
         <v>44657.0</v>
       </c>
-      <c r="L22" s="14"/>
-      <c r="M22" s="62" t="s">
-        <v>19</v>
+      <c r="L22" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M22" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O22" s="48" t="s">
-        <v>343</v>
-      </c>
-      <c r="P22" s="14"/>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14"/>
-      <c r="S22" s="14"/>
-      <c r="T22" s="14"/>
-      <c r="U22" s="14"/>
-      <c r="V22" s="14"/>
-      <c r="W22" s="14"/>
-      <c r="X22" s="14"/>
-      <c r="Y22" s="14"/>
-      <c r="Z22" s="14"/>
-      <c r="AA22" s="14"/>
-      <c r="AB22" s="14"/>
-      <c r="AC22" s="14"/>
-      <c r="AD22" s="14"/>
-      <c r="AE22" s="14"/>
-      <c r="AF22" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="B23" s="13" t="s">
+        <v>379</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>380</v>
+      </c>
+      <c r="D23" s="13" t="s">
         <v>381</v>
       </c>
-      <c r="B23" s="13" t="s">
-        <v>382</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>383</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>384</v>
-      </c>
       <c r="E23" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K23" s="15">
-        <v>44727.0</v>
-      </c>
-      <c r="L23" s="14"/>
-      <c r="M23" s="13" t="s">
-        <v>19</v>
+        <v>44657.0</v>
+      </c>
+      <c r="L23" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M23" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>266</v>
+        <v>345</v>
       </c>
       <c r="O23" s="48" t="s">
-        <v>385</v>
-      </c>
-      <c r="P23" s="14"/>
-      <c r="Q23" s="14"/>
-      <c r="R23" s="14"/>
-      <c r="S23" s="14"/>
-      <c r="T23" s="14"/>
-      <c r="U23" s="14"/>
-      <c r="V23" s="14"/>
-      <c r="W23" s="14"/>
-      <c r="X23" s="14"/>
-      <c r="Y23" s="14"/>
-      <c r="Z23" s="14"/>
-      <c r="AA23" s="14"/>
-      <c r="AB23" s="14"/>
-      <c r="AC23" s="14"/>
-      <c r="AD23" s="14"/>
-      <c r="AE23" s="14"/>
-      <c r="AF23" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>388</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
-      <c r="I24" s="14"/>
-      <c r="J24" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K24" s="15">
-        <v>44727.0</v>
-      </c>
-      <c r="L24" s="14"/>
-      <c r="M24" s="13" t="s">
-        <v>19</v>
+        <v>44657.0</v>
+      </c>
+      <c r="L24" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M24" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>266</v>
+        <v>345</v>
       </c>
       <c r="O24" s="48" t="s">
-        <v>385</v>
-      </c>
-      <c r="P24" s="14"/>
-      <c r="Q24" s="14"/>
-      <c r="R24" s="14"/>
-      <c r="S24" s="14"/>
-      <c r="T24" s="14"/>
-      <c r="U24" s="14"/>
-      <c r="V24" s="14"/>
-      <c r="W24" s="14"/>
-      <c r="X24" s="14"/>
-      <c r="Y24" s="14"/>
-      <c r="Z24" s="14"/>
-      <c r="AA24" s="14"/>
-      <c r="AB24" s="14"/>
-      <c r="AC24" s="14"/>
-      <c r="AD24" s="14"/>
-      <c r="AE24" s="14"/>
-      <c r="AF24" s="14"/>
+        <v>346</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="14"/>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K25" s="15">
         <v>44727.0</v>
       </c>
-      <c r="L25" s="14"/>
-      <c r="M25" s="13" t="s">
-        <v>19</v>
+      <c r="L25" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M25" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N25" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O25" s="48" t="s">
-        <v>385</v>
-      </c>
-      <c r="P25" s="14"/>
-      <c r="Q25" s="14"/>
-      <c r="R25" s="14"/>
-      <c r="S25" s="14"/>
-      <c r="T25" s="14"/>
-      <c r="U25" s="14"/>
-      <c r="V25" s="14"/>
-      <c r="W25" s="14"/>
-      <c r="X25" s="14"/>
-      <c r="Y25" s="14"/>
-      <c r="Z25" s="14"/>
-      <c r="AA25" s="14"/>
-      <c r="AB25" s="14"/>
-      <c r="AC25" s="14"/>
-      <c r="AD25" s="14"/>
-      <c r="AE25" s="14"/>
-      <c r="AF25" s="14"/>
+        <v>388</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>394</v>
-      </c>
-      <c r="D26" s="14"/>
+        <v>391</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>387</v>
+      </c>
       <c r="E26" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K26" s="15">
-        <v>44776.0</v>
-      </c>
-      <c r="L26" s="14"/>
-      <c r="M26" s="13" t="s">
-        <v>19</v>
+        <v>44727.0</v>
+      </c>
+      <c r="L26" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N26" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O26" s="48" t="s">
-        <v>395</v>
-      </c>
-      <c r="P26" s="14"/>
-      <c r="Q26" s="14"/>
-      <c r="R26" s="14"/>
-      <c r="S26" s="14"/>
-      <c r="T26" s="14"/>
-      <c r="U26" s="14"/>
-      <c r="V26" s="14"/>
-      <c r="W26" s="14"/>
-      <c r="X26" s="14"/>
-      <c r="Y26" s="14"/>
-      <c r="Z26" s="14"/>
-      <c r="AA26" s="14"/>
-      <c r="AB26" s="14"/>
-      <c r="AC26" s="14"/>
-      <c r="AD26" s="14"/>
-      <c r="AE26" s="14"/>
-      <c r="AF26" s="14"/>
+        <v>388</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>398</v>
-      </c>
-      <c r="D27" s="14"/>
+        <v>394</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>387</v>
+      </c>
       <c r="E27" s="27" t="s">
-        <v>331</v>
-      </c>
-      <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="14"/>
-      <c r="I27" s="14"/>
-      <c r="J27" s="14"/>
+        <v>329</v>
+      </c>
       <c r="K27" s="15">
-        <v>44776.0</v>
-      </c>
-      <c r="L27" s="14"/>
-      <c r="M27" s="13" t="s">
-        <v>19</v>
+        <v>44727.0</v>
+      </c>
+      <c r="L27" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>332</v>
       </c>
       <c r="N27" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O27" s="48" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" s="13" t="s">
         <v>395</v>
       </c>
-      <c r="P27" s="14"/>
-      <c r="Q27" s="14"/>
-      <c r="R27" s="14"/>
-      <c r="S27" s="14"/>
-      <c r="T27" s="14"/>
-      <c r="U27" s="14"/>
-      <c r="V27" s="14"/>
-      <c r="W27" s="14"/>
-      <c r="X27" s="14"/>
-      <c r="Y27" s="14"/>
-      <c r="Z27" s="14"/>
-      <c r="AA27" s="14"/>
-      <c r="AB27" s="14"/>
-      <c r="AC27" s="14"/>
-      <c r="AD27" s="14"/>
-      <c r="AE27" s="14"/>
-      <c r="AF27" s="14"/>
+      <c r="B28" s="13" t="s">
+        <v>396</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>397</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="K28" s="15">
+        <v>44776.0</v>
+      </c>
+      <c r="L28" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="N28" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="O28" s="48" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="13" t="s">
+        <v>399</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>400</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>401</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="K29" s="15">
+        <v>44776.0</v>
+      </c>
+      <c r="L29" s="98">
+        <v>45643.0</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="N29" s="13" t="s">
+        <v>266</v>
+      </c>
+      <c r="O29" s="48" t="s">
+        <v>398</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A13:B14">
+  <conditionalFormatting sqref="A15:B16">
     <cfRule type="expression" dxfId="3" priority="1">
-      <formula>$M10="proposed"</formula>
+      <formula>$M12="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A21:B21">
+  <conditionalFormatting sqref="A23:B23">
     <cfRule type="expression" dxfId="3" priority="2">
-      <formula>$M11="proposed"</formula>
+      <formula>$M13="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF39">
+  <conditionalFormatting sqref="A2:AF41">
     <cfRule type="expression" dxfId="3" priority="3">
       <formula>$M2="proposed"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF39">
+  <conditionalFormatting sqref="A2:AF41">
     <cfRule type="expression" dxfId="2" priority="4">
       <formula>$M2="accepted"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2:AF39">
+  <conditionalFormatting sqref="A2:AF41">
     <cfRule type="expression" dxfId="0" priority="5">
       <formula>$M2="changed"</formula>
     </cfRule>
   </conditionalFormatting>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="J2"/>
-    <hyperlink r:id="rId2" ref="O2"/>
-    <hyperlink r:id="rId3" ref="O4"/>
-    <hyperlink r:id="rId4" ref="O6"/>
-    <hyperlink r:id="rId5" ref="O7"/>
-    <hyperlink r:id="rId6" ref="O8"/>
-    <hyperlink r:id="rId7" ref="O9"/>
-    <hyperlink r:id="rId8" ref="O10"/>
-    <hyperlink r:id="rId9" ref="O11"/>
-    <hyperlink r:id="rId10" ref="O12"/>
-    <hyperlink r:id="rId11" ref="O13"/>
-    <hyperlink r:id="rId12" ref="O14"/>
-    <hyperlink r:id="rId13" ref="O15"/>
-    <hyperlink r:id="rId14" ref="O16"/>
-    <hyperlink r:id="rId15" ref="O17"/>
-    <hyperlink r:id="rId16" ref="O18"/>
-    <hyperlink r:id="rId17" ref="O19"/>
-    <hyperlink r:id="rId18" ref="O20"/>
-    <hyperlink r:id="rId19" ref="O21"/>
-    <hyperlink r:id="rId20" ref="O22"/>
-    <hyperlink r:id="rId21" ref="O23"/>
-    <hyperlink r:id="rId22" ref="O24"/>
-    <hyperlink r:id="rId23" ref="O25"/>
-    <hyperlink r:id="rId24" ref="O26"/>
-    <hyperlink r:id="rId25" ref="O27"/>
+    <hyperlink r:id="rId1" ref="J3"/>
+    <hyperlink r:id="rId2" ref="O3"/>
+    <hyperlink r:id="rId3" ref="O6"/>
+    <hyperlink r:id="rId4" ref="O8"/>
+    <hyperlink r:id="rId5" ref="O9"/>
+    <hyperlink r:id="rId6" ref="O10"/>
+    <hyperlink r:id="rId7" ref="O11"/>
+    <hyperlink r:id="rId8" ref="O12"/>
+    <hyperlink r:id="rId9" ref="O13"/>
+    <hyperlink r:id="rId10" ref="O14"/>
+    <hyperlink r:id="rId11" ref="O15"/>
+    <hyperlink r:id="rId12" ref="O16"/>
+    <hyperlink r:id="rId13" ref="O17"/>
+    <hyperlink r:id="rId14" ref="O18"/>
+    <hyperlink r:id="rId15" ref="O19"/>
+    <hyperlink r:id="rId16" ref="O20"/>
+    <hyperlink r:id="rId17" ref="O21"/>
+    <hyperlink r:id="rId18" ref="O22"/>
+    <hyperlink r:id="rId19" ref="O23"/>
+    <hyperlink r:id="rId20" ref="O24"/>
+    <hyperlink r:id="rId21" ref="O25"/>
+    <hyperlink r:id="rId22" ref="O26"/>
+    <hyperlink r:id="rId23" ref="O27"/>
+    <hyperlink r:id="rId24" ref="O28"/>
+    <hyperlink r:id="rId25" ref="O29"/>
   </hyperlinks>
   <drawing r:id="rId26"/>
 </worksheet>
@@ -13930,7 +13580,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="107" t="s">
+      <c r="C1" s="108" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -13951,19 +13601,19 @@
       <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="108" t="s">
+      <c r="J1" s="109" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="109" t="s">
+      <c r="K1" s="110" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="110" t="s">
+      <c r="L1" s="111" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="110" t="s">
+      <c r="M1" s="111" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="111" t="s">
+      <c r="N1" s="112" t="s">
         <v>13</v>
       </c>
       <c r="O1" s="8" t="s">
@@ -13972,32 +13622,32 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>324</v>
-      </c>
-      <c r="B2" s="112" t="s">
-        <v>325</v>
-      </c>
-      <c r="C2" s="113" t="s">
         <v>326</v>
       </c>
-      <c r="D2" s="114" t="s">
+      <c r="B2" s="113" t="s">
+        <v>327</v>
+      </c>
+      <c r="C2" s="114" t="s">
+        <v>328</v>
+      </c>
+      <c r="D2" s="115" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="114" t="s">
+      <c r="E2" s="115" t="s">
         <v>26</v>
       </c>
       <c r="F2" s="33"/>
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
-      <c r="I2" s="114" t="s">
-        <v>327</v>
-      </c>
-      <c r="J2" s="115"/>
-      <c r="K2" s="116"/>
-      <c r="L2" s="116"/>
-      <c r="M2" s="114"/>
-      <c r="N2" s="114"/>
-      <c r="O2" s="117" t="s">
+      <c r="I2" s="115" t="s">
+        <v>330</v>
+      </c>
+      <c r="J2" s="116"/>
+      <c r="K2" s="117"/>
+      <c r="L2" s="117"/>
+      <c r="M2" s="115"/>
+      <c r="N2" s="115"/>
+      <c r="O2" s="118" t="s">
         <v>27</v>
       </c>
       <c r="P2" s="33"/>
@@ -14019,34 +13669,34 @@
       <c r="AF2" s="33"/>
     </row>
     <row r="3">
-      <c r="A3" s="118" t="s">
-        <v>329</v>
-      </c>
-      <c r="B3" s="119" t="s">
-        <v>329</v>
-      </c>
-      <c r="C3" s="118" t="s">
-        <v>330</v>
+      <c r="A3" s="119" t="s">
+        <v>333</v>
+      </c>
+      <c r="B3" s="120" t="s">
+        <v>333</v>
+      </c>
+      <c r="C3" s="119" t="s">
+        <v>334</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>331</v>
+        <v>402</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
-      <c r="I3" s="120" t="s">
-        <v>332</v>
+      <c r="I3" s="121" t="s">
+        <v>335</v>
       </c>
       <c r="J3" s="36"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="122"/>
+      <c r="K3" s="122"/>
+      <c r="L3" s="123"/>
       <c r="M3" s="10"/>
-      <c r="N3" s="118"/>
-      <c r="O3" s="120" t="s">
+      <c r="N3" s="119"/>
+      <c r="O3" s="121" t="s">
         <v>142</v>
       </c>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="123"/>
+      <c r="P3" s="124"/>
+      <c r="Q3" s="124"/>
       <c r="R3" s="36"/>
       <c r="S3" s="36"/>
       <c r="T3" s="36"/>
@@ -14075,13 +13725,13 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="10"/>
@@ -14092,7 +13742,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -14121,13 +13771,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="10"/>
@@ -14138,7 +13788,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -14167,13 +13817,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="10"/>
@@ -14184,7 +13834,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -14213,13 +13863,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="10"/>
@@ -14230,7 +13880,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
@@ -14259,13 +13909,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="10"/>
@@ -14276,7 +13926,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -14305,13 +13955,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="10"/>
@@ -14322,7 +13972,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
@@ -14351,13 +14001,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="10"/>
@@ -14368,7 +14018,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -14397,13 +14047,13 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="10"/>
@@ -14414,7 +14064,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="13" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
@@ -14443,13 +14093,13 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="B14" s="124" t="s">
-        <v>425</v>
+        <v>428</v>
+      </c>
+      <c r="B14" s="125" t="s">
+        <v>429</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="10"/>
@@ -14458,19 +14108,19 @@
       </c>
       <c r="G14" s="36"/>
       <c r="H14" s="36"/>
-      <c r="I14" s="125"/>
+      <c r="I14" s="126"/>
       <c r="J14" s="13" t="s">
-        <v>402</v>
-      </c>
-      <c r="K14" s="121"/>
-      <c r="L14" s="126"/>
+        <v>406</v>
+      </c>
+      <c r="K14" s="122"/>
+      <c r="L14" s="127"/>
       <c r="M14" s="10" t="s">
         <v>41</v>
       </c>
       <c r="N14" s="10"/>
-      <c r="O14" s="120"/>
-      <c r="P14" s="123"/>
-      <c r="Q14" s="123"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="124"/>
+      <c r="Q14" s="124"/>
       <c r="R14" s="36"/>
       <c r="S14" s="36"/>
       <c r="T14" s="36"/>
@@ -14490,42 +14140,42 @@
     <row r="15">
       <c r="E15" s="10"/>
       <c r="K15" s="15"/>
-      <c r="M15" s="118"/>
+      <c r="M15" s="119"/>
     </row>
     <row r="16">
       <c r="E16" s="10"/>
       <c r="K16" s="15"/>
-      <c r="M16" s="118"/>
+      <c r="M16" s="119"/>
     </row>
     <row r="17">
       <c r="E17" s="10"/>
       <c r="K17" s="15"/>
-      <c r="M17" s="118"/>
+      <c r="M17" s="119"/>
     </row>
     <row r="18">
       <c r="E18" s="10"/>
       <c r="K18" s="15"/>
-      <c r="M18" s="118"/>
+      <c r="M18" s="119"/>
     </row>
     <row r="19">
       <c r="E19" s="10"/>
       <c r="K19" s="15"/>
-      <c r="M19" s="118"/>
+      <c r="M19" s="119"/>
     </row>
     <row r="20">
       <c r="E20" s="10"/>
       <c r="K20" s="15"/>
-      <c r="M20" s="118"/>
+      <c r="M20" s="119"/>
     </row>
     <row r="21">
       <c r="E21" s="10"/>
       <c r="K21" s="15"/>
-      <c r="M21" s="118"/>
+      <c r="M21" s="119"/>
     </row>
     <row r="22">
       <c r="E22" s="10"/>
       <c r="K22" s="15"/>
-      <c r="M22" s="118"/>
+      <c r="M22" s="119"/>
     </row>
     <row r="23">
       <c r="E23" s="10"/>

</xml_diff>

<commit_message>
fix dpv:HumanSubject - add definition and label
- added definition and label for `dpv:HumanSubject`
- no existing source found for 'Human Subject'
- thanks to @TallTed - see #205
  https://github.com/w3c/dpv/issues/205#issuecomment-2560239487
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1048" uniqueCount="445">
   <si>
     <t>Term</t>
   </si>
@@ -1086,6 +1086,12 @@
   </si>
   <si>
     <t>HumanSubject</t>
+  </si>
+  <si>
+    <t>Human Subject</t>
+  </si>
+  <si>
+    <t>The individual (or category of individuals) that is the subject within some context such as personal data (dpv:DataSubject) or technology (tech:Subject)</t>
   </si>
   <si>
     <t>Harshvardhan J. Pandit, Delaram Golpayegani</t>
@@ -5719,13 +5725,13 @@
     </row>
     <row r="2">
       <c r="A2" s="82" t="s">
-        <v>431</v>
+        <v>433</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>433</v>
+        <v>435</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>17</v>
@@ -5735,7 +5741,7 @@
         <v>dpv:DataSubject</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>434</v>
+        <v>436</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -5748,7 +5754,7 @@
         <v>45643.0</v>
       </c>
       <c r="M2" s="90" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N2" s="82" t="s">
         <v>201</v>
@@ -5772,13 +5778,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>435</v>
+        <v>437</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>436</v>
+        <v>438</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>25</v>
@@ -5801,10 +5807,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>438</v>
+        <v>440</v>
       </c>
       <c r="O3" s="48" t="s">
-        <v>439</v>
+        <v>441</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -5822,19 +5828,19 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>440</v>
+        <v>442</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="C4" s="90" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F4" s="13" t="s">
         <v>77</v>
@@ -12604,8 +12610,12 @@
       <c r="A2" s="27" t="s">
         <v>324</v>
       </c>
-      <c r="B2" s="63"/>
-      <c r="C2" s="62"/>
+      <c r="B2" s="90" t="s">
+        <v>325</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>326</v>
+      </c>
       <c r="D2" s="96" t="s">
         <v>34</v>
       </c>
@@ -12617,15 +12627,15 @@
       <c r="H2" s="23"/>
       <c r="I2" s="97"/>
       <c r="J2" s="23"/>
-      <c r="K2" s="25"/>
-      <c r="L2" s="98">
+      <c r="K2" s="98">
         <v>45643.0</v>
       </c>
+      <c r="L2" s="14"/>
       <c r="M2" s="27" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="O2" s="97"/>
       <c r="P2" s="23"/>
@@ -12648,16 +12658,16 @@
     </row>
     <row r="3">
       <c r="A3" s="99" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B3" s="100" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C3" s="101" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -12666,10 +12676,10 @@
       <c r="G3" s="102"/>
       <c r="H3" s="102"/>
       <c r="I3" s="96" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="J3" s="103" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="K3" s="104">
         <v>43560.0</v>
@@ -12678,7 +12688,7 @@
         <v>45643.0</v>
       </c>
       <c r="M3" s="99" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N3" s="96" t="s">
         <v>130</v>
@@ -12709,22 +12719,22 @@
     </row>
     <row r="5">
       <c r="A5" s="62" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="106" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="25">
@@ -12734,7 +12744,7 @@
         <v>45643.0</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N5" s="62" t="s">
         <v>20</v>
@@ -12762,16 +12772,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K6" s="15">
         <v>44650.0</v>
@@ -12780,33 +12790,33 @@
         <v>45643.0</v>
       </c>
       <c r="M6" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N6" s="40" t="s">
         <v>266</v>
       </c>
       <c r="O6" s="48" t="s">
-        <v>338</v>
+        <v>340</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="62" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="B7" s="63" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="C7" s="62" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="E7" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
       <c r="I7" s="107" t="s">
-        <v>342</v>
+        <v>344</v>
       </c>
       <c r="J7" s="62"/>
       <c r="K7" s="25">
@@ -12816,7 +12826,7 @@
         <v>45643.0</v>
       </c>
       <c r="M7" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N7" s="27" t="s">
         <v>101</v>
@@ -12844,16 +12854,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K8" s="15">
         <v>44657.0</v>
@@ -12862,27 +12872,27 @@
         <v>45643.0</v>
       </c>
       <c r="M8" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O8" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K9" s="15">
         <v>44657.0</v>
@@ -12891,27 +12901,27 @@
         <v>45643.0</v>
       </c>
       <c r="M9" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O9" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K10" s="15">
         <v>44657.0</v>
@@ -12920,27 +12930,27 @@
         <v>45643.0</v>
       </c>
       <c r="M10" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O10" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K11" s="15">
         <v>44657.0</v>
@@ -12949,27 +12959,27 @@
         <v>45643.0</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O11" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K12" s="15">
         <v>44657.0</v>
@@ -12978,27 +12988,27 @@
         <v>45643.0</v>
       </c>
       <c r="M12" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K13" s="15">
         <v>44657.0</v>
@@ -13007,27 +13017,27 @@
         <v>45643.0</v>
       </c>
       <c r="M13" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O13" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K14" s="15">
         <v>44657.0</v>
@@ -13036,30 +13046,30 @@
         <v>45643.0</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O14" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I15" s="13" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="K15" s="15">
         <v>44657.0</v>
@@ -13068,27 +13078,27 @@
         <v>45643.0</v>
       </c>
       <c r="M15" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O15" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K16" s="15">
         <v>44657.0</v>
@@ -13097,27 +13107,27 @@
         <v>45643.0</v>
       </c>
       <c r="M16" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O16" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K17" s="15">
         <v>44657.0</v>
@@ -13126,27 +13136,27 @@
         <v>45643.0</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O17" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K18" s="15">
         <v>44657.0</v>
@@ -13155,27 +13165,27 @@
         <v>45643.0</v>
       </c>
       <c r="M18" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O18" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K19" s="15">
         <v>44657.0</v>
@@ -13184,27 +13194,27 @@
         <v>45643.0</v>
       </c>
       <c r="M19" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O19" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K20" s="15">
         <v>44657.0</v>
@@ -13213,27 +13223,27 @@
         <v>45643.0</v>
       </c>
       <c r="M20" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O20" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K21" s="15">
         <v>44657.0</v>
@@ -13242,30 +13252,30 @@
         <v>45643.0</v>
       </c>
       <c r="M21" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O21" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="I22" s="13" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="K22" s="15">
         <v>44657.0</v>
@@ -13274,30 +13284,30 @@
         <v>45643.0</v>
       </c>
       <c r="M22" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O22" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="D23" s="13" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K23" s="15">
         <v>44657.0</v>
@@ -13306,27 +13316,27 @@
         <v>45643.0</v>
       </c>
       <c r="M23" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O23" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K24" s="15">
         <v>44657.0</v>
@@ -13335,30 +13345,30 @@
         <v>45643.0</v>
       </c>
       <c r="M24" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="O24" s="48" t="s">
-        <v>346</v>
+        <v>348</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K25" s="15">
         <v>44727.0</v>
@@ -13367,30 +13377,30 @@
         <v>45643.0</v>
       </c>
       <c r="M25" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N25" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O25" s="48" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
+        <v>391</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>392</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>393</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>389</v>
       </c>
-      <c r="B26" s="13" t="s">
-        <v>390</v>
-      </c>
-      <c r="C26" s="13" t="s">
-        <v>391</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>387</v>
-      </c>
       <c r="E26" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K26" s="15">
         <v>44727.0</v>
@@ -13399,30 +13409,30 @@
         <v>45643.0</v>
       </c>
       <c r="M26" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N26" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O26" s="48" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>394</v>
+        <v>396</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K27" s="15">
         <v>44727.0</v>
@@ -13431,27 +13441,27 @@
         <v>45643.0</v>
       </c>
       <c r="M27" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N27" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O27" s="48" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="13" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K28" s="15">
         <v>44776.0</v>
@@ -13460,27 +13470,27 @@
         <v>45643.0</v>
       </c>
       <c r="M28" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N28" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O28" s="48" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="K29" s="15">
         <v>44776.0</v>
@@ -13489,13 +13499,13 @@
         <v>45643.0</v>
       </c>
       <c r="M29" s="27" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="N29" s="13" t="s">
         <v>266</v>
       </c>
       <c r="O29" s="48" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
     </row>
   </sheetData>
@@ -13622,13 +13632,13 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="B2" s="113" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="C2" s="114" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="D2" s="115" t="s">
         <v>34</v>
@@ -13640,7 +13650,7 @@
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
       <c r="I2" s="115" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="J2" s="116"/>
       <c r="K2" s="117"/>
@@ -13670,22 +13680,22 @@
     </row>
     <row r="3">
       <c r="A3" s="119" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="B3" s="120" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C3" s="119" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
       <c r="I3" s="121" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="J3" s="36"/>
       <c r="K3" s="122"/>
@@ -13725,13 +13735,13 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="10"/>
@@ -13742,7 +13752,7 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
@@ -13771,13 +13781,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>407</v>
+        <v>409</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>408</v>
+        <v>410</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>409</v>
+        <v>411</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="10"/>
@@ -13788,7 +13798,7 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
@@ -13817,13 +13827,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>411</v>
+        <v>413</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>412</v>
+        <v>414</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="10"/>
@@ -13834,7 +13844,7 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
@@ -13863,13 +13873,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>413</v>
+        <v>415</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>414</v>
+        <v>416</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="10"/>
@@ -13880,7 +13890,7 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
@@ -13909,13 +13919,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>416</v>
+        <v>418</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>417</v>
+        <v>419</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="10"/>
@@ -13926,7 +13936,7 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
@@ -13955,13 +13965,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>419</v>
+        <v>421</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>420</v>
+        <v>422</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>421</v>
+        <v>423</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="10"/>
@@ -13972,7 +13982,7 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
@@ -14001,13 +14011,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>424</v>
+        <v>426</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="10"/>
@@ -14018,7 +14028,7 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
@@ -14047,13 +14057,13 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>425</v>
+        <v>427</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>426</v>
+        <v>428</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>427</v>
+        <v>429</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="10"/>
@@ -14064,7 +14074,7 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
@@ -14093,13 +14103,13 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="B14" s="125" t="s">
-        <v>429</v>
+        <v>431</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>430</v>
+        <v>432</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="10"/>
@@ -14110,7 +14120,7 @@
       <c r="H14" s="36"/>
       <c r="I14" s="126"/>
       <c r="J14" s="13" t="s">
-        <v>406</v>
+        <v>408</v>
       </c>
       <c r="K14" s="122"/>
       <c r="L14" s="127"/>

</xml_diff>

<commit_message>
fixes #407 typo in DPV entity properties
- persona -> personal (DPV, module entity)
- also includes fixes from a6064a09cc6418aa95d3ae47254ad0ab569dbcaa re.
  DPV EntityControl to EntityInvolvement (DPV)
- also includes updates to HTML structure (all)

Co-authored-by: Delaram Golpayegani <sgolpays@tcd.ie>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -717,7 +717,7 @@
     <t>has recipient data controller</t>
   </si>
   <si>
-    <t>Indicates inclusion or applicability of a Data Controller as a Recipient of persona data</t>
+    <t>Indicates inclusion or applicability of a Data Controller as a Recipient of personal data</t>
   </si>
   <si>
     <t>hasRecipientThirdParty</t>
@@ -726,7 +726,7 @@
     <t>has recipient third party</t>
   </si>
   <si>
-    <t>Indicates inclusion or applicability of a Third Party as a Recipient of persona data</t>
+    <t>Indicates inclusion or applicability of a Third Party as a Recipient of personal data</t>
   </si>
   <si>
     <t>dpv:ThirdParty</t>

</xml_diff>

<commit_message>
Adds `DataHolder`,`DataUser` to SECTOR-HEALTH
- see #416
- concepts are added for supporting implementation of EU-EHDS and
  DE-GDNG extensions
- concepts are NOT extended in these extensions currently, this should
  be done in a separate commit after ensuring the definitions align

Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -3,16 +3,17 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
   <sheets>
-    <sheet state="visible" name="Entities" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Entities_properties" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Entities_Authority" sheetId="3" r:id="rId6"/>
-    <sheet state="visible" name="Entities_Authority_properties" sheetId="4" r:id="rId7"/>
-    <sheet state="visible" name="Entities_LegalRole" sheetId="5" r:id="rId8"/>
-    <sheet state="visible" name="Entities_LegalRole_properties" sheetId="6" r:id="rId9"/>
-    <sheet state="visible" name="Entities_Organisation" sheetId="7" r:id="rId10"/>
-    <sheet state="visible" name="Entities_DataSubject" sheetId="8" r:id="rId11"/>
-    <sheet state="visible" name="Entities_DataSubjectMinor" sheetId="9" r:id="rId12"/>
-    <sheet state="visible" name="Entities_DataSubject_properties" sheetId="10" r:id="rId13"/>
+    <sheet state="visible" name="Entities" sheetId="1" r:id="rId5"/>
+    <sheet state="visible" name="Entities_properties" sheetId="2" r:id="rId6"/>
+    <sheet state="visible" name="Entities_Authority" sheetId="3" r:id="rId7"/>
+    <sheet state="visible" name="Entities_Authority_properties" sheetId="4" r:id="rId8"/>
+    <sheet state="visible" name="Entities_LegalRole" sheetId="5" r:id="rId9"/>
+    <sheet state="visible" name="Entities_LegalRole_properties" sheetId="6" r:id="rId10"/>
+    <sheet state="visible" name="Entities_Organisation" sheetId="7" r:id="rId11"/>
+    <sheet state="visible" name="Entities_DataSubject" sheetId="8" r:id="rId12"/>
+    <sheet state="visible" name="Entities_DataSubjectMinor" sheetId="9" r:id="rId13"/>
+    <sheet state="visible" name="Entities_DataSubject_properties" sheetId="10" r:id="rId14"/>
+    <sheet state="visible" name="Entities_Healthcare" sheetId="11" r:id="rId15"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="468">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="477">
   <si>
     <t>Term</t>
   </si>
@@ -1516,6 +1517,33 @@
   <si>
     <t>Indicates association with Human Subject</t>
   </si>
+  <si>
+    <t>DataUser</t>
+  </si>
+  <si>
+    <t>Data Holder</t>
+  </si>
+  <si>
+    <t>Natural or legal person with access to health data (draft definition)</t>
+  </si>
+  <si>
+    <t>to extend in GDNG and EHDS extensions</t>
+  </si>
+  <si>
+    <t>none, but based on GDNG's definition</t>
+  </si>
+  <si>
+    <t>Julian Flake</t>
+  </si>
+  <si>
+    <t>DataHolder</t>
+  </si>
+  <si>
+    <t>Data User</t>
+  </si>
+  <si>
+    <t>Natural or legal person requested or obtained access to health data (draft definition)</t>
+  </si>
 </sst>
 </file>
 
@@ -1524,7 +1552,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="37">
+  <fonts count="39">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1705,6 +1733,16 @@
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1802,7 +1840,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="134">
+  <cellXfs count="138">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2199,6 +2237,18 @@
     <xf borderId="0" fillId="3" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="37" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="3" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -2310,6 +2360,10 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
+<file path=xl/drawings/drawing11.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
@@ -2340,6 +2394,10 @@
 
 <file path=xl/drawings/drawing9.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<x18tc:personList xmlns:x18tc="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5977,6 +6035,480 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1.0" ySplit="1.0" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="B1" sqref="B1" pane="topRight"/>
+      <selection activeCell="A2" sqref="A2" pane="bottomLeft"/>
+      <selection activeCell="B2" sqref="B2" pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="2" width="24.38"/>
+    <col customWidth="1" min="3" max="3" width="34.25"/>
+    <col customWidth="1" min="5" max="7" width="15.38"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="28.5" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="96" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="38" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="B2" s="91" t="s">
+        <v>469</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="D2" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="108" t="s">
+        <v>471</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>472</v>
+      </c>
+      <c r="K2" s="99">
+        <v>46055.0</v>
+      </c>
+      <c r="L2" s="14"/>
+      <c r="M2" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="N2" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="O2" s="98"/>
+      <c r="P2" s="23"/>
+      <c r="Q2" s="23"/>
+      <c r="R2" s="23"/>
+      <c r="S2" s="23"/>
+      <c r="T2" s="23"/>
+      <c r="U2" s="23"/>
+      <c r="V2" s="23"/>
+      <c r="W2" s="23"/>
+      <c r="X2" s="23"/>
+      <c r="Y2" s="23"/>
+      <c r="Z2" s="23"/>
+      <c r="AA2" s="23"/>
+      <c r="AB2" s="23"/>
+      <c r="AC2" s="23"/>
+      <c r="AD2" s="23"/>
+      <c r="AE2" s="23"/>
+      <c r="AF2" s="23"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="100" t="s">
+        <v>474</v>
+      </c>
+      <c r="B3" s="134" t="s">
+        <v>475</v>
+      </c>
+      <c r="C3" s="135" t="s">
+        <v>476</v>
+      </c>
+      <c r="D3" s="100" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="100" t="s">
+        <v>26</v>
+      </c>
+      <c r="F3" s="103"/>
+      <c r="G3" s="103"/>
+      <c r="H3" s="103"/>
+      <c r="I3" s="100" t="s">
+        <v>471</v>
+      </c>
+      <c r="J3" s="136" t="s">
+        <v>472</v>
+      </c>
+      <c r="K3" s="99">
+        <v>46055.0</v>
+      </c>
+      <c r="L3" s="99"/>
+      <c r="M3" s="100" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" s="100" t="s">
+        <v>473</v>
+      </c>
+      <c r="O3" s="137"/>
+      <c r="P3" s="103"/>
+      <c r="Q3" s="103"/>
+      <c r="R3" s="103"/>
+      <c r="S3" s="103"/>
+      <c r="T3" s="103"/>
+      <c r="U3" s="103"/>
+      <c r="V3" s="103"/>
+      <c r="W3" s="103"/>
+      <c r="X3" s="103"/>
+      <c r="Y3" s="103"/>
+      <c r="Z3" s="103"/>
+      <c r="AA3" s="103"/>
+      <c r="AB3" s="103"/>
+      <c r="AC3" s="103"/>
+      <c r="AD3" s="103"/>
+      <c r="AE3" s="103"/>
+      <c r="AF3" s="103"/>
+    </row>
+    <row r="4">
+      <c r="L4" s="99"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="62"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="62"/>
+      <c r="E5" s="27"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="23"/>
+      <c r="I5" s="107"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="99"/>
+      <c r="M5" s="27"/>
+      <c r="N5" s="62"/>
+      <c r="O5" s="107"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="23"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="23"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="23"/>
+      <c r="AC5" s="23"/>
+      <c r="AD5" s="23"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+    </row>
+    <row r="6">
+      <c r="E6" s="27"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="27"/>
+      <c r="N6" s="40"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="27"/>
+      <c r="B7" s="91"/>
+      <c r="C7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="108"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="109"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="27"/>
+      <c r="N7" s="27"/>
+      <c r="O7" s="98"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
+      <c r="S7" s="23"/>
+      <c r="T7" s="23"/>
+      <c r="U7" s="23"/>
+      <c r="V7" s="23"/>
+      <c r="W7" s="23"/>
+      <c r="X7" s="23"/>
+      <c r="Y7" s="23"/>
+      <c r="Z7" s="23"/>
+      <c r="AA7" s="23"/>
+      <c r="AB7" s="23"/>
+      <c r="AC7" s="23"/>
+      <c r="AD7" s="23"/>
+      <c r="AE7" s="23"/>
+      <c r="AF7" s="23"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="62"/>
+      <c r="B8" s="63"/>
+      <c r="C8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="23"/>
+      <c r="G8" s="23"/>
+      <c r="H8" s="23"/>
+      <c r="I8" s="110"/>
+      <c r="J8" s="62"/>
+      <c r="K8" s="25"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="27"/>
+      <c r="N8" s="27"/>
+      <c r="O8" s="107"/>
+      <c r="P8" s="29"/>
+      <c r="Q8" s="29"/>
+      <c r="R8" s="23"/>
+      <c r="S8" s="23"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="23"/>
+      <c r="V8" s="23"/>
+      <c r="W8" s="23"/>
+      <c r="X8" s="23"/>
+      <c r="Y8" s="23"/>
+      <c r="Z8" s="23"/>
+      <c r="AA8" s="23"/>
+      <c r="AB8" s="23"/>
+      <c r="AC8" s="23"/>
+      <c r="AD8" s="23"/>
+      <c r="AE8" s="23"/>
+      <c r="AF8" s="23"/>
+    </row>
+    <row r="9">
+      <c r="E9" s="27"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="99"/>
+      <c r="M9" s="27"/>
+    </row>
+    <row r="10">
+      <c r="E10" s="27"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="99"/>
+      <c r="M10" s="27"/>
+    </row>
+    <row r="11">
+      <c r="E11" s="27"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="99"/>
+      <c r="M11" s="27"/>
+    </row>
+    <row r="12">
+      <c r="E12" s="27"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="99"/>
+      <c r="M12" s="27"/>
+    </row>
+    <row r="13">
+      <c r="E13" s="27"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="99"/>
+      <c r="M13" s="27"/>
+    </row>
+    <row r="14">
+      <c r="E14" s="27"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="99"/>
+      <c r="M14" s="27"/>
+    </row>
+    <row r="15">
+      <c r="E15" s="27"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="99"/>
+      <c r="M15" s="27"/>
+    </row>
+    <row r="16">
+      <c r="E16" s="27"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="99"/>
+      <c r="M16" s="27"/>
+    </row>
+    <row r="17">
+      <c r="E17" s="27"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="99"/>
+      <c r="M17" s="27"/>
+    </row>
+    <row r="18">
+      <c r="E18" s="27"/>
+      <c r="K18" s="15"/>
+      <c r="L18" s="99"/>
+      <c r="M18" s="27"/>
+    </row>
+    <row r="19">
+      <c r="E19" s="27"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="99"/>
+      <c r="M19" s="27"/>
+    </row>
+    <row r="20">
+      <c r="E20" s="27"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="99"/>
+      <c r="M20" s="27"/>
+    </row>
+    <row r="21">
+      <c r="E21" s="27"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="99"/>
+      <c r="M21" s="27"/>
+    </row>
+    <row r="22">
+      <c r="E22" s="27"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="99"/>
+      <c r="M22" s="27"/>
+    </row>
+    <row r="23">
+      <c r="E23" s="27"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="99"/>
+      <c r="M23" s="27"/>
+    </row>
+    <row r="24">
+      <c r="E24" s="27"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="27"/>
+    </row>
+    <row r="25">
+      <c r="E25" s="27"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="99"/>
+      <c r="M25" s="27"/>
+    </row>
+    <row r="26">
+      <c r="E26" s="27"/>
+      <c r="K26" s="111"/>
+      <c r="L26" s="112"/>
+      <c r="M26" s="101"/>
+      <c r="N26" s="101"/>
+    </row>
+    <row r="27">
+      <c r="E27" s="27"/>
+      <c r="K27" s="15"/>
+      <c r="L27" s="99"/>
+      <c r="M27" s="27"/>
+    </row>
+    <row r="28">
+      <c r="E28" s="27"/>
+      <c r="K28" s="15"/>
+      <c r="L28" s="99"/>
+      <c r="M28" s="27"/>
+    </row>
+    <row r="29">
+      <c r="E29" s="27"/>
+      <c r="K29" s="111"/>
+      <c r="L29" s="112"/>
+      <c r="M29" s="101"/>
+      <c r="N29" s="101"/>
+    </row>
+    <row r="30">
+      <c r="E30" s="27"/>
+      <c r="K30" s="15"/>
+      <c r="L30" s="99"/>
+      <c r="M30" s="27"/>
+    </row>
+    <row r="31">
+      <c r="E31" s="27"/>
+      <c r="K31" s="111"/>
+      <c r="L31" s="112"/>
+      <c r="M31" s="101"/>
+      <c r="N31" s="101"/>
+    </row>
+    <row r="32">
+      <c r="E32" s="27"/>
+      <c r="K32" s="15"/>
+      <c r="L32" s="99"/>
+      <c r="M32" s="27"/>
+    </row>
+    <row r="33">
+      <c r="E33" s="27"/>
+      <c r="K33" s="111"/>
+      <c r="L33" s="112"/>
+      <c r="M33" s="101"/>
+      <c r="N33" s="101"/>
+    </row>
+    <row r="34">
+      <c r="E34" s="27"/>
+      <c r="K34" s="15"/>
+      <c r="L34" s="99"/>
+      <c r="M34" s="27"/>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A16:B17">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>$M13="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A24:B24">
+    <cfRule type="expression" dxfId="3" priority="2">
+      <formula>$M14="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AF46">
+    <cfRule type="expression" dxfId="3" priority="3">
+      <formula>$M2="proposed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AF46">
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>$M2="accepted"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:AF46">
+    <cfRule type="expression" dxfId="0" priority="5">
+      <formula>$M2="changed"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>

</xml_diff>

<commit_message>
Add Agent, development concepts to DPV, TECH, AI
- #197 Agent and Legal Agent -- can be closed as completed, new issue
  should be opened for AgenticAI
- Adds `Agent`, `LegalAgent` to DPV
- Adds `SoftwareAgent`, `UserAgent` to TECH
- Adds `AIAgent` to AI (with new section in HTML)
- #294 Development phase -- for review by Delaram
- Adds `ModelTraining` (modified) and `ModelFineTuning` to AI
- Adds `DataOperation` with collection, preparation phases to AI (with
  new section in HTML)

Co-authored-by: Arthit Suriyawongkul <arthit@gmail.com>
Co-authored-by: Delaram Golpayegani <sgolpays@tcd.ie>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1125" uniqueCount="477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="486">
   <si>
     <t>Term</t>
   </si>
@@ -128,6 +128,9 @@
     <t>dpv:LegalEntity</t>
   </si>
   <si>
+    <t>A representative may not be a 'legal agent' if it is authorised to only represent the entity and not to take actions on its behalf</t>
+  </si>
+  <si>
     <t>(GDPR Art.27,https://eur-lex.europa.eu/eli/reg/2016/679/art_27/oj)</t>
   </si>
   <si>
@@ -183,6 +186,30 @@
   </si>
   <si>
     <t>A legal entity that has one or more subsidiary entities operating under it</t>
+  </si>
+  <si>
+    <t>Agent</t>
+  </si>
+  <si>
+    <t>An Agent is a dpv:Entity that is (a) acting on behalf of another Entity; and (b) is authorised to do so by that Entity</t>
+  </si>
+  <si>
+    <t>the Entity the Agent is acting on behalf of can be a human or non-human and a legal or non-legal entity. For specific distinction, see dpv:LegalAgent and tech:MachineAgent. The form and validity of authorisation through which the Agent is empowered to represent and act on behalf of the Entity is not defined or covered in this concept</t>
+  </si>
+  <si>
+    <t>LegalAgent</t>
+  </si>
+  <si>
+    <t>Legal Agent</t>
+  </si>
+  <si>
+    <t>A Legal Agent is a Legal Entity that is authorised to act on behalf of another entity</t>
+  </si>
+  <si>
+    <t>dpv:Agent,dpv:LegalEntity</t>
+  </si>
+  <si>
+    <t>Legal agents may be human or non-human (e.g. an organisation), but they must be 'legal persons' i.e. recognised by law as such. The agency and the mechanisms through which it is given, acquired, or expressed is governed by relevant jurisdictional frameworks e.g. power of attorney</t>
   </si>
   <si>
     <t>domain</t>
@@ -2790,9 +2817,11 @@
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
+      <c r="I5" s="22" t="s">
+        <v>35</v>
+      </c>
       <c r="J5" s="24" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K5" s="25">
         <v>44139.0</v>
@@ -2802,10 +2831,10 @@
         <v>19</v>
       </c>
       <c r="N5" s="27" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="O5" s="28" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -2826,13 +2855,13 @@
     </row>
     <row r="6">
       <c r="A6" s="30" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="30" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>17</v>
@@ -2848,7 +2877,7 @@
       <c r="K6" s="33"/>
       <c r="L6" s="33"/>
       <c r="M6" s="32" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N6" s="33"/>
       <c r="O6" s="33"/>
@@ -2871,13 +2900,13 @@
     </row>
     <row r="7">
       <c r="A7" s="34" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B7" s="30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D7" s="34" t="s">
         <v>17</v>
@@ -2898,7 +2927,7 @@
         <v>19</v>
       </c>
       <c r="N7" s="32" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="O7" s="33"/>
       <c r="P7" s="33"/>
@@ -2920,16 +2949,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>26</v>
@@ -2947,7 +2976,7 @@
         <v>19</v>
       </c>
       <c r="N8" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O8" s="14"/>
       <c r="P8" s="14"/>
@@ -2955,16 +2984,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>26</v>
@@ -2982,17 +3011,85 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
       <c r="Q9" s="14"/>
     </row>
     <row r="10">
-      <c r="B10" s="36"/>
+      <c r="A10" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="J10" s="14"/>
+      <c r="K10" s="15">
+        <v>45958.0</v>
+      </c>
+      <c r="L10" s="14"/>
+      <c r="M10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O10" s="14"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="14"/>
     </row>
     <row r="11">
-      <c r="B11" s="36"/>
+      <c r="A11" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="14"/>
+      <c r="K11" s="15">
+        <v>45958.0</v>
+      </c>
+      <c r="L11" s="14"/>
+      <c r="M11" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="O11" s="14"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="14"/>
     </row>
     <row r="12">
       <c r="B12" s="36"/>
@@ -5829,13 +5926,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -5850,7 +5947,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -5867,13 +5964,13 @@
     </row>
     <row r="2">
       <c r="A2" s="82" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="C2" s="82" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>17</v>
@@ -5883,7 +5980,7 @@
         <v>dpv:DataSubject</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -5896,10 +5993,10 @@
         <v>45643.0</v>
       </c>
       <c r="M2" s="91" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N2" s="82" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="O2" s="85" t="s">
         <v>27</v>
@@ -5920,13 +6017,13 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
       <c r="D3" s="13" t="s">
         <v>25</v>
@@ -5935,7 +6032,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G3" s="14"/>
       <c r="H3" s="14"/>
@@ -5949,10 +6046,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="O3" s="48" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -5970,22 +6067,22 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
       <c r="C4" s="91" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
       <c r="D4" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
@@ -6104,13 +6201,13 @@
     </row>
     <row r="2">
       <c r="A2" s="27" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
       <c r="D2" s="100" t="s">
         <v>25</v>
@@ -6122,10 +6219,10 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="108" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="J2" s="22" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="K2" s="99">
         <v>46055.0</v>
@@ -6135,7 +6232,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="O2" s="98"/>
       <c r="P2" s="23"/>
@@ -6158,13 +6255,13 @@
     </row>
     <row r="3">
       <c r="A3" s="100" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="B3" s="134" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
       <c r="C3" s="135" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="D3" s="100" t="s">
         <v>25</v>
@@ -6176,10 +6273,10 @@
       <c r="G3" s="103"/>
       <c r="H3" s="103"/>
       <c r="I3" s="100" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
       <c r="J3" s="136" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
       <c r="K3" s="99">
         <v>46055.0</v>
@@ -6189,7 +6286,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="100" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
       <c r="O3" s="137"/>
       <c r="P3" s="103"/>
@@ -6536,13 +6633,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -6557,7 +6654,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -6574,13 +6671,13 @@
     </row>
     <row r="2">
       <c r="A2" s="39" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>25</v>
@@ -6589,7 +6686,7 @@
         <v>17</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G2" s="41"/>
       <c r="H2" s="42"/>
@@ -6603,10 +6700,10 @@
         <v>19</v>
       </c>
       <c r="N2" s="40" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" s="46"/>
       <c r="Q2" s="46"/>
@@ -6624,13 +6721,13 @@
     </row>
     <row r="3">
       <c r="A3" s="39" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C3" s="39" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="D3" s="40" t="s">
         <v>25</v>
@@ -6639,7 +6736,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="40" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G3" s="41"/>
       <c r="H3" s="42"/>
@@ -6653,10 +6750,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="40" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" s="46"/>
       <c r="Q3" s="46"/>
@@ -6674,13 +6771,13 @@
     </row>
     <row r="4">
       <c r="A4" s="39" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="C4" s="39" t="s">
-        <v>68</v>
+        <v>77</v>
       </c>
       <c r="D4" s="40" t="s">
         <v>25</v>
@@ -6689,7 +6786,7 @@
         <v>17</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G4" s="41"/>
       <c r="H4" s="42"/>
@@ -6703,10 +6800,10 @@
         <v>19</v>
       </c>
       <c r="N4" s="40" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="O4" s="45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P4" s="46"/>
       <c r="Q4" s="46"/>
@@ -6724,13 +6821,13 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
@@ -6739,12 +6836,12 @@
         <v>25</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="13" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="J5" s="14"/>
       <c r="K5" s="47">
@@ -6776,22 +6873,22 @@
     </row>
     <row r="6">
       <c r="A6" s="39" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="B6" s="39" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C6" s="40" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D6" s="40" t="s">
         <v>25</v>
       </c>
       <c r="E6" s="40" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="F6" s="40" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G6" s="40"/>
       <c r="H6" s="42"/>
@@ -6805,10 +6902,10 @@
         <v>19</v>
       </c>
       <c r="N6" s="40" t="s">
-        <v>62</v>
+        <v>71</v>
       </c>
       <c r="O6" s="45" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P6" s="46"/>
       <c r="Q6" s="46"/>
@@ -6826,13 +6923,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>17</v>
@@ -6841,7 +6938,7 @@
         <v>25</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
@@ -6858,7 +6955,7 @@
         <v>20</v>
       </c>
       <c r="O7" s="49" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -6876,22 +6973,22 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
@@ -6924,22 +7021,22 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B9" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="13" t="s">
         <v>86</v>
-      </c>
-      <c r="C9" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>77</v>
       </c>
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
@@ -6953,7 +7050,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O9" s="14"/>
       <c r="P9" s="14"/>
@@ -6972,22 +7069,22 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G10" s="14"/>
       <c r="H10" s="14"/>
@@ -7001,7 +7098,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O10" s="14"/>
       <c r="P10" s="14"/>
@@ -7020,22 +7117,22 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>25</v>
       </c>
       <c r="E11" s="13" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G11" s="14"/>
       <c r="H11" s="14"/>
@@ -7068,22 +7165,22 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="E12" s="13" t="s">
         <v>25</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="K12" s="15">
         <v>45453.0</v>
@@ -7092,10 +7189,10 @@
         <v>45875.0</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -7209,16 +7306,16 @@
     </row>
     <row r="2">
       <c r="A2" s="50" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="B2" s="51" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="C2" s="51" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="D2" s="52" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
       <c r="E2" s="53" t="s">
         <v>26</v>
@@ -7236,10 +7333,10 @@
         <v>19</v>
       </c>
       <c r="N2" s="56" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="O2" s="57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P2" s="29"/>
       <c r="Q2" s="29"/>
@@ -7257,16 +7354,16 @@
     </row>
     <row r="3">
       <c r="A3" s="50" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
       <c r="B3" s="58" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
       <c r="C3" s="51" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="D3" s="51" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E3" s="56" t="s">
         <v>26</v>
@@ -7284,10 +7381,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="56" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="O3" s="57" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P3" s="29"/>
       <c r="Q3" s="29"/>
@@ -7305,16 +7402,16 @@
     </row>
     <row r="4">
       <c r="A4" s="51" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
       <c r="B4" s="56" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="D4" s="51" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -7324,7 +7421,7 @@
       <c r="H4" s="23"/>
       <c r="I4" s="59"/>
       <c r="J4" s="60" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
       <c r="K4" s="55">
         <v>44594.0</v>
@@ -7355,16 +7452,16 @@
     </row>
     <row r="5">
       <c r="A5" s="58" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B5" s="56" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
       <c r="D5" s="58" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -7374,7 +7471,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="60" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="K5" s="55">
         <v>44594.0</v>
@@ -7405,16 +7502,16 @@
     </row>
     <row r="6">
       <c r="A6" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" s="56" t="s">
+        <v>127</v>
+      </c>
+      <c r="D6" s="51" t="s">
         <v>116</v>
-      </c>
-      <c r="B6" s="56" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" s="56" t="s">
-        <v>118</v>
-      </c>
-      <c r="D6" s="51" t="s">
-        <v>107</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -7424,7 +7521,7 @@
       <c r="H6" s="23"/>
       <c r="I6" s="23"/>
       <c r="J6" s="61" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="K6" s="55">
         <v>44594.0</v>
@@ -10300,13 +10397,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -10321,7 +10418,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -10338,19 +10435,19 @@
     </row>
     <row r="2">
       <c r="A2" s="39" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
       <c r="C2" s="39" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>17</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="F2" s="46"/>
       <c r="G2" s="41"/>
@@ -10365,10 +10462,10 @@
         <v>19</v>
       </c>
       <c r="N2" s="40" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O2" s="45" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="P2" s="46"/>
       <c r="Q2" s="46"/>
@@ -10386,16 +10483,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>17</v>
@@ -10413,10 +10510,10 @@
         <v>19</v>
       </c>
       <c r="N3" s="13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O3" s="45" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -10540,13 +10637,13 @@
     </row>
     <row r="2">
       <c r="A2" s="62" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="B2" s="63" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
       <c r="C2" s="64" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D2" s="62" t="s">
         <v>34</v>
@@ -10558,10 +10655,10 @@
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
       <c r="I2" s="27" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="J2" s="65" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="K2" s="25">
         <v>43560.0</v>
@@ -10573,7 +10670,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="62" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="O2" s="28" t="s">
         <v>27</v>
@@ -10594,16 +10691,16 @@
     </row>
     <row r="3">
       <c r="A3" s="13" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -10613,7 +10710,7 @@
       <c r="H3" s="14"/>
       <c r="I3" s="14"/>
       <c r="J3" s="66" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="K3" s="15">
         <v>43620.0</v>
@@ -10626,7 +10723,7 @@
         <v>20</v>
       </c>
       <c r="O3" s="48" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="P3" s="14"/>
       <c r="Q3" s="14"/>
@@ -10644,16 +10741,16 @@
     </row>
     <row r="4">
       <c r="A4" s="13" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>26</v>
@@ -10662,7 +10759,7 @@
       <c r="G4" s="14"/>
       <c r="H4" s="14"/>
       <c r="I4" s="13" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="J4" s="14"/>
       <c r="K4" s="15">
@@ -10676,7 +10773,7 @@
         <v>20</v>
       </c>
       <c r="O4" s="48" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="P4" s="14"/>
       <c r="Q4" s="14"/>
@@ -10694,13 +10791,13 @@
     </row>
     <row r="5">
       <c r="A5" s="62" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
       <c r="C5" s="64" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
       <c r="D5" s="62" t="s">
         <v>34</v>
@@ -10710,16 +10807,16 @@
       </c>
       <c r="F5" s="21"/>
       <c r="G5" s="21" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
       <c r="H5" s="21" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="I5" s="67" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
       <c r="J5" s="68" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="K5" s="25">
         <v>43560.0</v>
@@ -10731,7 +10828,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="62" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="O5" s="28" t="s">
         <v>27</v>
@@ -10752,13 +10849,13 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
       <c r="D6" s="62" t="s">
         <v>34</v>
@@ -10770,10 +10867,10 @@
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="13" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="J6" s="66" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
       <c r="K6" s="15">
         <v>43620.0</v>
@@ -10788,7 +10885,7 @@
         <v>20</v>
       </c>
       <c r="O6" s="48" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="P6" s="14"/>
       <c r="Q6" s="14"/>
@@ -10806,13 +10903,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
       <c r="D7" s="13" t="s">
         <v>34</v>
@@ -10824,10 +10921,10 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="13" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="J7" s="69" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
       <c r="K7" s="15">
         <v>44447.0</v>
@@ -10837,10 +10934,10 @@
         <v>19</v>
       </c>
       <c r="N7" s="40" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="O7" s="48" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="P7" s="14"/>
       <c r="Q7" s="14"/>
@@ -10858,16 +10955,16 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>26</v>
@@ -10876,10 +10973,10 @@
       <c r="G8" s="14"/>
       <c r="H8" s="14"/>
       <c r="I8" s="70" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="K8" s="15">
         <v>44447.0</v>
@@ -10889,10 +10986,10 @@
         <v>19</v>
       </c>
       <c r="N8" s="40" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="O8" s="48" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="P8" s="14"/>
       <c r="Q8" s="14"/>
@@ -10910,16 +11007,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="E9" s="13" t="s">
         <v>26</v>
@@ -10928,7 +11025,7 @@
       <c r="G9" s="14"/>
       <c r="H9" s="14"/>
       <c r="I9" s="13" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="J9" s="14"/>
       <c r="K9" s="15">
@@ -10939,7 +11036,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="40" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="O9" s="48" t="s">
         <v>21</v>
@@ -10960,16 +11057,16 @@
     </row>
     <row r="10">
       <c r="A10" s="71" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B10" s="71" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="D10" s="73" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="E10" s="74" t="s">
         <v>26</v>
@@ -10979,7 +11076,7 @@
       <c r="H10" s="75"/>
       <c r="I10" s="75"/>
       <c r="J10" s="76" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
       <c r="K10" s="77">
         <v>44139.0</v>
@@ -10991,10 +11088,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="79" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
       <c r="O10" s="80" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P10" s="81"/>
       <c r="Q10" s="81"/>
@@ -11012,13 +11109,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>34</v>
@@ -11058,13 +11155,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>34</v>
@@ -11167,13 +11264,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>55</v>
+        <v>64</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -11188,7 +11285,7 @@
         <v>9</v>
       </c>
       <c r="K1" s="38" t="s">
-        <v>57</v>
+        <v>66</v>
       </c>
       <c r="L1" s="6" t="s">
         <v>11</v>
@@ -11205,13 +11302,13 @@
     </row>
     <row r="2">
       <c r="A2" s="82" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
       <c r="C2" s="83" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
       <c r="D2" s="82" t="s">
         <v>17</v>
@@ -11221,7 +11318,7 @@
         <v>dpv:DataController</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
@@ -11237,7 +11334,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="82" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
       <c r="O2" s="85" t="s">
         <v>27</v>
@@ -11258,22 +11355,22 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="D3" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="F3" s="86" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
       <c r="G3" s="23"/>
       <c r="H3" s="23"/>
@@ -11287,7 +11384,7 @@
         <v>19</v>
       </c>
       <c r="N3" s="21" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="O3" s="88" t="s">
         <v>31</v>
@@ -11308,22 +11405,22 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="B4" s="21" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
       <c r="C4" s="27" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D4" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="F4" s="86" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G4" s="23"/>
       <c r="H4" s="23"/>
@@ -11337,7 +11434,7 @@
         <v>19</v>
       </c>
       <c r="N4" s="21" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="O4" s="88" t="s">
         <v>31</v>
@@ -11358,28 +11455,28 @@
     </row>
     <row r="5">
       <c r="A5" s="13" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
       <c r="C5" s="89" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="D5" s="13" t="s">
         <v>17</v>
       </c>
       <c r="E5" s="13" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G5" s="14"/>
       <c r="H5" s="14"/>
       <c r="I5" s="14"/>
       <c r="J5" s="13" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
       <c r="K5" s="15">
         <v>43559.0</v>
@@ -11391,7 +11488,7 @@
         <v>19</v>
       </c>
       <c r="N5" s="13" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="O5" s="48" t="s">
         <v>27</v>
@@ -11412,22 +11509,22 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
       <c r="B6" s="21" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
       <c r="F6" s="86" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G6" s="23"/>
       <c r="H6" s="23"/>
@@ -11441,7 +11538,7 @@
         <v>19</v>
       </c>
       <c r="N6" s="21" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="O6" s="88" t="s">
         <v>31</v>
@@ -11462,22 +11559,22 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
       <c r="D7" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F7" s="86" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G7" s="23"/>
       <c r="H7" s="23"/>
@@ -11491,7 +11588,7 @@
         <v>19</v>
       </c>
       <c r="N7" s="21" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="O7" s="88" t="s">
         <v>31</v>
@@ -11512,22 +11609,22 @@
     </row>
     <row r="8">
       <c r="A8" s="27" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
       <c r="B8" s="27" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
       <c r="C8" s="27" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="D8" s="27" t="s">
         <v>17</v>
       </c>
       <c r="E8" s="27" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
       <c r="F8" s="27" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
@@ -11560,22 +11657,22 @@
     </row>
     <row r="9">
       <c r="A9" s="21" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="B9" s="21" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
       <c r="C9" s="27" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D9" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G9" s="23"/>
       <c r="H9" s="23"/>
@@ -11589,7 +11686,7 @@
         <v>19</v>
       </c>
       <c r="N9" s="21" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="O9" s="88" t="s">
         <v>31</v>
@@ -11610,22 +11707,22 @@
     </row>
     <row r="10">
       <c r="A10" s="21" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="B10" s="21" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="C10" s="27" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E10" s="21" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
       <c r="F10" s="86" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="G10" s="23"/>
       <c r="H10" s="23"/>
@@ -11639,7 +11736,7 @@
         <v>19</v>
       </c>
       <c r="N10" s="21" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
       <c r="O10" s="88" t="s">
         <v>31</v>
@@ -11660,22 +11757,22 @@
     </row>
     <row r="11">
       <c r="A11" s="21" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="C11" s="27" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
       <c r="D11" s="21" t="s">
         <v>17</v>
       </c>
       <c r="E11" s="21" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="F11" s="86" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="G11" s="23"/>
       <c r="H11" s="23"/>
@@ -11689,10 +11786,10 @@
         <v>19</v>
       </c>
       <c r="N11" s="21" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="O11" s="88" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="P11" s="29"/>
       <c r="Q11" s="29"/>
@@ -11710,22 +11807,22 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="D12" s="13" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G12" s="14"/>
       <c r="H12" s="14"/>
@@ -11758,22 +11855,22 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="D13" s="13" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="E13" s="13" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="G13" s="14"/>
       <c r="H13" s="14"/>
@@ -11897,13 +11994,13 @@
     </row>
     <row r="2">
       <c r="A2" s="21" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="B2" s="82" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="D2" s="21" t="s">
         <v>34</v>
@@ -11945,16 +12042,16 @@
     </row>
     <row r="3">
       <c r="A3" s="21" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="B3" s="91" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="D3" s="86" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E3" s="22" t="s">
         <v>26</v>
@@ -11964,7 +12061,7 @@
       <c r="H3" s="23"/>
       <c r="I3" s="23"/>
       <c r="J3" s="21" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="K3" s="25">
         <v>44594.0</v>
@@ -11997,16 +12094,16 @@
     </row>
     <row r="4">
       <c r="A4" s="21" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="D4" s="86" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E4" s="22" t="s">
         <v>26</v>
@@ -12047,16 +12144,16 @@
     </row>
     <row r="5">
       <c r="A5" s="21" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="B5" s="91" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
       <c r="C5" s="21" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D5" s="86" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E5" s="22" t="s">
         <v>26</v>
@@ -12066,7 +12163,7 @@
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="21" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="K5" s="25">
         <v>44594.0</v>
@@ -12099,16 +12196,16 @@
     </row>
     <row r="6">
       <c r="A6" s="21" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
       <c r="B6" s="91" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="D6" s="86" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E6" s="22" t="s">
         <v>26</v>
@@ -12149,16 +12246,16 @@
     </row>
     <row r="7">
       <c r="A7" s="21" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
       <c r="B7" s="91" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="C7" s="21" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
       <c r="D7" s="86" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E7" s="22" t="s">
         <v>26</v>
@@ -12168,7 +12265,7 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="21" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="K7" s="25">
         <v>44594.0</v>
@@ -12201,16 +12298,16 @@
     </row>
     <row r="8">
       <c r="A8" s="21" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="B8" s="91" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
       <c r="C8" s="21" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="D8" s="86" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E8" s="22" t="s">
         <v>26</v>
@@ -12220,7 +12317,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="21" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="K8" s="25">
         <v>44594.0</v>
@@ -12253,16 +12350,16 @@
     </row>
     <row r="9">
       <c r="A9" s="51" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="B9" s="51" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
       <c r="C9" s="51" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D9" s="93" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E9" s="22" t="s">
         <v>26</v>
@@ -12272,7 +12369,7 @@
       <c r="H9" s="23"/>
       <c r="I9" s="23"/>
       <c r="J9" s="60" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="K9" s="55">
         <v>44643.0</v>
@@ -12284,10 +12381,10 @@
         <v>19</v>
       </c>
       <c r="N9" s="51" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="O9" s="94" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="P9" s="29"/>
       <c r="Q9" s="29"/>
@@ -12305,13 +12402,13 @@
     </row>
     <row r="10">
       <c r="A10" s="51" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="B10" s="51" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
       <c r="C10" s="93" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D10" s="22" t="s">
         <v>25</v>
@@ -12332,10 +12429,10 @@
         <v>19</v>
       </c>
       <c r="N10" s="51" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="O10" s="94" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
       <c r="P10" s="29"/>
       <c r="Q10" s="29"/>
@@ -12353,13 +12450,13 @@
     </row>
     <row r="11">
       <c r="A11" s="95" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
       <c r="B11" s="95" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="D11" s="13" t="s">
         <v>34</v>
@@ -12380,7 +12477,7 @@
         <v>19</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O11" s="14"/>
       <c r="P11" s="14"/>
@@ -12399,13 +12496,13 @@
     </row>
     <row r="12">
       <c r="A12" s="95" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="B12" s="95" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>34</v>
@@ -12426,7 +12523,7 @@
         <v>19</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O12" s="14"/>
       <c r="P12" s="14"/>
@@ -12445,13 +12542,13 @@
     </row>
     <row r="13">
       <c r="A13" s="95" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B13" s="95" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="D13" s="13" t="s">
         <v>34</v>
@@ -12472,7 +12569,7 @@
         <v>19</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O13" s="14"/>
       <c r="P13" s="14"/>
@@ -12491,13 +12588,13 @@
     </row>
     <row r="14">
       <c r="A14" s="95" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="B14" s="95" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>34</v>
@@ -12518,7 +12615,7 @@
         <v>19</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O14" s="14"/>
       <c r="P14" s="14"/>
@@ -12537,13 +12634,13 @@
     </row>
     <row r="15">
       <c r="A15" s="95" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="B15" s="95" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="D15" s="13" t="s">
         <v>34</v>
@@ -12564,7 +12661,7 @@
         <v>19</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O15" s="14"/>
       <c r="P15" s="14"/>
@@ -12583,16 +12680,16 @@
     </row>
     <row r="16">
       <c r="A16" s="39" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
       <c r="D16" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E16" s="40" t="s">
         <v>26</v>
@@ -12610,7 +12707,7 @@
         <v>19</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O16" s="40"/>
       <c r="P16" s="46"/>
@@ -12629,16 +12726,16 @@
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
       <c r="D17" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E17" s="40" t="s">
         <v>26</v>
@@ -12656,7 +12753,7 @@
         <v>19</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="14"/>
@@ -12675,16 +12772,16 @@
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="D18" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E18" s="40" t="s">
         <v>26</v>
@@ -12702,7 +12799,7 @@
         <v>19</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O18" s="14"/>
       <c r="P18" s="14"/>
@@ -12721,16 +12818,16 @@
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="D19" s="40" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="E19" s="40" t="s">
         <v>26</v>
@@ -12748,7 +12845,7 @@
         <v>19</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O19" s="14"/>
       <c r="P19" s="14"/>
@@ -12767,16 +12864,16 @@
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="D20" s="40" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="E20" s="40" t="s">
         <v>26</v>
@@ -12794,7 +12891,7 @@
         <v>19</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O20" s="14"/>
       <c r="P20" s="14"/>
@@ -12813,16 +12910,16 @@
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
       <c r="D21" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E21" s="40" t="s">
         <v>26</v>
@@ -12840,7 +12937,7 @@
         <v>19</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O21" s="14"/>
       <c r="P21" s="14"/>
@@ -12859,16 +12956,16 @@
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
       <c r="C22" s="13" t="s">
+        <v>315</v>
+      </c>
+      <c r="D22" s="40" t="s">
         <v>306</v>
-      </c>
-      <c r="D22" s="40" t="s">
-        <v>297</v>
       </c>
       <c r="E22" s="40" t="s">
         <v>26</v>
@@ -12886,7 +12983,7 @@
         <v>19</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O22" s="14"/>
       <c r="P22" s="14"/>
@@ -12905,16 +13002,16 @@
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E23" s="40" t="s">
         <v>26</v>
@@ -12932,7 +13029,7 @@
         <v>19</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O23" s="14"/>
       <c r="P23" s="14"/>
@@ -12951,16 +13048,16 @@
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
       <c r="D24" s="40" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E24" s="40" t="s">
         <v>26</v>
@@ -12978,7 +13075,7 @@
         <v>19</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O24" s="14"/>
       <c r="P24" s="14"/>
@@ -12997,16 +13094,16 @@
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>313</v>
+        <v>322</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>26</v>
@@ -13024,7 +13121,7 @@
         <v>19</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O25" s="14"/>
       <c r="P25" s="14"/>
@@ -13043,16 +13140,16 @@
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>315</v>
+        <v>324</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>316</v>
+        <v>325</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="E26" s="13" t="s">
         <v>26</v>
@@ -13070,7 +13167,7 @@
         <v>19</v>
       </c>
       <c r="N26" s="13" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="14"/>
@@ -13089,62 +13186,62 @@
     </row>
     <row r="39">
       <c r="A39" s="8" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="13" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="13" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="13" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="13" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="13" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="13" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="13" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="13" t="s">
-        <v>325</v>
+        <v>334</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="13" t="s">
-        <v>326</v>
+        <v>335</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="13" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="13" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -13256,13 +13353,13 @@
     </row>
     <row r="2">
       <c r="A2" s="27" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
       <c r="B2" s="91" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
       <c r="D2" s="97" t="s">
         <v>34</v>
@@ -13283,7 +13380,7 @@
         <v>19</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="O2" s="98"/>
       <c r="P2" s="23"/>
@@ -13306,16 +13403,16 @@
     </row>
     <row r="3">
       <c r="A3" s="100" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="B3" s="101" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C3" s="102" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="D3" s="13" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="E3" s="13" t="s">
         <v>26</v>
@@ -13324,10 +13421,10 @@
       <c r="G3" s="103"/>
       <c r="H3" s="103"/>
       <c r="I3" s="97" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="J3" s="104" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
       <c r="K3" s="105">
         <v>43560.0</v>
@@ -13336,10 +13433,10 @@
         <v>45643.0</v>
       </c>
       <c r="M3" s="100" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N3" s="97" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="O3" s="106" t="s">
         <v>27</v>
@@ -13367,25 +13464,25 @@
     </row>
     <row r="5">
       <c r="A5" s="62" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="B5" s="63" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C5" s="62" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="E5" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F5" s="23"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="107" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="J5" s="23"/>
       <c r="K5" s="25">
@@ -13395,13 +13492,13 @@
         <v>45643.0</v>
       </c>
       <c r="M5" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N5" s="62" t="s">
         <v>20</v>
       </c>
       <c r="O5" s="107" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="P5" s="29"/>
       <c r="Q5" s="29"/>
@@ -13423,16 +13520,16 @@
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="E6" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K6" s="15">
         <v>44650.0</v>
@@ -13441,28 +13538,28 @@
         <v>45643.0</v>
       </c>
       <c r="M6" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N6" s="40" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O6" s="48" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="27" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="B7" s="91" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="C7" s="27" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
@@ -13500,25 +13597,25 @@
     </row>
     <row r="8">
       <c r="A8" s="62" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="B8" s="63" t="s">
+        <v>359</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="C8" s="27" t="s">
-        <v>351</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>341</v>
-      </c>
       <c r="E8" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F8" s="23"/>
       <c r="G8" s="23"/>
       <c r="H8" s="23"/>
       <c r="I8" s="110" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
       <c r="J8" s="62"/>
       <c r="K8" s="25">
@@ -13528,13 +13625,13 @@
         <v>45643.0</v>
       </c>
       <c r="M8" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N8" s="27" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="O8" s="107" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="P8" s="29"/>
       <c r="Q8" s="29"/>
@@ -13556,16 +13653,16 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
       <c r="E9" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K9" s="15">
         <v>44657.0</v>
@@ -13574,27 +13671,27 @@
         <v>45643.0</v>
       </c>
       <c r="M9" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N9" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O9" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
       <c r="E10" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K10" s="15">
         <v>44657.0</v>
@@ -13603,27 +13700,27 @@
         <v>45643.0</v>
       </c>
       <c r="M10" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N10" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O10" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
       <c r="E11" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K11" s="15">
         <v>44657.0</v>
@@ -13632,27 +13729,27 @@
         <v>45643.0</v>
       </c>
       <c r="M11" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N11" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O11" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
       <c r="E12" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K12" s="15">
         <v>44657.0</v>
@@ -13661,27 +13758,27 @@
         <v>45643.0</v>
       </c>
       <c r="M12" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N12" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O12" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="E13" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K13" s="15">
         <v>44657.0</v>
@@ -13690,27 +13787,27 @@
         <v>45643.0</v>
       </c>
       <c r="M13" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N13" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O13" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="13" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
       <c r="E14" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K14" s="15">
         <v>44657.0</v>
@@ -13719,27 +13816,27 @@
         <v>45643.0</v>
       </c>
       <c r="M14" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N14" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O14" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="13" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
       <c r="E15" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K15" s="15">
         <v>44657.0</v>
@@ -13748,30 +13845,30 @@
         <v>45643.0</v>
       </c>
       <c r="M15" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N15" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O15" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="13" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="E16" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
       <c r="K16" s="15">
         <v>44657.0</v>
@@ -13780,27 +13877,27 @@
         <v>45643.0</v>
       </c>
       <c r="M16" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N16" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O16" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="13" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
       <c r="E17" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K17" s="15">
         <v>44657.0</v>
@@ -13809,27 +13906,27 @@
         <v>45643.0</v>
       </c>
       <c r="M17" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N17" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O17" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="13" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="E18" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K18" s="15">
         <v>44657.0</v>
@@ -13838,27 +13935,27 @@
         <v>45643.0</v>
       </c>
       <c r="M18" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N18" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O18" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="13" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
       <c r="E19" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K19" s="15">
         <v>44657.0</v>
@@ -13867,27 +13964,27 @@
         <v>45643.0</v>
       </c>
       <c r="M19" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N19" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O19" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="13" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
       <c r="E20" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K20" s="15">
         <v>44657.0</v>
@@ -13896,27 +13993,27 @@
         <v>45643.0</v>
       </c>
       <c r="M20" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N20" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O20" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="13" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
       <c r="E21" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K21" s="15">
         <v>44657.0</v>
@@ -13925,27 +14022,27 @@
         <v>45643.0</v>
       </c>
       <c r="M21" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N21" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O21" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="13" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
       <c r="E22" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K22" s="15">
         <v>44657.0</v>
@@ -13954,30 +14051,30 @@
         <v>45643.0</v>
       </c>
       <c r="M22" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N22" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O22" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="13" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
       <c r="E23" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="I23" s="13" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="K23" s="15">
         <v>44657.0</v>
@@ -13986,30 +14083,30 @@
         <v>45643.0</v>
       </c>
       <c r="M23" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N23" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O23" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="13" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
       <c r="E24" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K24" s="15">
         <v>44657.0</v>
@@ -14018,27 +14115,27 @@
         <v>45643.0</v>
       </c>
       <c r="M24" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N24" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O24" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="13" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
       <c r="E25" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K25" s="15">
         <v>44657.0</v>
@@ -14047,30 +14144,30 @@
         <v>45643.0</v>
       </c>
       <c r="M25" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N25" s="13" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="O25" s="48" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="13" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="E26" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
@@ -14108,19 +14205,19 @@
     </row>
     <row r="27">
       <c r="A27" s="13" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
       <c r="E27" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K27" s="15">
         <v>44727.0</v>
@@ -14129,30 +14226,30 @@
         <v>45643.0</v>
       </c>
       <c r="M27" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N27" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O27" s="48" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="13" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="E28" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K28" s="15">
         <v>44727.0</v>
@@ -14161,30 +14258,30 @@
         <v>45643.0</v>
       </c>
       <c r="M28" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N28" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O28" s="48" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="13" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="E29" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -14222,19 +14319,19 @@
     </row>
     <row r="30">
       <c r="A30" s="13" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="E30" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K30" s="15">
         <v>44727.0</v>
@@ -14243,28 +14340,28 @@
         <v>45643.0</v>
       </c>
       <c r="M30" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N30" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O30" s="48" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="13" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
       <c r="D31" s="14"/>
       <c r="E31" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="14"/>
@@ -14302,19 +14399,19 @@
     </row>
     <row r="32">
       <c r="A32" s="13" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
       <c r="D32" s="13" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="E32" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K32" s="15">
         <v>44776.0</v>
@@ -14323,28 +14420,28 @@
         <v>45643.0</v>
       </c>
       <c r="M32" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N32" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O32" s="48" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="13" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
       <c r="D33" s="14"/>
       <c r="E33" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -14382,19 +14479,19 @@
     </row>
     <row r="34">
       <c r="A34" s="13" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="D34" s="13" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
       <c r="E34" s="27" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="K34" s="15">
         <v>44776.0</v>
@@ -14403,13 +14500,13 @@
         <v>45643.0</v>
       </c>
       <c r="M34" s="27" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="N34" s="13" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="O34" s="48" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -14536,13 +14633,13 @@
     </row>
     <row r="2">
       <c r="A2" s="32" t="s">
-        <v>333</v>
+        <v>342</v>
       </c>
       <c r="B2" s="118" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="C2" s="119" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
       <c r="D2" s="120" t="s">
         <v>34</v>
@@ -14554,7 +14651,7 @@
       <c r="G2" s="33"/>
       <c r="H2" s="33"/>
       <c r="I2" s="120" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="J2" s="121"/>
       <c r="K2" s="122"/>
@@ -14584,22 +14681,22 @@
     </row>
     <row r="3">
       <c r="A3" s="124" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="B3" s="125" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="C3" s="124" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="F3" s="36"/>
       <c r="G3" s="36"/>
       <c r="H3" s="36"/>
       <c r="I3" s="126" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="J3" s="36"/>
       <c r="K3" s="127"/>
@@ -14607,7 +14704,7 @@
       <c r="M3" s="10"/>
       <c r="N3" s="124"/>
       <c r="O3" s="126" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="P3" s="129"/>
       <c r="Q3" s="129"/>
@@ -14634,18 +14731,18 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="13" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="D6" s="14"/>
       <c r="E6" s="10"/>
@@ -14656,12 +14753,12 @@
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K6" s="15"/>
       <c r="L6" s="14"/>
       <c r="M6" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N6" s="14"/>
       <c r="O6" s="14"/>
@@ -14685,13 +14782,13 @@
     </row>
     <row r="7">
       <c r="A7" s="13" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="D7" s="14"/>
       <c r="E7" s="10"/>
@@ -14702,12 +14799,12 @@
       <c r="H7" s="14"/>
       <c r="I7" s="14"/>
       <c r="J7" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K7" s="15"/>
       <c r="L7" s="14"/>
       <c r="M7" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N7" s="14"/>
       <c r="O7" s="14"/>
@@ -14731,13 +14828,13 @@
     </row>
     <row r="8">
       <c r="A8" s="13" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="D8" s="14"/>
       <c r="E8" s="10"/>
@@ -14748,12 +14845,12 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K8" s="15"/>
       <c r="L8" s="14"/>
       <c r="M8" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N8" s="14"/>
       <c r="O8" s="14"/>
@@ -14777,13 +14874,13 @@
     </row>
     <row r="9">
       <c r="A9" s="13" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
       <c r="D9" s="14"/>
       <c r="E9" s="10"/>
@@ -14794,12 +14891,12 @@
       <c r="H9" s="14"/>
       <c r="I9" s="14"/>
       <c r="J9" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K9" s="15"/>
       <c r="L9" s="14"/>
       <c r="M9" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N9" s="14"/>
       <c r="O9" s="14"/>
@@ -14823,13 +14920,13 @@
     </row>
     <row r="10">
       <c r="A10" s="13" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
       <c r="D10" s="14"/>
       <c r="E10" s="10"/>
@@ -14840,12 +14937,12 @@
       <c r="H10" s="14"/>
       <c r="I10" s="14"/>
       <c r="J10" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K10" s="15"/>
       <c r="L10" s="14"/>
       <c r="M10" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N10" s="14"/>
       <c r="O10" s="14"/>
@@ -14869,13 +14966,13 @@
     </row>
     <row r="11">
       <c r="A11" s="13" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="10"/>
@@ -14886,12 +14983,12 @@
       <c r="H11" s="14"/>
       <c r="I11" s="14"/>
       <c r="J11" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K11" s="15"/>
       <c r="L11" s="14"/>
       <c r="M11" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N11" s="14"/>
       <c r="O11" s="14"/>
@@ -14915,13 +15012,13 @@
     </row>
     <row r="12">
       <c r="A12" s="13" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="10"/>
@@ -14932,12 +15029,12 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K12" s="15"/>
       <c r="L12" s="14"/>
       <c r="M12" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N12" s="14"/>
       <c r="O12" s="14"/>
@@ -14961,13 +15058,13 @@
     </row>
     <row r="13">
       <c r="A13" s="13" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="10"/>
@@ -14978,12 +15075,12 @@
       <c r="H13" s="14"/>
       <c r="I13" s="14"/>
       <c r="J13" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K13" s="15"/>
       <c r="L13" s="14"/>
       <c r="M13" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N13" s="14"/>
       <c r="O13" s="14"/>
@@ -15007,13 +15104,13 @@
     </row>
     <row r="14">
       <c r="A14" s="10" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="B14" s="130" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="10"/>
@@ -15024,12 +15121,12 @@
       <c r="H14" s="36"/>
       <c r="I14" s="131"/>
       <c r="J14" s="13" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
       <c r="K14" s="127"/>
       <c r="L14" s="132"/>
       <c r="M14" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="126"/>

</xml_diff>

<commit_message>
fix `DataUser` and `DataHolder` in SECTOR-HEALTH
- terms and labels/definitions were mixed
- reported by @nuthub in #416

Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -1545,25 +1545,25 @@
     <t>Indicates association with Human Subject</t>
   </si>
   <si>
+    <t>DataHolder</t>
+  </si>
+  <si>
+    <t>Data Holder</t>
+  </si>
+  <si>
+    <t>Natural or legal person with access to health data (draft definition)</t>
+  </si>
+  <si>
+    <t>to extend in GDNG and EHDS extensions</t>
+  </si>
+  <si>
+    <t>none, but based on GDNG's definition</t>
+  </si>
+  <si>
+    <t>Julian Flake</t>
+  </si>
+  <si>
     <t>DataUser</t>
-  </si>
-  <si>
-    <t>Data Holder</t>
-  </si>
-  <si>
-    <t>Natural or legal person with access to health data (draft definition)</t>
-  </si>
-  <si>
-    <t>to extend in GDNG and EHDS extensions</t>
-  </si>
-  <si>
-    <t>none, but based on GDNG's definition</t>
-  </si>
-  <si>
-    <t>Julian Flake</t>
-  </si>
-  <si>
-    <t>DataHolder</t>
   </si>
   <si>
     <t>Data User</t>
@@ -6200,7 +6200,7 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="13" t="s">
         <v>477</v>
       </c>
       <c r="B2" s="91" t="s">
@@ -6254,7 +6254,7 @@
       <c r="AF2" s="23"/>
     </row>
     <row r="3">
-      <c r="A3" s="100" t="s">
+      <c r="A3" s="27" t="s">
         <v>483</v>
       </c>
       <c r="B3" s="134" t="s">

</xml_diff>

<commit_message>
SECTOR-HEALTH prefix `HealthData<term>` entities
- added `Health` as prefix to `DataHolder` and `DataUser` in
  SECTOR-HEALTH to better align these terms with those in EU-EHDS and
  GDNG extensions
- modified definition of entities to better reflect their roles

Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1142" uniqueCount="486">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="484">
   <si>
     <t>Term</t>
   </si>
@@ -1545,31 +1545,25 @@
     <t>Indicates association with Human Subject</t>
   </si>
   <si>
-    <t>DataHolder</t>
-  </si>
-  <si>
-    <t>Data Holder</t>
-  </si>
-  <si>
-    <t>Natural or legal person with access to health data (draft definition)</t>
-  </si>
-  <si>
-    <t>to extend in GDNG and EHDS extensions</t>
-  </si>
-  <si>
-    <t>none, but based on GDNG's definition</t>
+    <t>HealthDataHolder</t>
+  </si>
+  <si>
+    <t>Health Data Holder</t>
+  </si>
+  <si>
+    <t>Entity that has the authority to use and make available health data (draft definition)</t>
   </si>
   <si>
     <t>Julian Flake</t>
   </si>
   <si>
-    <t>DataUser</t>
-  </si>
-  <si>
-    <t>Data User</t>
-  </si>
-  <si>
-    <t>Natural or legal person requested or obtained access to health data (draft definition)</t>
+    <t>HealthDataUser</t>
+  </si>
+  <si>
+    <t>Health Data User</t>
+  </si>
+  <si>
+    <t>Entity that has requested or obtained access to use health data (draft definition)</t>
   </si>
 </sst>
 </file>
@@ -6218,21 +6212,17 @@
       <c r="F2" s="23"/>
       <c r="G2" s="23"/>
       <c r="H2" s="23"/>
-      <c r="I2" s="108" t="s">
-        <v>480</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>481</v>
-      </c>
+      <c r="I2" s="108"/>
+      <c r="J2" s="22"/>
       <c r="K2" s="99">
-        <v>46055.0</v>
+        <v>46059.0</v>
       </c>
       <c r="L2" s="14"/>
       <c r="M2" s="27" t="s">
         <v>19</v>
       </c>
       <c r="N2" s="27" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="O2" s="98"/>
       <c r="P2" s="23"/>
@@ -6255,13 +6245,13 @@
     </row>
     <row r="3">
       <c r="A3" s="27" t="s">
+        <v>481</v>
+      </c>
+      <c r="B3" s="134" t="s">
+        <v>482</v>
+      </c>
+      <c r="C3" s="135" t="s">
         <v>483</v>
-      </c>
-      <c r="B3" s="134" t="s">
-        <v>484</v>
-      </c>
-      <c r="C3" s="135" t="s">
-        <v>485</v>
       </c>
       <c r="D3" s="100" t="s">
         <v>25</v>
@@ -6272,21 +6262,17 @@
       <c r="F3" s="103"/>
       <c r="G3" s="103"/>
       <c r="H3" s="103"/>
-      <c r="I3" s="100" t="s">
-        <v>480</v>
-      </c>
-      <c r="J3" s="136" t="s">
-        <v>481</v>
-      </c>
+      <c r="I3" s="100"/>
+      <c r="J3" s="136"/>
       <c r="K3" s="99">
-        <v>46055.0</v>
+        <v>46059.0</v>
       </c>
       <c r="L3" s="99"/>
       <c r="M3" s="100" t="s">
         <v>19</v>
       </c>
       <c r="N3" s="100" t="s">
-        <v>482</v>
+        <v>480</v>
       </c>
       <c r="O3" s="137"/>
       <c r="P3" s="103"/>

</xml_diff>

<commit_message>
Proposed concepts from @besteves4 for EU-EHDS
- includes source spreadsheets, RDF and HTML outputs
- the concepts are still in a proposed stage, which should be changed to
  accepted with the vocab in draft form (confirm with contributors)

Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>
Co-authored-by: Julian Flake <flake@uni-koblenz.de>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1138" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1224" uniqueCount="530">
   <si>
     <t>Term</t>
   </si>
@@ -1565,6 +1565,144 @@
   <si>
     <t>Entity that has requested or obtained access to use health data (draft definition)</t>
   </si>
+  <si>
+    <t>HealthProfessional</t>
+  </si>
+  <si>
+    <t>Health Professional</t>
+  </si>
+  <si>
+    <t>An entity that works as a health professional</t>
+  </si>
+  <si>
+    <t>HealthcareProvider</t>
+  </si>
+  <si>
+    <t>Healthcare Provider</t>
+  </si>
+  <si>
+    <t>An entity that provides healthcare-related services</t>
+  </si>
+  <si>
+    <t>HealthDataAccessBody</t>
+  </si>
+  <si>
+    <t>Health Data Access Body</t>
+  </si>
+  <si>
+    <t>An entity responsible for granting access to electronic health data for secondary use</t>
+  </si>
+  <si>
+    <t>EHRSystemManufacturer</t>
+  </si>
+  <si>
+    <t>Electronic Health Record System Manufacturer</t>
+  </si>
+  <si>
+    <t>Actor that manufactures electronic health record systems</t>
+  </si>
+  <si>
+    <t>tech:Manufacturer</t>
+  </si>
+  <si>
+    <t>tech:Actor</t>
+  </si>
+  <si>
+    <t>EHRSystemSupplier</t>
+  </si>
+  <si>
+    <t>Electronic Health Record System Supplier</t>
+  </si>
+  <si>
+    <t>Actor that supplies electronic health record systems</t>
+  </si>
+  <si>
+    <t>tech:Supplier</t>
+  </si>
+  <si>
+    <t>EHRSystemImporter</t>
+  </si>
+  <si>
+    <t>Electronic Health Record System Importer</t>
+  </si>
+  <si>
+    <t>Actor that imports electronic health record systems</t>
+  </si>
+  <si>
+    <t>tech:Importer</t>
+  </si>
+  <si>
+    <t>EHDS Art.32</t>
+  </si>
+  <si>
+    <t>EHRSystemDistributor</t>
+  </si>
+  <si>
+    <t>Electronic Health Record System Distributor</t>
+  </si>
+  <si>
+    <t>Actor that distributes electronic health record systems</t>
+  </si>
+  <si>
+    <t>tech:Distributor</t>
+  </si>
+  <si>
+    <t>EHDS Art.33</t>
+  </si>
+  <si>
+    <t>WellnessAppManufacturer</t>
+  </si>
+  <si>
+    <t>Wellness App Manufacturer</t>
+  </si>
+  <si>
+    <t>Actor that manufactures wellness apps</t>
+  </si>
+  <si>
+    <t>WellnessAppSupplier</t>
+  </si>
+  <si>
+    <t>Wellness App Supplier</t>
+  </si>
+  <si>
+    <t>Actor that supplies wellness apps</t>
+  </si>
+  <si>
+    <t>WellnessAppDistributor</t>
+  </si>
+  <si>
+    <t>Wellness App Distributor</t>
+  </si>
+  <si>
+    <t>Actor that distributes wellness apps</t>
+  </si>
+  <si>
+    <t>EHDS Art.47.9</t>
+  </si>
+  <si>
+    <t>DigitalHealthAuthority</t>
+  </si>
+  <si>
+    <t>Digital Health Authority</t>
+  </si>
+  <si>
+    <t>An authority tasked with overseeing the implementation and enforcement of primary use provisions</t>
+  </si>
+  <si>
+    <t>EHDS Art.19</t>
+  </si>
+  <si>
+    <t>MedicalDeviceManufacturer</t>
+  </si>
+  <si>
+    <t>Medical Device Manufacturer</t>
+  </si>
+  <si>
+    <t>Actor that manufactures medical devices</t>
+  </si>
+  <si>
+    <t>EHDS Art.27.1</t>
+  </si>
 </sst>
 </file>
 
@@ -1573,7 +1711,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
   </numFmts>
-  <fonts count="39">
+  <fonts count="40">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -1764,8 +1902,12 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1794,6 +1936,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFCE5CD"/>
         <bgColor rgb="FFFCE5CD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCFE2F3"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -1861,7 +2009,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="144">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -2270,6 +2418,24 @@
     <xf borderId="0" fillId="3" fontId="38" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="0" fillId="6" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="39" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="39" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="6" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -6294,163 +6460,620 @@
       <c r="AF3" s="103"/>
     </row>
     <row r="4">
-      <c r="L4" s="99"/>
+      <c r="A4" s="138" t="s">
+        <v>484</v>
+      </c>
+      <c r="B4" s="138" t="s">
+        <v>485</v>
+      </c>
+      <c r="C4" s="138" t="s">
+        <v>486</v>
+      </c>
+      <c r="D4" s="138" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="139"/>
+      <c r="F4" s="139"/>
+      <c r="G4" s="139"/>
+      <c r="H4" s="139"/>
+      <c r="I4" s="139"/>
+      <c r="J4" s="139"/>
+      <c r="K4" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L4" s="141"/>
+      <c r="M4" s="138" t="s">
+        <v>42</v>
+      </c>
+      <c r="N4" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" s="139"/>
+      <c r="P4" s="139"/>
+      <c r="Q4" s="139"/>
+      <c r="R4" s="139"/>
+      <c r="S4" s="139"/>
+      <c r="T4" s="139"/>
+      <c r="U4" s="139"/>
+      <c r="V4" s="139"/>
+      <c r="W4" s="139"/>
+      <c r="X4" s="139"/>
+      <c r="Y4" s="139"/>
+      <c r="Z4" s="139"/>
+      <c r="AA4" s="139"/>
+      <c r="AB4" s="139"/>
+      <c r="AC4" s="139"/>
+      <c r="AD4" s="139"/>
+      <c r="AE4" s="139"/>
+      <c r="AF4" s="139"/>
     </row>
     <row r="5">
-      <c r="A5" s="62"/>
-      <c r="B5" s="63"/>
-      <c r="C5" s="62"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="99"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="62"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23"/>
-      <c r="V5" s="23"/>
-      <c r="W5" s="23"/>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="23"/>
-      <c r="AC5" s="23"/>
-      <c r="AD5" s="23"/>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
+      <c r="A5" s="142" t="s">
+        <v>487</v>
+      </c>
+      <c r="B5" s="142" t="s">
+        <v>488</v>
+      </c>
+      <c r="C5" s="142" t="s">
+        <v>489</v>
+      </c>
+      <c r="D5" s="138" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="143"/>
+      <c r="F5" s="139"/>
+      <c r="G5" s="139"/>
+      <c r="H5" s="139"/>
+      <c r="I5" s="143"/>
+      <c r="J5" s="139"/>
+      <c r="K5" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L5" s="141"/>
+      <c r="M5" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N5" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" s="143"/>
+      <c r="P5" s="139"/>
+      <c r="Q5" s="139"/>
+      <c r="R5" s="139"/>
+      <c r="S5" s="139"/>
+      <c r="T5" s="139"/>
+      <c r="U5" s="139"/>
+      <c r="V5" s="139"/>
+      <c r="W5" s="139"/>
+      <c r="X5" s="139"/>
+      <c r="Y5" s="139"/>
+      <c r="Z5" s="139"/>
+      <c r="AA5" s="139"/>
+      <c r="AB5" s="139"/>
+      <c r="AC5" s="139"/>
+      <c r="AD5" s="139"/>
+      <c r="AE5" s="139"/>
+      <c r="AF5" s="139"/>
     </row>
     <row r="6">
-      <c r="E6" s="27"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="99"/>
-      <c r="M6" s="27"/>
-      <c r="N6" s="40"/>
+      <c r="A6" s="138" t="s">
+        <v>490</v>
+      </c>
+      <c r="B6" s="138" t="s">
+        <v>491</v>
+      </c>
+      <c r="C6" s="138" t="s">
+        <v>492</v>
+      </c>
+      <c r="D6" s="138" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="143"/>
+      <c r="F6" s="139"/>
+      <c r="G6" s="139"/>
+      <c r="H6" s="139"/>
+      <c r="I6" s="139"/>
+      <c r="J6" s="139"/>
+      <c r="K6" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L6" s="141"/>
+      <c r="M6" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N6" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" s="139"/>
+      <c r="P6" s="139"/>
+      <c r="Q6" s="139"/>
+      <c r="R6" s="139"/>
+      <c r="S6" s="139"/>
+      <c r="T6" s="139"/>
+      <c r="U6" s="139"/>
+      <c r="V6" s="139"/>
+      <c r="W6" s="139"/>
+      <c r="X6" s="139"/>
+      <c r="Y6" s="139"/>
+      <c r="Z6" s="139"/>
+      <c r="AA6" s="139"/>
+      <c r="AB6" s="139"/>
+      <c r="AC6" s="139"/>
+      <c r="AD6" s="139"/>
+      <c r="AE6" s="139"/>
+      <c r="AF6" s="139"/>
     </row>
     <row r="7">
-      <c r="A7" s="27"/>
-      <c r="B7" s="91"/>
-      <c r="C7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="108"/>
-      <c r="J7" s="62"/>
-      <c r="K7" s="109"/>
-      <c r="L7" s="99"/>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="98"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23"/>
-      <c r="V7" s="23"/>
-      <c r="W7" s="23"/>
-      <c r="X7" s="23"/>
-      <c r="Y7" s="23"/>
-      <c r="Z7" s="23"/>
-      <c r="AA7" s="23"/>
-      <c r="AB7" s="23"/>
-      <c r="AC7" s="23"/>
-      <c r="AD7" s="23"/>
-      <c r="AE7" s="23"/>
-      <c r="AF7" s="23"/>
+      <c r="A7" s="142" t="s">
+        <v>493</v>
+      </c>
+      <c r="B7" s="142" t="s">
+        <v>494</v>
+      </c>
+      <c r="C7" s="142" t="s">
+        <v>495</v>
+      </c>
+      <c r="D7" s="138" t="s">
+        <v>496</v>
+      </c>
+      <c r="E7" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F7" s="139"/>
+      <c r="G7" s="139"/>
+      <c r="H7" s="139"/>
+      <c r="I7" s="143"/>
+      <c r="J7" s="143"/>
+      <c r="K7" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L7" s="141"/>
+      <c r="M7" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N7" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="O7" s="143"/>
+      <c r="P7" s="139"/>
+      <c r="Q7" s="139"/>
+      <c r="R7" s="139"/>
+      <c r="S7" s="139"/>
+      <c r="T7" s="139"/>
+      <c r="U7" s="139"/>
+      <c r="V7" s="139"/>
+      <c r="W7" s="139"/>
+      <c r="X7" s="139"/>
+      <c r="Y7" s="139"/>
+      <c r="Z7" s="139"/>
+      <c r="AA7" s="139"/>
+      <c r="AB7" s="139"/>
+      <c r="AC7" s="139"/>
+      <c r="AD7" s="139"/>
+      <c r="AE7" s="139"/>
+      <c r="AF7" s="139"/>
     </row>
     <row r="8">
-      <c r="A8" s="62"/>
-      <c r="B8" s="63"/>
-      <c r="C8" s="27"/>
-      <c r="E8" s="27"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="110"/>
-      <c r="J8" s="62"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="99"/>
-      <c r="M8" s="27"/>
-      <c r="N8" s="27"/>
-      <c r="O8" s="107"/>
-      <c r="P8" s="29"/>
-      <c r="Q8" s="29"/>
-      <c r="R8" s="23"/>
-      <c r="S8" s="23"/>
-      <c r="T8" s="23"/>
-      <c r="U8" s="23"/>
-      <c r="V8" s="23"/>
-      <c r="W8" s="23"/>
-      <c r="X8" s="23"/>
-      <c r="Y8" s="23"/>
-      <c r="Z8" s="23"/>
-      <c r="AA8" s="23"/>
-      <c r="AB8" s="23"/>
-      <c r="AC8" s="23"/>
-      <c r="AD8" s="23"/>
-      <c r="AE8" s="23"/>
-      <c r="AF8" s="23"/>
+      <c r="A8" s="142" t="s">
+        <v>498</v>
+      </c>
+      <c r="B8" s="142" t="s">
+        <v>499</v>
+      </c>
+      <c r="C8" s="142" t="s">
+        <v>500</v>
+      </c>
+      <c r="D8" s="138" t="s">
+        <v>501</v>
+      </c>
+      <c r="E8" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F8" s="139"/>
+      <c r="G8" s="139"/>
+      <c r="H8" s="139"/>
+      <c r="I8" s="143"/>
+      <c r="J8" s="143"/>
+      <c r="K8" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L8" s="141"/>
+      <c r="M8" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N8" s="142" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="143"/>
+      <c r="P8" s="139"/>
+      <c r="Q8" s="139"/>
+      <c r="R8" s="139"/>
+      <c r="S8" s="139"/>
+      <c r="T8" s="139"/>
+      <c r="U8" s="139"/>
+      <c r="V8" s="139"/>
+      <c r="W8" s="139"/>
+      <c r="X8" s="139"/>
+      <c r="Y8" s="139"/>
+      <c r="Z8" s="139"/>
+      <c r="AA8" s="139"/>
+      <c r="AB8" s="139"/>
+      <c r="AC8" s="139"/>
+      <c r="AD8" s="139"/>
+      <c r="AE8" s="139"/>
+      <c r="AF8" s="139"/>
     </row>
     <row r="9">
-      <c r="E9" s="27"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="99"/>
-      <c r="M9" s="27"/>
+      <c r="A9" s="138" t="s">
+        <v>502</v>
+      </c>
+      <c r="B9" s="138" t="s">
+        <v>503</v>
+      </c>
+      <c r="C9" s="138" t="s">
+        <v>504</v>
+      </c>
+      <c r="D9" s="138" t="s">
+        <v>505</v>
+      </c>
+      <c r="E9" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F9" s="139"/>
+      <c r="G9" s="139"/>
+      <c r="H9" s="139"/>
+      <c r="I9" s="139"/>
+      <c r="J9" s="138" t="s">
+        <v>506</v>
+      </c>
+      <c r="K9" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L9" s="141"/>
+      <c r="M9" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N9" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O9" s="139"/>
+      <c r="P9" s="139"/>
+      <c r="Q9" s="139"/>
+      <c r="R9" s="139"/>
+      <c r="S9" s="139"/>
+      <c r="T9" s="139"/>
+      <c r="U9" s="139"/>
+      <c r="V9" s="139"/>
+      <c r="W9" s="139"/>
+      <c r="X9" s="139"/>
+      <c r="Y9" s="139"/>
+      <c r="Z9" s="139"/>
+      <c r="AA9" s="139"/>
+      <c r="AB9" s="139"/>
+      <c r="AC9" s="139"/>
+      <c r="AD9" s="139"/>
+      <c r="AE9" s="33"/>
+      <c r="AF9" s="33"/>
     </row>
     <row r="10">
-      <c r="E10" s="27"/>
-      <c r="K10" s="15"/>
-      <c r="L10" s="99"/>
-      <c r="M10" s="27"/>
+      <c r="A10" s="138" t="s">
+        <v>507</v>
+      </c>
+      <c r="B10" s="138" t="s">
+        <v>508</v>
+      </c>
+      <c r="C10" s="138" t="s">
+        <v>509</v>
+      </c>
+      <c r="D10" s="138" t="s">
+        <v>510</v>
+      </c>
+      <c r="E10" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F10" s="139"/>
+      <c r="G10" s="139"/>
+      <c r="H10" s="139"/>
+      <c r="I10" s="139"/>
+      <c r="J10" s="138" t="s">
+        <v>511</v>
+      </c>
+      <c r="K10" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L10" s="141"/>
+      <c r="M10" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O10" s="139"/>
+      <c r="P10" s="139"/>
+      <c r="Q10" s="139"/>
+      <c r="R10" s="139"/>
+      <c r="S10" s="139"/>
+      <c r="T10" s="139"/>
+      <c r="U10" s="139"/>
+      <c r="V10" s="139"/>
+      <c r="W10" s="139"/>
+      <c r="X10" s="139"/>
+      <c r="Y10" s="139"/>
+      <c r="Z10" s="139"/>
+      <c r="AA10" s="139"/>
+      <c r="AB10" s="139"/>
+      <c r="AC10" s="139"/>
+      <c r="AD10" s="139"/>
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
     </row>
     <row r="11">
-      <c r="E11" s="27"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="99"/>
-      <c r="M11" s="27"/>
+      <c r="A11" s="138" t="s">
+        <v>512</v>
+      </c>
+      <c r="B11" s="138" t="s">
+        <v>513</v>
+      </c>
+      <c r="C11" s="138" t="s">
+        <v>514</v>
+      </c>
+      <c r="D11" s="138" t="s">
+        <v>496</v>
+      </c>
+      <c r="E11" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F11" s="139"/>
+      <c r="G11" s="139"/>
+      <c r="H11" s="139"/>
+      <c r="I11" s="139"/>
+      <c r="J11" s="139"/>
+      <c r="K11" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L11" s="141"/>
+      <c r="M11" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N11" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O11" s="139"/>
+      <c r="P11" s="139"/>
+      <c r="Q11" s="139"/>
+      <c r="R11" s="139"/>
+      <c r="S11" s="139"/>
+      <c r="T11" s="139"/>
+      <c r="U11" s="139"/>
+      <c r="V11" s="139"/>
+      <c r="W11" s="139"/>
+      <c r="X11" s="139"/>
+      <c r="Y11" s="139"/>
+      <c r="Z11" s="139"/>
+      <c r="AA11" s="139"/>
+      <c r="AB11" s="139"/>
+      <c r="AC11" s="139"/>
+      <c r="AD11" s="139"/>
+      <c r="AE11" s="139"/>
+      <c r="AF11" s="139"/>
     </row>
     <row r="12">
-      <c r="E12" s="27"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="99"/>
-      <c r="M12" s="27"/>
+      <c r="A12" s="138" t="s">
+        <v>515</v>
+      </c>
+      <c r="B12" s="138" t="s">
+        <v>516</v>
+      </c>
+      <c r="C12" s="138" t="s">
+        <v>517</v>
+      </c>
+      <c r="D12" s="138" t="s">
+        <v>501</v>
+      </c>
+      <c r="E12" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F12" s="139"/>
+      <c r="G12" s="139"/>
+      <c r="H12" s="139"/>
+      <c r="I12" s="139"/>
+      <c r="J12" s="139"/>
+      <c r="K12" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L12" s="141"/>
+      <c r="M12" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O12" s="139"/>
+      <c r="P12" s="139"/>
+      <c r="Q12" s="139"/>
+      <c r="R12" s="139"/>
+      <c r="S12" s="139"/>
+      <c r="T12" s="139"/>
+      <c r="U12" s="139"/>
+      <c r="V12" s="139"/>
+      <c r="W12" s="139"/>
+      <c r="X12" s="139"/>
+      <c r="Y12" s="139"/>
+      <c r="Z12" s="139"/>
+      <c r="AA12" s="139"/>
+      <c r="AB12" s="139"/>
+      <c r="AC12" s="139"/>
+      <c r="AD12" s="139"/>
+      <c r="AE12" s="139"/>
+      <c r="AF12" s="139"/>
     </row>
     <row r="13">
-      <c r="E13" s="27"/>
-      <c r="K13" s="15"/>
-      <c r="L13" s="99"/>
-      <c r="M13" s="27"/>
+      <c r="A13" s="138" t="s">
+        <v>518</v>
+      </c>
+      <c r="B13" s="138" t="s">
+        <v>519</v>
+      </c>
+      <c r="C13" s="138" t="s">
+        <v>520</v>
+      </c>
+      <c r="D13" s="138" t="s">
+        <v>510</v>
+      </c>
+      <c r="E13" s="142" t="s">
+        <v>497</v>
+      </c>
+      <c r="F13" s="139"/>
+      <c r="G13" s="139"/>
+      <c r="H13" s="139"/>
+      <c r="I13" s="139"/>
+      <c r="J13" s="138" t="s">
+        <v>521</v>
+      </c>
+      <c r="K13" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L13" s="141"/>
+      <c r="M13" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O13" s="139"/>
+      <c r="P13" s="139"/>
+      <c r="Q13" s="139"/>
+      <c r="R13" s="139"/>
+      <c r="S13" s="139"/>
+      <c r="T13" s="139"/>
+      <c r="U13" s="139"/>
+      <c r="V13" s="139"/>
+      <c r="W13" s="139"/>
+      <c r="X13" s="139"/>
+      <c r="Y13" s="139"/>
+      <c r="Z13" s="139"/>
+      <c r="AA13" s="139"/>
+      <c r="AB13" s="139"/>
+      <c r="AC13" s="139"/>
+      <c r="AD13" s="139"/>
+      <c r="AE13" s="139"/>
+      <c r="AF13" s="139"/>
     </row>
     <row r="14">
-      <c r="E14" s="27"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="99"/>
-      <c r="M14" s="27"/>
+      <c r="A14" s="138" t="s">
+        <v>522</v>
+      </c>
+      <c r="B14" s="138" t="s">
+        <v>523</v>
+      </c>
+      <c r="C14" s="138" t="s">
+        <v>524</v>
+      </c>
+      <c r="D14" s="138" t="s">
+        <v>116</v>
+      </c>
+      <c r="E14" s="142" t="s">
+        <v>34</v>
+      </c>
+      <c r="F14" s="139"/>
+      <c r="G14" s="139"/>
+      <c r="H14" s="139"/>
+      <c r="I14" s="139"/>
+      <c r="J14" s="138" t="s">
+        <v>525</v>
+      </c>
+      <c r="K14" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L14" s="141"/>
+      <c r="M14" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O14" s="139"/>
+      <c r="P14" s="139"/>
+      <c r="Q14" s="139"/>
+      <c r="R14" s="139"/>
+      <c r="S14" s="139"/>
+      <c r="T14" s="139"/>
+      <c r="U14" s="139"/>
+      <c r="V14" s="139"/>
+      <c r="W14" s="139"/>
+      <c r="X14" s="139"/>
+      <c r="Y14" s="139"/>
+      <c r="Z14" s="139"/>
+      <c r="AA14" s="139"/>
+      <c r="AB14" s="139"/>
+      <c r="AC14" s="139"/>
+      <c r="AD14" s="139"/>
+      <c r="AE14" s="33"/>
+      <c r="AF14" s="33"/>
     </row>
     <row r="15">
-      <c r="E15" s="27"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="99"/>
-      <c r="M15" s="27"/>
+      <c r="A15" s="138" t="s">
+        <v>526</v>
+      </c>
+      <c r="B15" s="138" t="s">
+        <v>527</v>
+      </c>
+      <c r="C15" s="138" t="s">
+        <v>528</v>
+      </c>
+      <c r="D15" s="138" t="s">
+        <v>496</v>
+      </c>
+      <c r="E15" s="142" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="139"/>
+      <c r="G15" s="139"/>
+      <c r="H15" s="139"/>
+      <c r="I15" s="139"/>
+      <c r="J15" s="138" t="s">
+        <v>529</v>
+      </c>
+      <c r="K15" s="140">
+        <v>46057.0</v>
+      </c>
+      <c r="L15" s="141"/>
+      <c r="M15" s="142" t="s">
+        <v>42</v>
+      </c>
+      <c r="N15" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="O15" s="139"/>
+      <c r="P15" s="139"/>
+      <c r="Q15" s="139"/>
+      <c r="R15" s="139"/>
+      <c r="S15" s="139"/>
+      <c r="T15" s="139"/>
+      <c r="U15" s="139"/>
+      <c r="V15" s="139"/>
+      <c r="W15" s="139"/>
+      <c r="X15" s="139"/>
+      <c r="Y15" s="139"/>
+      <c r="Z15" s="139"/>
+      <c r="AA15" s="139"/>
+      <c r="AB15" s="139"/>
+      <c r="AC15" s="139"/>
+      <c r="AD15" s="139"/>
+      <c r="AE15" s="33"/>
+      <c r="AF15" s="33"/>
     </row>
     <row r="16">
+      <c r="A16" s="14"/>
+      <c r="B16" s="14"/>
       <c r="E16" s="27"/>
       <c r="K16" s="15"/>
       <c r="L16" s="99"/>
       <c r="M16" s="27"/>
     </row>
     <row r="17">
+      <c r="A17" s="14"/>
+      <c r="B17" s="14"/>
       <c r="E17" s="27"/>
       <c r="K17" s="15"/>
       <c r="L17" s="99"/>
@@ -6493,6 +7116,8 @@
       <c r="M23" s="27"/>
     </row>
     <row r="24">
+      <c r="A24" s="14"/>
+      <c r="B24" s="14"/>
       <c r="E24" s="27"/>
       <c r="K24" s="15"/>
       <c r="L24" s="99"/>

</xml_diff>

<commit_message>
Add to PR #239 SECTOR-HEALTH
- fix issues in template for sector by adding conditional modules for
  health which are not present in other sectors
- add additional concepts for data, purpose, tech, entities
- generate RDF and HTML outputs

Co-authored-by: Beatriz Esteves <beatriz.gc.esteves@gmail.com>
</commit_message>
<xml_diff>
--- a/code/vocab_csv/entities.xlsx
+++ b/code/vocab_csv/entities.xlsx
@@ -6482,8 +6482,8 @@
         <v>46057.0</v>
       </c>
       <c r="L4" s="141"/>
-      <c r="M4" s="138" t="s">
-        <v>42</v>
+      <c r="M4" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N4" s="138" t="s">
         <v>46</v>
@@ -6530,8 +6530,8 @@
         <v>46057.0</v>
       </c>
       <c r="L5" s="141"/>
-      <c r="M5" s="142" t="s">
-        <v>42</v>
+      <c r="M5" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N5" s="142" t="s">
         <v>46</v>
@@ -6578,8 +6578,8 @@
         <v>46057.0</v>
       </c>
       <c r="L6" s="141"/>
-      <c r="M6" s="142" t="s">
-        <v>42</v>
+      <c r="M6" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N6" s="142" t="s">
         <v>46</v>
@@ -6628,8 +6628,8 @@
         <v>46057.0</v>
       </c>
       <c r="L7" s="141"/>
-      <c r="M7" s="142" t="s">
-        <v>42</v>
+      <c r="M7" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N7" s="142" t="s">
         <v>46</v>
@@ -6678,8 +6678,8 @@
         <v>46057.0</v>
       </c>
       <c r="L8" s="141"/>
-      <c r="M8" s="142" t="s">
-        <v>42</v>
+      <c r="M8" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N8" s="142" t="s">
         <v>46</v>
@@ -6730,8 +6730,8 @@
         <v>46057.0</v>
       </c>
       <c r="L9" s="141"/>
-      <c r="M9" s="142" t="s">
-        <v>42</v>
+      <c r="M9" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N9" s="138" t="s">
         <v>46</v>
@@ -6782,8 +6782,8 @@
         <v>46057.0</v>
       </c>
       <c r="L10" s="141"/>
-      <c r="M10" s="142" t="s">
-        <v>42</v>
+      <c r="M10" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N10" s="138" t="s">
         <v>46</v>
@@ -6832,8 +6832,8 @@
         <v>46057.0</v>
       </c>
       <c r="L11" s="141"/>
-      <c r="M11" s="142" t="s">
-        <v>42</v>
+      <c r="M11" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N11" s="138" t="s">
         <v>46</v>
@@ -6882,8 +6882,8 @@
         <v>46057.0</v>
       </c>
       <c r="L12" s="141"/>
-      <c r="M12" s="142" t="s">
-        <v>42</v>
+      <c r="M12" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N12" s="138" t="s">
         <v>46</v>
@@ -6934,8 +6934,8 @@
         <v>46057.0</v>
       </c>
       <c r="L13" s="141"/>
-      <c r="M13" s="142" t="s">
-        <v>42</v>
+      <c r="M13" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N13" s="138" t="s">
         <v>46</v>
@@ -6986,8 +6986,8 @@
         <v>46057.0</v>
       </c>
       <c r="L14" s="141"/>
-      <c r="M14" s="142" t="s">
-        <v>42</v>
+      <c r="M14" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N14" s="138" t="s">
         <v>46</v>
@@ -7038,8 +7038,8 @@
         <v>46057.0</v>
       </c>
       <c r="L15" s="141"/>
-      <c r="M15" s="142" t="s">
-        <v>42</v>
+      <c r="M15" s="100" t="s">
+        <v>19</v>
       </c>
       <c r="N15" s="138" t="s">
         <v>46</v>
@@ -7064,16 +7064,12 @@
       <c r="AF15" s="33"/>
     </row>
     <row r="16">
-      <c r="A16" s="14"/>
-      <c r="B16" s="14"/>
       <c r="E16" s="27"/>
       <c r="K16" s="15"/>
       <c r="L16" s="99"/>
       <c r="M16" s="27"/>
     </row>
     <row r="17">
-      <c r="A17" s="14"/>
-      <c r="B17" s="14"/>
       <c r="E17" s="27"/>
       <c r="K17" s="15"/>
       <c r="L17" s="99"/>
@@ -7116,8 +7112,6 @@
       <c r="M23" s="27"/>
     </row>
     <row r="24">
-      <c r="A24" s="14"/>
-      <c r="B24" s="14"/>
       <c r="E24" s="27"/>
       <c r="K24" s="15"/>
       <c r="L24" s="99"/>

</xml_diff>